<commit_message>
Updated for week 6.
</commit_message>
<xml_diff>
--- a/NFL Wins.xlsx
+++ b/NFL Wins.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27430"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9660" windowHeight="16100" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12180" windowHeight="16100" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="93">
   <si>
     <t>Arizona Cardinals</t>
   </si>
@@ -269,6 +269,54 @@
   </si>
   <si>
     <t>Output</t>
+  </si>
+  <si>
+    <t>Week 6</t>
+  </si>
+  <si>
+    <t>Week 7</t>
+  </si>
+  <si>
+    <t>Week 8</t>
+  </si>
+  <si>
+    <t>Week 9</t>
+  </si>
+  <si>
+    <t>Week 10</t>
+  </si>
+  <si>
+    <t>Week 11</t>
+  </si>
+  <si>
+    <t>Week 12</t>
+  </si>
+  <si>
+    <t>Week 13</t>
+  </si>
+  <si>
+    <t>Week 14</t>
+  </si>
+  <si>
+    <t>Week 15</t>
+  </si>
+  <si>
+    <t>Week 16</t>
+  </si>
+  <si>
+    <t>Week 17</t>
+  </si>
+  <si>
+    <t>Wildcard</t>
+  </si>
+  <si>
+    <t>Divisonal</t>
+  </si>
+  <si>
+    <t>Conference</t>
+  </si>
+  <si>
+    <t>SuperBowl</t>
   </si>
 </sst>
 </file>
@@ -308,15 +356,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -324,8 +378,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="59">
+  <cellStyleXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -385,15 +448,47 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="59">
+  <cellStyles count="85">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -423,6 +518,19 @@
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -452,6 +560,19 @@
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -787,7 +908,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -1068,62 +1189,116 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H37"/>
+  <dimension ref="A1:Y38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A33"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="A33" sqref="A2:A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="4" max="5" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.33203125" customWidth="1"/>
+    <col min="2" max="2" width="0.6640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="13" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="21" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1">
+    <row r="1" spans="1:25" s="1" customFormat="1" ht="16" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="6" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" t="str">
-        <f>CONCATENATE("['",$B2,"', ","'",$C2,"' ,",$D2,",",$E2,",",$F2,",",$G2,",",$H2,"],")</f>
-        <v>['49ers', 'Greg' ,1,1,1,1,1],</v>
-      </c>
-      <c r="B2" t="s">
-        <v>69</v>
-      </c>
+      <c r="J1" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="R1" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="S1" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="T1" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="U1" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="V1" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="W1" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="X1" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="Y1" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25">
+      <c r="A2" s="2" t="str">
+        <f>CONCATENATE("['",$C2,"', ","'",$D2,"' ,",$E2,",",$F2,",",$G2,",",$H2,",",$I2,",",$J2,"],")</f>
+        <v>['Greg', '49ers' ,1,1,1,1,1,1],</v>
+      </c>
+      <c r="B2" s="3"/>
       <c r="C2" t="s">
         <v>33</v>
       </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2" s="2">
-        <v>1</v>
-      </c>
-      <c r="F2">
+      <c r="D2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="2">
         <v>1</v>
       </c>
       <c r="G2">
@@ -1132,133 +1307,153 @@
       <c r="H2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" t="str">
-        <f t="shared" ref="A3:A33" si="0">CONCATENATE("['",$B3,"', ","'",$C3,"' ,",$D3,",",$E3,",",$F3,",",$G3,",",$H3,"],")</f>
-        <v>['Bears', 'Jeff' ,0,0,0,1,0],</v>
-      </c>
-      <c r="B3" t="s">
-        <v>52</v>
-      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25">
+      <c r="A3" s="2" t="str">
+        <f t="shared" ref="A3:A33" si="0">CONCATENATE("['",$C3,"', ","'",$D3,"' ,",$E3,",",$F3,",",$G3,",",$H3,",",$I3,",",$J3,"],")</f>
+        <v>['Jeff', 'Bears' ,0,0,0,1,1,1],</v>
+      </c>
+      <c r="B3" s="3"/>
       <c r="C3" t="s">
         <v>32</v>
       </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3" s="2">
-        <v>0</v>
-      </c>
-      <c r="F3">
+      <c r="D3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" t="str">
-        <f t="shared" si="0"/>
-        <v>['Bengals', 'Tim' ,1,1,1,2,0],</v>
-      </c>
-      <c r="B4" t="s">
-        <v>47</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25">
+      <c r="A4" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>['Tim', 'Bengals' ,1,1,1,2,2,2],</v>
+      </c>
+      <c r="B4" s="3"/>
       <c r="C4" t="s">
         <v>34</v>
       </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4" s="2">
-        <v>1</v>
-      </c>
-      <c r="F4">
+      <c r="D4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="2">
         <v>1</v>
       </c>
       <c r="G4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" t="str">
-        <f t="shared" si="0"/>
-        <v>['Bills', 'Greg' ,0,0,1,2,0],</v>
-      </c>
-      <c r="B5" t="s">
-        <v>54</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="I4">
+        <v>2</v>
+      </c>
+      <c r="J4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25">
+      <c r="A5" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>['Greg', 'Bills' ,0,0,1,2,3,4],</v>
+      </c>
+      <c r="B5" s="3"/>
       <c r="C5" t="s">
         <v>33</v>
       </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5" s="2">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
+      <c r="D5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" t="str">
-        <f t="shared" si="0"/>
-        <v>['Broncos', 'Zach' ,1,2,3,4,0],</v>
-      </c>
-      <c r="B6" t="s">
-        <v>40</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="I5">
+        <v>3</v>
+      </c>
+      <c r="J5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25">
+      <c r="A6" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>['Zach', 'Broncos' ,1,2,3,4,4,4],</v>
+      </c>
+      <c r="B6" s="3"/>
       <c r="C6" t="s">
         <v>35</v>
       </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6" s="2">
-        <v>2</v>
-      </c>
-      <c r="F6">
-        <v>3</v>
+      <c r="D6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" s="2">
+        <v>2</v>
       </c>
       <c r="G6">
+        <v>3</v>
+      </c>
+      <c r="H6">
         <v>4</v>
       </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" t="str">
-        <f t="shared" si="0"/>
-        <v>['Browns', 'Jeff' ,0,0,0,0,0],</v>
-      </c>
-      <c r="B7" t="s">
-        <v>49</v>
-      </c>
+      <c r="I6">
+        <v>4</v>
+      </c>
+      <c r="J6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25">
+      <c r="A7" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>['Jeff', 'Browns' ,0,0,0,0,0,0],</v>
+      </c>
+      <c r="B7" s="3"/>
       <c r="C7" t="s">
         <v>32</v>
       </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7" s="2">
-        <v>0</v>
-      </c>
-      <c r="F7">
+      <c r="D7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7" s="2">
         <v>0</v>
       </c>
       <c r="G7">
@@ -1267,812 +1462,943 @@
       <c r="H7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" t="str">
-        <f t="shared" si="0"/>
-        <v>['Buccaneers', 'Zach' ,1,1,1,1,0],</v>
-      </c>
-      <c r="B8" t="s">
-        <v>56</v>
-      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25">
+      <c r="A8" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>['Zach', 'Buccaneers' ,1,1,1,1,2,2],</v>
+      </c>
+      <c r="B8" s="3"/>
       <c r="C8" t="s">
         <v>35</v>
       </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8" s="2">
-        <v>1</v>
-      </c>
-      <c r="F8">
+      <c r="D8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8" s="2">
         <v>1</v>
       </c>
       <c r="G8">
         <v>1</v>
       </c>
       <c r="H8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" t="str">
-        <f t="shared" si="0"/>
-        <v>['Cardinals', 'Jeff' ,0,1,1,1,2],</v>
-      </c>
-      <c r="B9" t="s">
-        <v>65</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>2</v>
+      </c>
+      <c r="J8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25">
+      <c r="A9" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>['Jeff', 'Cardinals' ,0,1,1,1,2,3],</v>
+      </c>
+      <c r="B9" s="3"/>
       <c r="C9" t="s">
         <v>32</v>
       </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9" s="2">
-        <v>1</v>
-      </c>
-      <c r="F9">
+      <c r="D9" t="s">
+        <v>65</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9" s="2">
         <v>1</v>
       </c>
       <c r="G9">
         <v>1</v>
       </c>
       <c r="H9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" t="str">
-        <f t="shared" si="0"/>
-        <v>['Chargers', 'Jeff' ,0,1,1,1,0],</v>
-      </c>
-      <c r="B10" t="s">
-        <v>43</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>2</v>
+      </c>
+      <c r="J9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25">
+      <c r="A10" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>['Jeff', 'Chargers' ,0,1,1,1,1,2],</v>
+      </c>
+      <c r="B10" s="3"/>
       <c r="C10" t="s">
         <v>32</v>
       </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10" s="2">
-        <v>1</v>
-      </c>
-      <c r="F10">
+      <c r="D10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10" s="2">
         <v>1</v>
       </c>
       <c r="G10">
         <v>1</v>
       </c>
       <c r="H10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" t="str">
-        <f t="shared" si="0"/>
-        <v>['Chiefs', 'Zach' ,1,1,2,2,0],</v>
-      </c>
-      <c r="B11" t="s">
-        <v>44</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25">
+      <c r="A11" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>['Zach', 'Chiefs' ,1,1,2,2,2,3],</v>
+      </c>
+      <c r="B11" s="3"/>
       <c r="C11" t="s">
         <v>35</v>
       </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11" s="2">
-        <v>1</v>
-      </c>
-      <c r="F11">
-        <v>2</v>
+      <c r="D11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11" s="2">
+        <v>1</v>
       </c>
       <c r="G11">
         <v>2</v>
       </c>
       <c r="H11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" t="str">
-        <f t="shared" si="0"/>
-        <v>['Colts', 'Greg' ,0,0,1,1,0],</v>
-      </c>
-      <c r="B12" t="s">
-        <v>63</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="I11">
+        <v>2</v>
+      </c>
+      <c r="J11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25">
+      <c r="A12" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>['Greg', 'Colts' ,0,0,1,1,2,2],</v>
+      </c>
+      <c r="B12" s="3"/>
       <c r="C12" t="s">
         <v>33</v>
       </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12" s="2">
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <v>1</v>
+      <c r="D12" t="s">
+        <v>63</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12" s="2">
+        <v>0</v>
       </c>
       <c r="G12">
         <v>1</v>
       </c>
       <c r="H12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" t="str">
-        <f t="shared" si="0"/>
-        <v>['Cowboys', 'Greg' ,0,1,2,3,0],</v>
-      </c>
-      <c r="B13" t="s">
-        <v>61</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>2</v>
+      </c>
+      <c r="J12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25">
+      <c r="A13" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>['Greg', 'Cowboys' ,0,1,2,3,4,5],</v>
+      </c>
+      <c r="B13" s="3"/>
       <c r="C13" t="s">
         <v>33</v>
       </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13" s="2">
-        <v>1</v>
-      </c>
-      <c r="F13">
-        <v>2</v>
+      <c r="D13" t="s">
+        <v>61</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13" s="2">
+        <v>1</v>
       </c>
       <c r="G13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" t="str">
-        <f t="shared" si="0"/>
-        <v>['Dolphins', 'Tim' ,0,0,1,1,0],</v>
-      </c>
-      <c r="B14" t="s">
-        <v>58</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="I13">
+        <v>4</v>
+      </c>
+      <c r="J13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25">
+      <c r="A14" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>['Tim', 'Dolphins' ,0,0,1,1,1,2],</v>
+      </c>
+      <c r="B14" s="3"/>
       <c r="C14" t="s">
         <v>34</v>
       </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14" s="2">
-        <v>0</v>
-      </c>
-      <c r="F14">
-        <v>1</v>
+      <c r="D14" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14" s="2">
+        <v>0</v>
       </c>
       <c r="G14">
         <v>1</v>
       </c>
       <c r="H14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" t="str">
-        <f t="shared" si="0"/>
-        <v>['Eagles', 'Zach' ,1,2,3,3,0],</v>
-      </c>
-      <c r="B15" t="s">
-        <v>50</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25">
+      <c r="A15" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>['Zach', 'Eagles' ,1,2,3,3,3,3],</v>
+      </c>
+      <c r="B15" s="3"/>
       <c r="C15" t="s">
         <v>35</v>
       </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15" s="2">
-        <v>2</v>
-      </c>
-      <c r="F15">
-        <v>3</v>
+      <c r="D15" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15" s="2">
+        <v>2</v>
       </c>
       <c r="G15">
         <v>3</v>
       </c>
       <c r="H15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" t="str">
-        <f t="shared" si="0"/>
-        <v>['Falcons', 'Greg' ,0,1,2,3,0],</v>
-      </c>
-      <c r="B16" t="s">
-        <v>57</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="I15">
+        <v>3</v>
+      </c>
+      <c r="J15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25">
+      <c r="A16" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>['Greg', 'Falcons' ,0,1,2,3,4,4],</v>
+      </c>
+      <c r="B16" s="3"/>
       <c r="C16" t="s">
         <v>33</v>
       </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16" s="2">
-        <v>1</v>
-      </c>
-      <c r="F16">
-        <v>2</v>
+      <c r="D16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16" s="2">
+        <v>1</v>
       </c>
       <c r="G16">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
-      <c r="A17" t="str">
-        <f t="shared" si="0"/>
-        <v>['Giants', 'Jeff' ,1,2,2,2,0],</v>
-      </c>
-      <c r="B17" t="s">
-        <v>60</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="I16">
+        <v>4</v>
+      </c>
+      <c r="J16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>['Jeff', 'Giants' ,1,2,2,2,2,3],</v>
+      </c>
+      <c r="B17" s="3"/>
       <c r="C17" t="s">
         <v>32</v>
       </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-      <c r="E17" s="2">
-        <v>2</v>
-      </c>
-      <c r="F17">
+      <c r="D17" t="s">
+        <v>60</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17" s="2">
         <v>2</v>
       </c>
       <c r="G17">
         <v>2</v>
       </c>
       <c r="H17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
-      <c r="A18" t="str">
-        <f t="shared" si="0"/>
-        <v>['Jaguars', 'Tim' ,0,0,0,1,0],</v>
-      </c>
-      <c r="B18" t="s">
-        <v>42</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="I17">
+        <v>2</v>
+      </c>
+      <c r="J17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>['Tim', 'Jaguars' ,0,0,0,1,1,2],</v>
+      </c>
+      <c r="B18" s="3"/>
       <c r="C18" t="s">
         <v>34</v>
       </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18" s="2">
-        <v>0</v>
-      </c>
-      <c r="F18">
+      <c r="D18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18" s="2">
         <v>0</v>
       </c>
       <c r="G18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19" t="str">
-        <f t="shared" si="0"/>
-        <v>['Jets', 'Tim' ,0,1,1,1,0],</v>
-      </c>
-      <c r="B19" t="s">
-        <v>48</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
+      </c>
+      <c r="J18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>['Tim', 'Jets' ,0,1,1,1,1,1],</v>
+      </c>
+      <c r="B19" s="3"/>
       <c r="C19" t="s">
         <v>34</v>
       </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19" s="2">
-        <v>1</v>
-      </c>
-      <c r="F19">
+      <c r="D19" t="s">
+        <v>48</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19" s="2">
         <v>1</v>
       </c>
       <c r="G19">
         <v>1</v>
       </c>
       <c r="H19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="A20" t="str">
-        <f t="shared" si="0"/>
-        <v>['Lions', 'Jeff' ,1,1,1,1,0],</v>
-      </c>
-      <c r="B20" t="s">
-        <v>62</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="I19">
+        <v>1</v>
+      </c>
+      <c r="J19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>['Jeff', 'Lions' ,1,1,1,1,2,3],</v>
+      </c>
+      <c r="B20" s="3"/>
       <c r="C20" t="s">
         <v>32</v>
       </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-      <c r="E20" s="2">
-        <v>1</v>
-      </c>
-      <c r="F20">
+      <c r="D20" t="s">
+        <v>62</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20" s="2">
         <v>1</v>
       </c>
       <c r="G20">
         <v>1</v>
       </c>
       <c r="H20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="A21" t="str">
-        <f t="shared" si="0"/>
-        <v>['Packers', 'Tim' ,1,1,2,2,0],</v>
-      </c>
-      <c r="B21" t="s">
-        <v>41</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <v>2</v>
+      </c>
+      <c r="J20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>['Tim', 'Packers' ,1,1,2,2,3,3],</v>
+      </c>
+      <c r="B21" s="3"/>
       <c r="C21" t="s">
         <v>34</v>
       </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-      <c r="E21" s="2">
-        <v>1</v>
-      </c>
-      <c r="F21">
-        <v>2</v>
+      <c r="D21" t="s">
+        <v>41</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21" s="2">
+        <v>1</v>
       </c>
       <c r="G21">
         <v>2</v>
       </c>
       <c r="H21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
-      <c r="A22" t="str">
-        <f t="shared" si="0"/>
-        <v>['Panthers', 'Greg' ,0,1,1,1,0],</v>
-      </c>
-      <c r="B22" t="s">
-        <v>39</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="I21">
+        <v>3</v>
+      </c>
+      <c r="J21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>['Greg', 'Panthers' ,0,1,1,1,1,1],</v>
+      </c>
+      <c r="B22" s="3"/>
       <c r="C22" t="s">
         <v>33</v>
       </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="E22" s="2">
-        <v>1</v>
-      </c>
-      <c r="F22">
+      <c r="D22" t="s">
+        <v>39</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22" s="2">
         <v>1</v>
       </c>
       <c r="G22">
         <v>1</v>
       </c>
       <c r="H22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
-      <c r="A23" t="str">
-        <f t="shared" si="0"/>
-        <v>['Patriots', 'Greg' ,1,2,3,3,0],</v>
-      </c>
-      <c r="B23" t="s">
-        <v>64</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <v>1</v>
+      </c>
+      <c r="J22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>['Greg', 'Patriots' ,1,2,3,3,4,5],</v>
+      </c>
+      <c r="B23" s="3"/>
       <c r="C23" t="s">
         <v>33</v>
       </c>
-      <c r="D23">
-        <v>1</v>
-      </c>
-      <c r="E23" s="2">
-        <v>2</v>
-      </c>
-      <c r="F23">
-        <v>3</v>
+      <c r="D23" t="s">
+        <v>64</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23" s="2">
+        <v>2</v>
       </c>
       <c r="G23">
         <v>3</v>
       </c>
       <c r="H23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
-      <c r="A24" t="str">
-        <f t="shared" si="0"/>
-        <v>['Raiders', 'Tim' ,1,1,2,3,0],</v>
-      </c>
-      <c r="B24" t="s">
-        <v>45</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="I23">
+        <v>4</v>
+      </c>
+      <c r="J23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>['Tim', 'Raiders' ,1,1,2,3,4,4],</v>
+      </c>
+      <c r="B24" s="3"/>
       <c r="C24" t="s">
         <v>34</v>
       </c>
-      <c r="D24">
-        <v>1</v>
-      </c>
-      <c r="E24" s="2">
-        <v>1</v>
-      </c>
-      <c r="F24">
-        <v>2</v>
+      <c r="D24" t="s">
+        <v>45</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24" s="2">
+        <v>1</v>
       </c>
       <c r="G24">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8">
-      <c r="A25" t="str">
-        <f t="shared" si="0"/>
-        <v>['Rams', 'Zach' ,0,1,2,3,0],</v>
-      </c>
-      <c r="B25" t="s">
-        <v>68</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="I24">
+        <v>4</v>
+      </c>
+      <c r="J24">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>['Zach', 'Rams' ,0,1,2,3,3,3],</v>
+      </c>
+      <c r="B25" s="3"/>
       <c r="C25" t="s">
         <v>35</v>
       </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-      <c r="E25" s="2">
-        <v>1</v>
-      </c>
-      <c r="F25">
-        <v>2</v>
+      <c r="D25" t="s">
+        <v>68</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25" s="2">
+        <v>1</v>
       </c>
       <c r="G25">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
-      <c r="A26" t="str">
-        <f t="shared" si="0"/>
-        <v>['Ravens', 'Jeff' ,1,2,3,3,0],</v>
-      </c>
-      <c r="B26" t="s">
-        <v>55</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="I25">
+        <v>3</v>
+      </c>
+      <c r="J25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>['Jeff', 'Ravens' ,1,2,3,3,3,3],</v>
+      </c>
+      <c r="B26" s="3"/>
       <c r="C26" t="s">
         <v>32</v>
       </c>
-      <c r="D26">
-        <v>1</v>
-      </c>
-      <c r="E26" s="2">
-        <v>2</v>
-      </c>
-      <c r="F26">
-        <v>3</v>
+      <c r="D26" t="s">
+        <v>55</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26" s="2">
+        <v>2</v>
       </c>
       <c r="G26">
         <v>3</v>
       </c>
       <c r="H26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8">
-      <c r="A27" t="str">
-        <f t="shared" si="0"/>
-        <v>['Redskins', 'Greg' ,0,0,1,2,0],</v>
-      </c>
-      <c r="B27" t="s">
-        <v>67</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="I26">
+        <v>3</v>
+      </c>
+      <c r="J26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>['Greg', 'Redskins' ,0,0,1,2,3,4],</v>
+      </c>
+      <c r="B27" s="3"/>
       <c r="C27" t="s">
         <v>33</v>
       </c>
-      <c r="D27">
-        <v>0</v>
-      </c>
-      <c r="E27" s="2">
-        <v>0</v>
-      </c>
-      <c r="F27">
-        <v>1</v>
+      <c r="D27" t="s">
+        <v>67</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27" s="2">
+        <v>0</v>
       </c>
       <c r="G27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8">
-      <c r="A28" t="str">
-        <f t="shared" si="0"/>
-        <v>['Saints', 'Zach' ,0,0,0,1,0],</v>
-      </c>
-      <c r="B28" t="s">
-        <v>46</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="I27">
+        <v>3</v>
+      </c>
+      <c r="J27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>['Zach', 'Saints' ,0,0,0,1,1,2],</v>
+      </c>
+      <c r="B28" s="3"/>
       <c r="C28" t="s">
         <v>35</v>
       </c>
-      <c r="D28">
-        <v>0</v>
-      </c>
-      <c r="E28" s="2">
-        <v>0</v>
-      </c>
-      <c r="F28">
+      <c r="D28" t="s">
+        <v>46</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28" s="2">
         <v>0</v>
       </c>
       <c r="G28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8">
-      <c r="A29" t="str">
-        <f t="shared" si="0"/>
-        <v>['Seahawks', 'Zach' ,1,1,2,3,0],</v>
-      </c>
-      <c r="B29" t="s">
-        <v>59</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="I28">
+        <v>1</v>
+      </c>
+      <c r="J28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>['Zach', 'Seahawks' ,1,1,2,3,3,4],</v>
+      </c>
+      <c r="B29" s="3"/>
       <c r="C29" t="s">
         <v>35</v>
       </c>
-      <c r="D29">
-        <v>1</v>
-      </c>
-      <c r="E29" s="2">
-        <v>1</v>
-      </c>
-      <c r="F29">
-        <v>2</v>
+      <c r="D29" t="s">
+        <v>59</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29" s="2">
+        <v>1</v>
       </c>
       <c r="G29">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8">
-      <c r="A30" t="str">
-        <f t="shared" si="0"/>
-        <v>['Steelers', 'Tim' ,1,2,2,3,0],</v>
-      </c>
-      <c r="B30" t="s">
-        <v>66</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="I29">
+        <v>3</v>
+      </c>
+      <c r="J29">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>['Tim', 'Steelers' ,1,2,2,3,4,4],</v>
+      </c>
+      <c r="B30" s="3"/>
       <c r="C30" t="s">
         <v>34</v>
       </c>
-      <c r="D30">
-        <v>1</v>
-      </c>
-      <c r="E30" s="2">
-        <v>2</v>
-      </c>
-      <c r="F30">
+      <c r="D30" t="s">
+        <v>66</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30" s="2">
         <v>2</v>
       </c>
       <c r="G30">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8">
-      <c r="A31" t="str">
-        <f t="shared" si="0"/>
-        <v>['Texans', 'Jeff' ,1,2,2,3,0],</v>
-      </c>
-      <c r="B31" t="s">
-        <v>53</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="I30">
+        <v>4</v>
+      </c>
+      <c r="J30">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>['Jeff', 'Texans' ,1,2,2,3,3,4],</v>
+      </c>
+      <c r="B31" s="3"/>
       <c r="C31" t="s">
         <v>32</v>
       </c>
-      <c r="D31">
-        <v>1</v>
-      </c>
-      <c r="E31" s="2">
-        <v>2</v>
-      </c>
-      <c r="F31">
+      <c r="D31" t="s">
+        <v>53</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31" s="2">
         <v>2</v>
       </c>
       <c r="G31">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8">
-      <c r="A32" t="str">
-        <f t="shared" si="0"/>
-        <v>['Titans', 'Zach' ,0,1,1,1,0],</v>
-      </c>
-      <c r="B32" t="s">
-        <v>51</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="I31">
+        <v>3</v>
+      </c>
+      <c r="J31">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>['Zach', 'Titans' ,0,1,1,1,2,3],</v>
+      </c>
+      <c r="B32" s="3"/>
       <c r="C32" t="s">
         <v>35</v>
       </c>
-      <c r="D32">
-        <v>0</v>
-      </c>
-      <c r="E32" s="2">
-        <v>1</v>
-      </c>
-      <c r="F32">
+      <c r="D32" t="s">
+        <v>51</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32" s="2">
         <v>1</v>
       </c>
       <c r="G32">
         <v>1</v>
       </c>
       <c r="H32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8">
-      <c r="A33" t="str">
-        <f t="shared" si="0"/>
-        <v>['Vikings', 'Tim' ,1,2,3,4,0],</v>
-      </c>
-      <c r="B33" t="s">
-        <v>74</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="I32">
+        <v>2</v>
+      </c>
+      <c r="J32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>['Tim', 'Vikings' ,1,2,3,4,5,5],</v>
+      </c>
+      <c r="B33" s="3"/>
       <c r="C33" t="s">
         <v>34</v>
       </c>
-      <c r="D33">
-        <v>1</v>
-      </c>
-      <c r="E33" s="2">
-        <v>2</v>
-      </c>
-      <c r="F33">
-        <v>3</v>
+      <c r="D33" t="s">
+        <v>74</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33" s="2">
+        <v>2</v>
       </c>
       <c r="G33">
+        <v>3</v>
+      </c>
+      <c r="H33">
         <v>4</v>
       </c>
-      <c r="H33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8">
-      <c r="B34" t="s">
+      <c r="I33">
+        <v>5</v>
+      </c>
+      <c r="J33">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" s="4" customFormat="1" ht="4" customHeight="1">
+      <c r="A34" s="3"/>
+      <c r="B34" s="3"/>
+      <c r="F34" s="3"/>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="D35" t="s">
         <v>32</v>
       </c>
-      <c r="D34">
-        <f>SUMIF($C$2:$C$33,$B34,D$2:D$33)</f>
+      <c r="E35">
+        <f t="shared" ref="E35:J37" si="1">SUMIF($C$2:$C$33,$D35,E$2:E$33)</f>
         <v>4</v>
       </c>
-      <c r="E34" s="2">
-        <f>SUMIF($C$2:$C$33,$B34,E$2:E$33)</f>
+      <c r="F35" s="2">
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="F34" s="2">
-        <f>SUMIF($C$2:$C$33,$B34,F$2:F$33)</f>
+      <c r="G35" s="2">
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="G34" s="2">
-        <f>SUMIF($C$2:$C$33,$B34,G$2:G$33)</f>
+      <c r="H35" s="2">
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="H34" s="2">
-        <f>SUMIF($C$2:$C$33,$B34,H$2:H$33)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8">
-      <c r="B35" t="s">
+      <c r="I35" s="2">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="J35" s="2">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
+      <c r="D36" t="s">
         <v>33</v>
       </c>
-      <c r="D35">
-        <f>SUMIF($C$2:$C$33,$B35,D$2:D$33)</f>
-        <v>2</v>
-      </c>
-      <c r="E35" s="2">
-        <f>SUMIF($C$2:$C$33,$B35,E$2:E$33)</f>
+      <c r="E36">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="F36" s="2">
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="F35" s="2">
-        <f>SUMIF($C$2:$C$33,$B35,F$2:F$33)</f>
+      <c r="G36" s="2">
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="G35" s="2">
-        <f>SUMIF($C$2:$C$33,$B35,G$2:G$33)</f>
+      <c r="H36" s="2">
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="H35" s="2">
-        <f>SUMIF($C$2:$C$33,$B35,H$2:H$33)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8">
-      <c r="B36" t="s">
+      <c r="I36" s="2">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="J36" s="2">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="D37" t="s">
         <v>34</v>
       </c>
-      <c r="D36">
-        <f>SUMIF($C$2:$C$33,$B36,D$2:D$33)</f>
+      <c r="E37">
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="E36" s="2">
-        <f>SUMIF($C$2:$C$33,$B36,E$2:E$33)</f>
+      <c r="F37" s="2">
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="F36" s="2">
-        <f>SUMIF($C$2:$C$33,$B36,F$2:F$33)</f>
+      <c r="G37" s="2">
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="G36" s="2">
-        <f>SUMIF($C$2:$C$33,$B36,G$2:G$33)</f>
+      <c r="H37" s="2">
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="H36" s="2">
-        <f>SUMIF($C$2:$C$33,$B36,H$2:H$33)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8">
-      <c r="B37" t="s">
+      <c r="I37" s="2">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="J37" s="2">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="D38" t="s">
         <v>35</v>
       </c>
-      <c r="D37">
-        <f>SUMIF($C$2:$C$33,$B$37,D$2:D$33)</f>
+      <c r="E38">
+        <f t="shared" ref="E38:J38" si="2">SUMIF($C$2:$C$33,$D$38,E$2:E$33)</f>
         <v>5</v>
       </c>
-      <c r="E37" s="2">
-        <f>SUMIF($C$2:$C$33,$B$37,E$2:E$33)</f>
+      <c r="F38" s="2">
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="F37" s="2">
-        <f>SUMIF($C$2:$C$33,$B$37,F$2:F$33)</f>
+      <c r="G38" s="2">
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
-      <c r="G37" s="2">
-        <f>SUMIF($C$2:$C$33,$B$37,G$2:G$33)</f>
+      <c r="H38" s="2">
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
-      <c r="H37" s="2">
-        <f>SUMIF($C$2:$C$33,$B$37,H$2:H$33)</f>
-        <v>0</v>
+      <c r="I38" s="2">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="J38" s="2">
+        <f t="shared" si="2"/>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="B2:C34">
-    <sortCondition ref="B34"/>
+  <sortState ref="D2:E34">
+    <sortCondition ref="D34"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Update to week 8 and add the mechanics to do so.
</commit_message>
<xml_diff>
--- a/NFL Wins.xlsx
+++ b/NFL Wins.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12180" windowHeight="16100" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9780" windowHeight="16100" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
@@ -388,7 +388,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="85">
+  <cellStyleXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -474,8 +474,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -487,8 +495,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="85">
+  <cellStyles count="93">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -531,6 +540,10 @@
     <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -573,6 +586,10 @@
     <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1189,10 +1206,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y38"/>
+  <dimension ref="A1:Y39"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="A33" sqref="A2:A33"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A2" workbookViewId="0">
+      <pane xSplit="4" topLeftCell="K1" activePane="topRight" state="frozenSplit"/>
+      <selection pane="topRight" activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1201,139 +1219,139 @@
     <col min="2" max="2" width="0.6640625" style="4" customWidth="1"/>
     <col min="3" max="3" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="13" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="7.5" bestFit="1" customWidth="1"/>
     <col min="14" max="21" width="8.5" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="10.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="1" customFormat="1" ht="16" thickBot="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:25">
+      <c r="E1" s="7">
+        <f t="shared" ref="E1:I1" si="0">F1-7</f>
+        <v>42626</v>
+      </c>
+      <c r="F1" s="7">
+        <f t="shared" si="0"/>
+        <v>42633</v>
+      </c>
+      <c r="G1" s="7">
+        <f t="shared" si="0"/>
+        <v>42640</v>
+      </c>
+      <c r="H1" s="7">
+        <f t="shared" si="0"/>
+        <v>42647</v>
+      </c>
+      <c r="I1" s="7">
+        <f t="shared" si="0"/>
+        <v>42654</v>
+      </c>
+      <c r="J1" s="7">
+        <f>K1-7</f>
+        <v>42661</v>
+      </c>
+      <c r="K1" s="7">
+        <v>42668</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" s="1" customFormat="1" ht="16" thickBot="1">
+      <c r="A2" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="6" t="s">
+      <c r="B2" s="5"/>
+      <c r="C2" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D2" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J2" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K2" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L2" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M2" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="N2" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="O2" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="P2" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="Q2" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="R2" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="S2" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="T1" s="6" t="s">
+      <c r="T2" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="U1" s="6" t="s">
+      <c r="U2" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="V1" s="6" t="s">
+      <c r="V2" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="W1" s="6" t="s">
+      <c r="W2" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="X1" s="6" t="s">
+      <c r="X2" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="Y1" s="6" t="s">
+      <c r="Y2" s="6" t="s">
         <v>92</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25">
-      <c r="A2" s="2" t="str">
-        <f>CONCATENATE("['",$C2,"', ","'",$D2,"' ,",$E2,",",$F2,",",$G2,",",$H2,",",$I2,",",$J2,"],")</f>
-        <v>['Greg', '49ers' ,1,1,1,1,1,1],</v>
-      </c>
-      <c r="B2" s="3"/>
-      <c r="C2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" t="s">
-        <v>69</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2" s="2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:25">
       <c r="A3" s="2" t="str">
-        <f t="shared" ref="A3:A33" si="0">CONCATENATE("['",$C3,"', ","'",$D3,"' ,",$E3,",",$F3,",",$G3,",",$H3,",",$I3,",",$J3,"],")</f>
-        <v>['Jeff', 'Bears' ,0,0,0,1,1,1],</v>
+        <f>CONCATENATE("['",$C3,"', ","'",$D3,"' ,",$E3,",",$F3,",",$G3,",",$H3,",",$I3,",",$J3,",",$K3,",",$L3,"],")</f>
+        <v>['Greg', '49ers' ,1,1,1,1,1,1,1,1],</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D3" t="s">
-        <v>52</v>
+        <v>69</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3">
         <v>1</v>
@@ -1342,57 +1360,69 @@
         <v>1</v>
       </c>
       <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:25">
       <c r="A4" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>['Tim', 'Bengals' ,1,1,1,2,2,2],</v>
+        <f t="shared" ref="A4:A34" si="1">CONCATENATE("['",$C4,"', ","'",$D4,"' ,",$E4,",",$F4,",",$G4,",",$H4,",",$I4,",",$J4,",",$K4,",",$L4,"],")</f>
+        <v>['Jeff', 'Bears' ,0,0,0,1,1,1,1,2],</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D4" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:25">
       <c r="A5" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>['Greg', 'Bills' ,0,0,1,2,3,4],</v>
+        <f t="shared" si="1"/>
+        <v>['Tim', 'Bengals' ,1,1,1,2,2,2,3,3],</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D5" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -1401,119 +1431,143 @@
         <v>2</v>
       </c>
       <c r="I5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J5">
-        <v>4</v>
+        <v>2</v>
+      </c>
+      <c r="K5">
+        <v>3</v>
+      </c>
+      <c r="L5">
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:25">
       <c r="A6" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>['Zach', 'Broncos' ,1,2,3,4,4,4],</v>
+        <f t="shared" si="1"/>
+        <v>['Greg', 'Bills' ,0,0,1,2,3,4,4,4],</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D6" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H6">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J6">
+        <v>4</v>
+      </c>
+      <c r="K6">
+        <v>4</v>
+      </c>
+      <c r="L6">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:25">
       <c r="A7" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>['Jeff', 'Browns' ,0,0,0,0,0,0],</v>
+        <f t="shared" si="1"/>
+        <v>['Zach', 'Broncos' ,1,2,3,4,4,4,5,6],</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D7" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H7">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I7">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J7">
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="K7">
+        <v>5</v>
+      </c>
+      <c r="L7">
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:25">
       <c r="A8" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>['Zach', 'Buccaneers' ,1,1,1,1,2,2],</v>
+        <f t="shared" si="1"/>
+        <v>['Jeff', 'Browns' ,0,0,0,0,0,0,0,0],</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D8" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J8">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:25">
       <c r="A9" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>['Jeff', 'Cardinals' ,0,1,1,1,2,3],</v>
+        <f t="shared" si="1"/>
+        <v>['Zach', 'Buccaneers' ,1,1,1,1,2,2,3,3],</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D9" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9" s="2">
         <v>1</v>
@@ -1528,20 +1582,26 @@
         <v>2</v>
       </c>
       <c r="J9">
+        <v>2</v>
+      </c>
+      <c r="K9">
+        <v>3</v>
+      </c>
+      <c r="L9">
         <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:25">
       <c r="A10" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>['Jeff', 'Chargers' ,0,1,1,1,1,2],</v>
+        <f t="shared" si="1"/>
+        <v>['Jeff', 'Cardinals' ,0,1,1,1,2,3,3,3],</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" t="s">
         <v>32</v>
       </c>
       <c r="D10" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -1556,280 +1616,334 @@
         <v>1</v>
       </c>
       <c r="I10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J10">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="K10">
+        <v>3</v>
+      </c>
+      <c r="L10">
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:25">
       <c r="A11" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>['Zach', 'Chiefs' ,1,1,2,2,2,3],</v>
+        <f t="shared" si="1"/>
+        <v>['Jeff', 'Chargers' ,0,1,1,1,1,2,3,4],</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F11" s="2">
         <v>1</v>
       </c>
       <c r="G11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J11">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="K11">
+        <v>3</v>
+      </c>
+      <c r="L11">
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:25">
       <c r="A12" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>['Greg', 'Colts' ,0,0,1,1,2,2],</v>
+        <f t="shared" si="1"/>
+        <v>['Zach', 'Chiefs' ,1,1,2,2,2,3,4,5],</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D12" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I12">
         <v>2</v>
       </c>
       <c r="J12">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="K12">
+        <v>4</v>
+      </c>
+      <c r="L12">
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:25">
       <c r="A13" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>['Greg', 'Cowboys' ,0,1,2,3,4,5],</v>
+        <f t="shared" si="1"/>
+        <v>['Greg', 'Colts' ,0,0,1,1,2,2,3,3],</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" t="s">
         <v>33</v>
       </c>
       <c r="D13" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E13">
         <v>0</v>
       </c>
       <c r="F13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H13">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J13">
-        <v>5</v>
+        <v>2</v>
+      </c>
+      <c r="K13">
+        <v>3</v>
+      </c>
+      <c r="L13">
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:25">
       <c r="A14" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>['Tim', 'Dolphins' ,0,0,1,1,1,2],</v>
+        <f t="shared" si="1"/>
+        <v>['Greg', 'Cowboys' ,0,1,2,3,4,5,5,6],</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D14" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="E14">
         <v>0</v>
       </c>
       <c r="F14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H14">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I14">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J14">
-        <v>2</v>
+        <v>5</v>
+      </c>
+      <c r="K14">
+        <v>5</v>
+      </c>
+      <c r="L14">
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:25">
       <c r="A15" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>['Zach', 'Eagles' ,1,2,3,3,3,3],</v>
+        <f t="shared" si="1"/>
+        <v>['Tim', 'Dolphins' ,0,0,1,1,1,2,3,3],</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D15" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="E15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F15" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G15">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H15">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I15">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J15">
+        <v>2</v>
+      </c>
+      <c r="K15">
+        <v>3</v>
+      </c>
+      <c r="L15">
         <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:25">
       <c r="A16" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>['Greg', 'Falcons' ,0,1,2,3,4,4],</v>
+        <f t="shared" si="1"/>
+        <v>['Zach', 'Eagles' ,1,2,3,3,3,3,4,4],</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D16" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G16">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H16">
         <v>3</v>
       </c>
       <c r="I16">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J16">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10">
+        <v>3</v>
+      </c>
+      <c r="K16">
+        <v>4</v>
+      </c>
+      <c r="L16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
       <c r="A17" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>['Jeff', 'Giants' ,1,2,2,2,2,3],</v>
+        <f t="shared" si="1"/>
+        <v>['Greg', 'Falcons' ,0,1,2,3,4,4,4,5],</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D17" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F17" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G17">
         <v>2</v>
       </c>
       <c r="H17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I17">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10">
+        <v>4</v>
+      </c>
+      <c r="K17">
+        <v>4</v>
+      </c>
+      <c r="L17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
       <c r="A18" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>['Tim', 'Jaguars' ,0,0,0,1,1,2],</v>
+        <f t="shared" si="1"/>
+        <v>['Jeff', 'Giants' ,1,2,2,2,2,3,4,4],</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D18" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F18" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10">
+        <v>3</v>
+      </c>
+      <c r="K18">
+        <v>4</v>
+      </c>
+      <c r="L18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
       <c r="A19" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>['Tim', 'Jets' ,0,1,1,1,1,1],</v>
+        <f t="shared" si="1"/>
+        <v>['Tim', 'Jaguars' ,0,0,0,1,1,2,2,2],</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" t="s">
         <v>34</v>
       </c>
       <c r="D19" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E19">
         <v>0</v>
       </c>
       <c r="F19" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H19">
         <v>1</v>
@@ -1838,23 +1952,29 @@
         <v>1</v>
       </c>
       <c r="J19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10">
+        <v>2</v>
+      </c>
+      <c r="K19">
+        <v>2</v>
+      </c>
+      <c r="L19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
       <c r="A20" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>['Jeff', 'Lions' ,1,1,1,1,2,3],</v>
+        <f t="shared" si="1"/>
+        <v>['Tim', 'Jets' ,0,1,1,1,1,1,2,3],</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D20" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="E20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F20" s="2">
         <v>1</v>
@@ -1866,23 +1986,29 @@
         <v>1</v>
       </c>
       <c r="I20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J20">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10">
+        <v>1</v>
+      </c>
+      <c r="K20">
+        <v>2</v>
+      </c>
+      <c r="L20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
       <c r="A21" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>['Tim', 'Packers' ,1,1,2,2,3,3],</v>
+        <f t="shared" si="1"/>
+        <v>['Jeff', 'Lions' ,1,1,1,1,2,3,4,4],</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D21" t="s">
-        <v>41</v>
+        <v>62</v>
       </c>
       <c r="E21">
         <v>1</v>
@@ -1891,100 +2017,118 @@
         <v>1</v>
       </c>
       <c r="G21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I21">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J21">
         <v>3</v>
       </c>
-    </row>
-    <row r="22" spans="1:10">
+      <c r="K21">
+        <v>4</v>
+      </c>
+      <c r="L21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
       <c r="A22" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>['Greg', 'Panthers' ,0,1,1,1,1,1],</v>
+        <f t="shared" si="1"/>
+        <v>['Tim', 'Packers' ,1,1,2,2,3,3,4,4],</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D22" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F22" s="2">
         <v>1</v>
       </c>
       <c r="G22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I22">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10">
+        <v>3</v>
+      </c>
+      <c r="K22">
+        <v>4</v>
+      </c>
+      <c r="L22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
       <c r="A23" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>['Greg', 'Patriots' ,1,2,3,3,4,5],</v>
+        <f t="shared" si="1"/>
+        <v>['Greg', 'Panthers' ,0,1,1,1,1,1,1,2],</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" t="s">
         <v>33</v>
       </c>
       <c r="D23" t="s">
-        <v>64</v>
+        <v>39</v>
       </c>
       <c r="E23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F23" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G23">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H23">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I23">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J23">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10">
+        <v>1</v>
+      </c>
+      <c r="K23">
+        <v>1</v>
+      </c>
+      <c r="L23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
       <c r="A24" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>['Tim', 'Raiders' ,1,1,2,3,4,4],</v>
+        <f t="shared" si="1"/>
+        <v>['Greg', 'Patriots' ,1,2,3,3,4,5,6,7],</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D24" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="E24">
         <v>1</v>
       </c>
       <c r="F24" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G24">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H24">
         <v>3</v>
@@ -1993,23 +2137,29 @@
         <v>4</v>
       </c>
       <c r="J24">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10">
+        <v>5</v>
+      </c>
+      <c r="K24">
+        <v>6</v>
+      </c>
+      <c r="L24">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
       <c r="A25" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>['Zach', 'Rams' ,0,1,2,3,3,3],</v>
+        <f t="shared" si="1"/>
+        <v>['Tim', 'Raiders' ,1,1,2,3,4,4,5,6],</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D25" t="s">
-        <v>68</v>
+        <v>45</v>
       </c>
       <c r="E25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F25" s="2">
         <v>1</v>
@@ -2021,32 +2171,38 @@
         <v>3</v>
       </c>
       <c r="I25">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J25">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10">
+        <v>4</v>
+      </c>
+      <c r="K25">
+        <v>5</v>
+      </c>
+      <c r="L25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
       <c r="A26" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>['Jeff', 'Ravens' ,1,2,3,3,3,3],</v>
+        <f t="shared" si="1"/>
+        <v>['Zach', 'Rams' ,0,1,2,3,3,3,3,3],</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D26" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="E26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F26" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G26">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H26">
         <v>3</v>
@@ -2057,49 +2213,61 @@
       <c r="J26">
         <v>3</v>
       </c>
-    </row>
-    <row r="27" spans="1:10">
+      <c r="K26">
+        <v>3</v>
+      </c>
+      <c r="L26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
       <c r="A27" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>['Greg', 'Redskins' ,0,0,1,2,3,4],</v>
+        <f t="shared" si="1"/>
+        <v>['Jeff', 'Ravens' ,1,2,3,3,3,3,3,3],</v>
       </c>
       <c r="B27" s="3"/>
       <c r="C27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D27" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="E27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F27" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G27">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H27">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I27">
         <v>3</v>
       </c>
       <c r="J27">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10">
+        <v>3</v>
+      </c>
+      <c r="K27">
+        <v>3</v>
+      </c>
+      <c r="L27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
       <c r="A28" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>['Zach', 'Saints' ,0,0,0,1,1,2],</v>
+        <f t="shared" si="1"/>
+        <v>['Greg', 'Redskins' ,0,0,1,2,3,4,4,4],</v>
       </c>
       <c r="B28" s="3"/>
       <c r="C28" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D28" t="s">
-        <v>46</v>
+        <v>67</v>
       </c>
       <c r="E28">
         <v>0</v>
@@ -2108,66 +2276,78 @@
         <v>0</v>
       </c>
       <c r="G28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H28">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I28">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J28">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10">
+        <v>4</v>
+      </c>
+      <c r="K28">
+        <v>4</v>
+      </c>
+      <c r="L28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
       <c r="A29" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>['Zach', 'Seahawks' ,1,1,2,3,3,4],</v>
+        <f t="shared" si="1"/>
+        <v>['Zach', 'Saints' ,0,0,0,1,1,2,2,3],</v>
       </c>
       <c r="B29" s="3"/>
       <c r="C29" t="s">
         <v>35</v>
       </c>
       <c r="D29" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="E29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F29" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G29">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H29">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I29">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J29">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10">
+        <v>2</v>
+      </c>
+      <c r="K29">
+        <v>2</v>
+      </c>
+      <c r="L29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
       <c r="A30" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>['Tim', 'Steelers' ,1,2,2,3,4,4],</v>
+        <f t="shared" si="1"/>
+        <v>['Zach', 'Seahawks' ,1,1,2,3,3,4,4,4],</v>
       </c>
       <c r="B30" s="3"/>
       <c r="C30" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D30" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="E30">
         <v>1</v>
       </c>
       <c r="F30" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G30">
         <v>2</v>
@@ -2176,23 +2356,29 @@
         <v>3</v>
       </c>
       <c r="I30">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J30">
         <v>4</v>
       </c>
-    </row>
-    <row r="31" spans="1:10">
+      <c r="K30">
+        <v>4</v>
+      </c>
+      <c r="L30">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
       <c r="A31" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>['Jeff', 'Texans' ,1,2,2,3,3,4],</v>
+        <f t="shared" si="1"/>
+        <v>['Tim', 'Steelers' ,1,2,2,3,4,4,4,4],</v>
       </c>
       <c r="B31" s="3"/>
       <c r="C31" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D31" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="E31">
         <v>1</v>
@@ -2207,193 +2393,280 @@
         <v>3</v>
       </c>
       <c r="I31">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J31">
         <v>4</v>
       </c>
-    </row>
-    <row r="32" spans="1:10">
+      <c r="K31">
+        <v>4</v>
+      </c>
+      <c r="L31">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
       <c r="A32" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>['Zach', 'Titans' ,0,1,1,1,2,3],</v>
+        <f t="shared" si="1"/>
+        <v>['Jeff', 'Texans' ,1,2,2,3,3,4,4,5],</v>
       </c>
       <c r="B32" s="3"/>
       <c r="C32" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D32" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F32" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G32">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H32">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I32">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J32">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10">
+        <v>4</v>
+      </c>
+      <c r="K32">
+        <v>4</v>
+      </c>
+      <c r="L32">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12">
       <c r="A33" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>['Tim', 'Vikings' ,1,2,3,4,5,5],</v>
+        <f t="shared" si="1"/>
+        <v>['Zach', 'Titans' ,0,1,1,1,2,3,3,4],</v>
       </c>
       <c r="B33" s="3"/>
       <c r="C33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D33" t="s">
+        <v>51</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33" s="2">
+        <v>1</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+      <c r="H33">
+        <v>1</v>
+      </c>
+      <c r="I33">
+        <v>2</v>
+      </c>
+      <c r="J33">
+        <v>3</v>
+      </c>
+      <c r="K33">
+        <v>3</v>
+      </c>
+      <c r="L33">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12">
+      <c r="A34" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>['Tim', 'Vikings' ,1,2,3,4,5,5,5,5],</v>
+      </c>
+      <c r="B34" s="3"/>
+      <c r="C34" t="s">
         <v>34</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D34" t="s">
         <v>74</v>
       </c>
-      <c r="E33">
-        <v>1</v>
-      </c>
-      <c r="F33" s="2">
-        <v>2</v>
-      </c>
-      <c r="G33">
-        <v>3</v>
-      </c>
-      <c r="H33">
-        <v>4</v>
-      </c>
-      <c r="I33">
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34" s="2">
+        <v>2</v>
+      </c>
+      <c r="G34">
+        <v>3</v>
+      </c>
+      <c r="H34">
+        <v>4</v>
+      </c>
+      <c r="I34">
         <v>5</v>
       </c>
-      <c r="J33">
+      <c r="J34">
         <v>5</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" s="4" customFormat="1" ht="4" customHeight="1">
-      <c r="A34" s="3"/>
-      <c r="B34" s="3"/>
-      <c r="F34" s="3"/>
-    </row>
-    <row r="35" spans="1:10">
-      <c r="D35" t="s">
+      <c r="K34">
+        <v>5</v>
+      </c>
+      <c r="L34">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" s="4" customFormat="1" ht="4" customHeight="1">
+      <c r="A35" s="3"/>
+      <c r="B35" s="3"/>
+      <c r="F35" s="3"/>
+    </row>
+    <row r="36" spans="1:12">
+      <c r="D36" t="s">
         <v>32</v>
       </c>
-      <c r="E35">
-        <f t="shared" ref="E35:J37" si="1">SUMIF($C$2:$C$33,$D35,E$2:E$33)</f>
-        <v>4</v>
-      </c>
-      <c r="F35" s="2">
-        <f t="shared" si="1"/>
+      <c r="E36">
+        <f t="shared" ref="E36:L38" si="2">SUMIF($C$3:$C$34,$D36,E$3:E$34)</f>
+        <v>4</v>
+      </c>
+      <c r="F36" s="2">
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="G35" s="2">
-        <f t="shared" si="1"/>
+      <c r="G36" s="2">
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="H35" s="2">
-        <f t="shared" si="1"/>
+      <c r="H36" s="2">
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="I35" s="2">
-        <f t="shared" si="1"/>
+      <c r="I36" s="2">
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
-      <c r="J35" s="2">
-        <f t="shared" si="1"/>
+      <c r="J36" s="2">
+        <f t="shared" si="2"/>
         <v>19</v>
       </c>
-    </row>
-    <row r="36" spans="1:10">
-      <c r="D36" t="s">
+      <c r="K36" s="2">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="L36" s="2">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12">
+      <c r="D37" t="s">
         <v>33</v>
       </c>
-      <c r="E36">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="F36" s="2">
-        <f t="shared" si="1"/>
+      <c r="E37">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="F37" s="2">
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="G36" s="2">
-        <f t="shared" si="1"/>
+      <c r="G37" s="2">
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="H36" s="2">
-        <f t="shared" si="1"/>
+      <c r="H37" s="2">
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
-      <c r="I36" s="2">
-        <f t="shared" si="1"/>
+      <c r="I37" s="2">
+        <f t="shared" si="2"/>
         <v>22</v>
       </c>
-      <c r="J36" s="2">
-        <f t="shared" si="1"/>
+      <c r="J37" s="2">
+        <f t="shared" si="2"/>
         <v>26</v>
       </c>
-    </row>
-    <row r="37" spans="1:10">
-      <c r="D37" t="s">
+      <c r="K37" s="2">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="L37" s="2">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12">
+      <c r="D38" t="s">
         <v>34</v>
       </c>
-      <c r="E37">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="F37" s="2">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="G37" s="2">
-        <f t="shared" si="1"/>
-        <v>12</v>
-      </c>
-      <c r="H37" s="2">
-        <f t="shared" si="1"/>
-        <v>17</v>
-      </c>
-      <c r="I37" s="2">
-        <f t="shared" si="1"/>
-        <v>21</v>
-      </c>
-      <c r="J37" s="2">
-        <f t="shared" si="1"/>
-        <v>23</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10">
-      <c r="D38" t="s">
-        <v>35</v>
-      </c>
       <c r="E38">
-        <f t="shared" ref="E38:J38" si="2">SUMIF($C$2:$C$33,$D$38,E$2:E$33)</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="F38" s="2">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G38" s="2">
         <f t="shared" si="2"/>
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H38" s="2">
         <f t="shared" si="2"/>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I38" s="2">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J38" s="2">
         <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="K38" s="2">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="L38" s="2">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12">
+      <c r="D39" t="s">
+        <v>35</v>
+      </c>
+      <c r="E39">
+        <f t="shared" ref="E39:L39" si="3">SUMIF($C$3:$C$34,$D$39,E$3:E$34)</f>
+        <v>5</v>
+      </c>
+      <c r="F39" s="2">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="G39" s="2">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+      <c r="H39" s="2">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
+      <c r="I39" s="2">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="J39" s="2">
+        <f t="shared" si="3"/>
         <v>24</v>
+      </c>
+      <c r="K39" s="2">
+        <f t="shared" si="3"/>
+        <v>28</v>
+      </c>
+      <c r="L39" s="2">
+        <f t="shared" si="3"/>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added the week 9 scores.
</commit_message>
<xml_diff>
--- a/NFL Wins.xlsx
+++ b/NFL Wins.xlsx
@@ -388,8 +388,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="93">
+  <cellStyleXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -497,7 +499,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="93">
+  <cellStyles count="95">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -544,6 +546,7 @@
     <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -590,6 +593,7 @@
     <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1209,8 +1213,8 @@
   <dimension ref="A1:Y39"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" topLeftCell="A2" workbookViewId="0">
-      <pane xSplit="4" topLeftCell="K1" activePane="topRight" state="frozenSplit"/>
-      <selection pane="topRight" activeCell="M34" sqref="M34"/>
+      <pane xSplit="4" topLeftCell="L1" activePane="topRight" state="frozenSplit"/>
+      <selection pane="topRight" activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1334,8 +1338,8 @@
     </row>
     <row r="3" spans="1:25">
       <c r="A3" s="2" t="str">
-        <f>CONCATENATE("['",$C3,"', ","'",$D3,"' ,",$E3,",",$F3,",",$G3,",",$H3,",",$I3,",",$J3,",",$K3,",",$L3,"],")</f>
-        <v>['Greg', '49ers' ,1,1,1,1,1,1,1,1],</v>
+        <f>CONCATENATE("['",$C3,"', ","'",$D3,"' ,",$E3,",",$F3,",",$G3,",",$H3,",",$I3,",",$J3,",",$K3,",",$L3,",",$M3,"],")</f>
+        <v>['Greg', '49ers' ,1,1,1,1,1,1,1,1,1],</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" t="s">
@@ -1368,11 +1372,14 @@
       <c r="L3">
         <v>1</v>
       </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:25">
       <c r="A4" s="2" t="str">
-        <f t="shared" ref="A4:A34" si="1">CONCATENATE("['",$C4,"', ","'",$D4,"' ,",$E4,",",$F4,",",$G4,",",$H4,",",$I4,",",$J4,",",$K4,",",$L4,"],")</f>
-        <v>['Jeff', 'Bears' ,0,0,0,1,1,1,1,2],</v>
+        <f t="shared" ref="A4:A34" si="1">CONCATENATE("['",$C4,"', ","'",$D4,"' ,",$E4,",",$F4,",",$G4,",",$H4,",",$I4,",",$J4,",",$K4,",",$L4,",",$M4,"],")</f>
+        <v>['Jeff', 'Bears' ,0,0,0,1,1,1,1,2,2],</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" t="s">
@@ -1405,11 +1412,14 @@
       <c r="L4">
         <v>2</v>
       </c>
+      <c r="M4">
+        <v>2</v>
+      </c>
     </row>
     <row r="5" spans="1:25">
       <c r="A5" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Tim', 'Bengals' ,1,1,1,2,2,2,3,3],</v>
+        <v>['Tim', 'Bengals' ,1,1,1,2,2,2,3,3,3],</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" t="s">
@@ -1442,11 +1452,14 @@
       <c r="L5">
         <v>3</v>
       </c>
+      <c r="M5">
+        <v>3</v>
+      </c>
     </row>
     <row r="6" spans="1:25">
       <c r="A6" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Greg', 'Bills' ,0,0,1,2,3,4,4,4],</v>
+        <v>['Greg', 'Bills' ,0,0,1,2,3,4,4,4,4],</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" t="s">
@@ -1479,11 +1492,14 @@
       <c r="L6">
         <v>4</v>
       </c>
+      <c r="M6">
+        <v>4</v>
+      </c>
     </row>
     <row r="7" spans="1:25">
       <c r="A7" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Zach', 'Broncos' ,1,2,3,4,4,4,5,6],</v>
+        <v>['Zach', 'Broncos' ,1,2,3,4,4,4,5,6,6],</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" t="s">
@@ -1516,11 +1532,14 @@
       <c r="L7">
         <v>6</v>
       </c>
+      <c r="M7">
+        <v>6</v>
+      </c>
     </row>
     <row r="8" spans="1:25">
       <c r="A8" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Jeff', 'Browns' ,0,0,0,0,0,0,0,0],</v>
+        <v>['Jeff', 'Browns' ,0,0,0,0,0,0,0,0,0],</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" t="s">
@@ -1553,11 +1572,14 @@
       <c r="L8">
         <v>0</v>
       </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:25">
       <c r="A9" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Zach', 'Buccaneers' ,1,1,1,1,2,2,3,3],</v>
+        <v>['Zach', 'Buccaneers' ,1,1,1,1,2,2,3,3,3],</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" t="s">
@@ -1590,11 +1612,14 @@
       <c r="L9">
         <v>3</v>
       </c>
+      <c r="M9">
+        <v>3</v>
+      </c>
     </row>
     <row r="10" spans="1:25">
       <c r="A10" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Jeff', 'Cardinals' ,0,1,1,1,2,3,3,3],</v>
+        <v>['Jeff', 'Cardinals' ,0,1,1,1,2,3,3,3,3],</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" t="s">
@@ -1627,11 +1652,14 @@
       <c r="L10">
         <v>3</v>
       </c>
+      <c r="M10">
+        <v>3</v>
+      </c>
     </row>
     <row r="11" spans="1:25">
       <c r="A11" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Jeff', 'Chargers' ,0,1,1,1,1,2,3,4],</v>
+        <v>['Jeff', 'Chargers' ,0,1,1,1,1,2,3,3,4],</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" t="s">
@@ -1662,13 +1690,16 @@
         <v>3</v>
       </c>
       <c r="L11">
+        <v>3</v>
+      </c>
+      <c r="M11">
         <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:25">
       <c r="A12" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Zach', 'Chiefs' ,1,1,2,2,2,3,4,5],</v>
+        <v>['Zach', 'Chiefs' ,1,1,2,2,2,3,4,5,6],</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" t="s">
@@ -1701,11 +1732,14 @@
       <c r="L12">
         <v>5</v>
       </c>
+      <c r="M12">
+        <v>6</v>
+      </c>
     </row>
     <row r="13" spans="1:25">
       <c r="A13" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Greg', 'Colts' ,0,0,1,1,2,2,3,3],</v>
+        <v>['Greg', 'Colts' ,0,0,1,1,2,2,3,3,4],</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" t="s">
@@ -1738,11 +1772,14 @@
       <c r="L13">
         <v>3</v>
       </c>
+      <c r="M13">
+        <v>4</v>
+      </c>
     </row>
     <row r="14" spans="1:25">
       <c r="A14" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Greg', 'Cowboys' ,0,1,2,3,4,5,5,6],</v>
+        <v>['Greg', 'Cowboys' ,0,1,2,3,4,5,5,6,7],</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" t="s">
@@ -1775,11 +1812,14 @@
       <c r="L14">
         <v>6</v>
       </c>
+      <c r="M14">
+        <v>7</v>
+      </c>
     </row>
     <row r="15" spans="1:25">
       <c r="A15" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Tim', 'Dolphins' ,0,0,1,1,1,2,3,3],</v>
+        <v>['Tim', 'Dolphins' ,0,0,1,1,1,2,3,3,4],</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" t="s">
@@ -1812,11 +1852,14 @@
       <c r="L15">
         <v>3</v>
       </c>
+      <c r="M15">
+        <v>4</v>
+      </c>
     </row>
     <row r="16" spans="1:25">
       <c r="A16" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Zach', 'Eagles' ,1,2,3,3,3,3,4,4],</v>
+        <v>['Zach', 'Eagles' ,1,2,3,3,3,3,4,4,4],</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" t="s">
@@ -1849,11 +1892,14 @@
       <c r="L16">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="1:12">
+      <c r="M16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
       <c r="A17" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Greg', 'Falcons' ,0,1,2,3,4,4,4,5],</v>
+        <v>['Greg', 'Falcons' ,0,1,2,3,4,4,4,5,6],</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" t="s">
@@ -1886,11 +1932,14 @@
       <c r="L17">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:12">
+      <c r="M17">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
       <c r="A18" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Jeff', 'Giants' ,1,2,2,2,2,3,4,4],</v>
+        <v>['Jeff', 'Giants' ,1,2,2,2,2,3,4,4,5],</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" t="s">
@@ -1923,11 +1972,14 @@
       <c r="L18">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="1:12">
+      <c r="M18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
       <c r="A19" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Tim', 'Jaguars' ,0,0,0,1,1,2,2,2],</v>
+        <v>['Tim', 'Jaguars' ,0,0,0,1,1,2,2,2,2],</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" t="s">
@@ -1960,11 +2012,14 @@
       <c r="L19">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:12">
+      <c r="M19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
       <c r="A20" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Tim', 'Jets' ,0,1,1,1,1,1,2,3],</v>
+        <v>['Tim', 'Jets' ,0,1,1,1,1,1,2,3,3],</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" t="s">
@@ -1997,11 +2052,14 @@
       <c r="L20">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="1:12">
+      <c r="M20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
       <c r="A21" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Jeff', 'Lions' ,1,1,1,1,2,3,4,4],</v>
+        <v>['Jeff', 'Lions' ,1,1,1,1,2,3,4,4,5],</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" t="s">
@@ -2034,11 +2092,14 @@
       <c r="L21">
         <v>4</v>
       </c>
-    </row>
-    <row r="22" spans="1:12">
+      <c r="M21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
       <c r="A22" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Tim', 'Packers' ,1,1,2,2,3,3,4,4],</v>
+        <v>['Tim', 'Packers' ,1,1,2,2,3,3,4,4,4],</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" t="s">
@@ -2071,11 +2132,14 @@
       <c r="L22">
         <v>4</v>
       </c>
-    </row>
-    <row r="23" spans="1:12">
+      <c r="M22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
       <c r="A23" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Greg', 'Panthers' ,0,1,1,1,1,1,1,2],</v>
+        <v>['Greg', 'Panthers' ,0,1,1,1,1,1,1,2,3],</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" t="s">
@@ -2108,11 +2172,14 @@
       <c r="L23">
         <v>2</v>
       </c>
-    </row>
-    <row r="24" spans="1:12">
+      <c r="M23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
       <c r="A24" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Greg', 'Patriots' ,1,2,3,3,4,5,6,7],</v>
+        <v>['Greg', 'Patriots' ,1,2,3,3,4,5,6,7,7],</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" t="s">
@@ -2145,11 +2212,14 @@
       <c r="L24">
         <v>7</v>
       </c>
-    </row>
-    <row r="25" spans="1:12">
+      <c r="M24">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
       <c r="A25" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Tim', 'Raiders' ,1,1,2,3,4,4,5,6],</v>
+        <v>['Tim', 'Raiders' ,1,1,2,3,4,4,5,6,7],</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" t="s">
@@ -2182,11 +2252,14 @@
       <c r="L25">
         <v>6</v>
       </c>
-    </row>
-    <row r="26" spans="1:12">
+      <c r="M25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
       <c r="A26" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Zach', 'Rams' ,0,1,2,3,3,3,3,3],</v>
+        <v>['Zach', 'Rams' ,0,1,2,3,3,3,3,3,3],</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" t="s">
@@ -2219,11 +2292,14 @@
       <c r="L26">
         <v>3</v>
       </c>
-    </row>
-    <row r="27" spans="1:12">
+      <c r="M26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13">
       <c r="A27" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Jeff', 'Ravens' ,1,2,3,3,3,3,3,3],</v>
+        <v>['Jeff', 'Ravens' ,1,2,3,3,3,3,3,3,4],</v>
       </c>
       <c r="B27" s="3"/>
       <c r="C27" t="s">
@@ -2256,11 +2332,14 @@
       <c r="L27">
         <v>3</v>
       </c>
-    </row>
-    <row r="28" spans="1:12">
+      <c r="M27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13">
       <c r="A28" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Greg', 'Redskins' ,0,0,1,2,3,4,4,4],</v>
+        <v>['Greg', 'Redskins' ,0,0,1,2,3,4,4,4,4],</v>
       </c>
       <c r="B28" s="3"/>
       <c r="C28" t="s">
@@ -2293,11 +2372,14 @@
       <c r="L28">
         <v>4</v>
       </c>
-    </row>
-    <row r="29" spans="1:12">
+      <c r="M28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13">
       <c r="A29" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Zach', 'Saints' ,0,0,0,1,1,2,2,3],</v>
+        <v>['Zach', 'Saints' ,0,0,0,1,1,2,2,3,4],</v>
       </c>
       <c r="B29" s="3"/>
       <c r="C29" t="s">
@@ -2330,11 +2412,14 @@
       <c r="L29">
         <v>3</v>
       </c>
-    </row>
-    <row r="30" spans="1:12">
+      <c r="M29">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13">
       <c r="A30" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Zach', 'Seahawks' ,1,1,2,3,3,4,4,4],</v>
+        <v>['Zach', 'Seahawks' ,1,1,2,3,3,4,4,4,5],</v>
       </c>
       <c r="B30" s="3"/>
       <c r="C30" t="s">
@@ -2367,11 +2452,14 @@
       <c r="L30">
         <v>4</v>
       </c>
-    </row>
-    <row r="31" spans="1:12">
+      <c r="M30">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13">
       <c r="A31" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Tim', 'Steelers' ,1,2,2,3,4,4,4,4],</v>
+        <v>['Tim', 'Steelers' ,1,2,2,3,4,4,4,4,4],</v>
       </c>
       <c r="B31" s="3"/>
       <c r="C31" t="s">
@@ -2404,11 +2492,14 @@
       <c r="L31">
         <v>4</v>
       </c>
-    </row>
-    <row r="32" spans="1:12">
+      <c r="M31">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13">
       <c r="A32" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Jeff', 'Texans' ,1,2,2,3,3,4,4,5],</v>
+        <v>['Jeff', 'Texans' ,1,2,2,3,3,4,4,5,5],</v>
       </c>
       <c r="B32" s="3"/>
       <c r="C32" t="s">
@@ -2441,11 +2532,14 @@
       <c r="L32">
         <v>5</v>
       </c>
-    </row>
-    <row r="33" spans="1:12">
+      <c r="M32">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13">
       <c r="A33" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Zach', 'Titans' ,0,1,1,1,2,3,3,4],</v>
+        <v>['Zach', 'Titans' ,0,1,1,1,2,3,3,4,4],</v>
       </c>
       <c r="B33" s="3"/>
       <c r="C33" t="s">
@@ -2478,11 +2572,14 @@
       <c r="L33">
         <v>4</v>
       </c>
-    </row>
-    <row r="34" spans="1:12">
+      <c r="M33">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13">
       <c r="A34" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Tim', 'Vikings' ,1,2,3,4,5,5,5,5],</v>
+        <v>['Tim', 'Vikings' ,1,2,3,4,5,5,5,5,5],</v>
       </c>
       <c r="B34" s="3"/>
       <c r="C34" t="s">
@@ -2515,18 +2612,21 @@
       <c r="L34">
         <v>5</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" s="4" customFormat="1" ht="4" customHeight="1">
+      <c r="M34">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" s="4" customFormat="1" ht="4" customHeight="1">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="F35" s="3"/>
     </row>
-    <row r="36" spans="1:12">
+    <row r="36" spans="1:13">
       <c r="D36" t="s">
         <v>32</v>
       </c>
       <c r="E36">
-        <f t="shared" ref="E36:L38" si="2">SUMIF($C$3:$C$34,$D36,E$3:E$34)</f>
+        <f t="shared" ref="E36:M38" si="2">SUMIF($C$3:$C$34,$D36,E$3:E$34)</f>
         <v>4</v>
       </c>
       <c r="F36" s="2">
@@ -2555,10 +2655,14 @@
       </c>
       <c r="L36" s="2">
         <f t="shared" si="2"/>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12">
+        <v>24</v>
+      </c>
+      <c r="M36" s="2">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13">
       <c r="D37" t="s">
         <v>33</v>
       </c>
@@ -2594,8 +2698,12 @@
         <f t="shared" si="2"/>
         <v>32</v>
       </c>
-    </row>
-    <row r="38" spans="1:12">
+      <c r="M37" s="2">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13">
       <c r="D38" t="s">
         <v>34</v>
       </c>
@@ -2631,13 +2739,17 @@
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
-    </row>
-    <row r="39" spans="1:12">
+      <c r="M38" s="2">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13">
       <c r="D39" t="s">
         <v>35</v>
       </c>
       <c r="E39">
-        <f t="shared" ref="E39:L39" si="3">SUMIF($C$3:$C$34,$D$39,E$3:E$34)</f>
+        <f t="shared" ref="E39:M39" si="3">SUMIF($C$3:$C$34,$D$39,E$3:E$34)</f>
         <v>5</v>
       </c>
       <c r="F39" s="2">
@@ -2667,6 +2779,10 @@
       <c r="L39" s="2">
         <f t="shared" si="3"/>
         <v>32</v>
+      </c>
+      <c r="M39" s="2">
+        <f t="shared" si="3"/>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added initial NBA wins
</commit_message>
<xml_diff>
--- a/NFL Wins.xlsx
+++ b/NFL Wins.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9780" windowHeight="16100" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20720" windowHeight="16100" tabRatio="500" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
-    <sheet name="Auto" sheetId="2" r:id="rId2"/>
+    <sheet name="NFL" sheetId="2" r:id="rId2"/>
+    <sheet name="NBA" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="teams" localSheetId="0">Original!$A$2:$G$9</definedName>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="123">
   <si>
     <t>Arizona Cardinals</t>
   </si>
@@ -317,6 +318,96 @@
   </si>
   <si>
     <t>SuperBowl</t>
+  </si>
+  <si>
+    <t>Charlotte</t>
+  </si>
+  <si>
+    <t>Cleveland</t>
+  </si>
+  <si>
+    <t>Atlanta</t>
+  </si>
+  <si>
+    <t>Chicago</t>
+  </si>
+  <si>
+    <t>Boston</t>
+  </si>
+  <si>
+    <t>Brooklyn</t>
+  </si>
+  <si>
+    <t>Detroit</t>
+  </si>
+  <si>
+    <t>Indiana</t>
+  </si>
+  <si>
+    <t>Miami</t>
+  </si>
+  <si>
+    <t>Toronto</t>
+  </si>
+  <si>
+    <t>Orlando</t>
+  </si>
+  <si>
+    <t>Milwaukee</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>Philadelphia</t>
+  </si>
+  <si>
+    <t>Washington</t>
+  </si>
+  <si>
+    <t>Oklahoma City</t>
+  </si>
+  <si>
+    <t>San Antonio</t>
+  </si>
+  <si>
+    <t>Denver</t>
+  </si>
+  <si>
+    <t>LA Clippers</t>
+  </si>
+  <si>
+    <t>Memphis</t>
+  </si>
+  <si>
+    <t>Golden State</t>
+  </si>
+  <si>
+    <t>Houston</t>
+  </si>
+  <si>
+    <t>L.A. Lakers</t>
+  </si>
+  <si>
+    <t>Portland</t>
+  </si>
+  <si>
+    <t>Sacramento</t>
+  </si>
+  <si>
+    <t>Utah</t>
+  </si>
+  <si>
+    <t>Dallas</t>
+  </si>
+  <si>
+    <t>New Orleans</t>
+  </si>
+  <si>
+    <t>Phoenix</t>
+  </si>
+  <si>
+    <t>Minnesota</t>
   </si>
 </sst>
 </file>
@@ -388,7 +479,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="95">
+  <cellStyleXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -484,8 +575,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -498,8 +593,9 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="95">
+  <cellStyles count="99">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -547,6 +643,10 @@
     <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1214,7 +1314,7 @@
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" topLeftCell="A2" workbookViewId="0">
       <pane xSplit="4" topLeftCell="L1" activePane="topRight" state="frozenSplit"/>
-      <selection pane="topRight" activeCell="M2" sqref="M2"/>
+      <selection pane="topRight" activeCell="N36" sqref="N36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1338,8 +1438,8 @@
     </row>
     <row r="3" spans="1:25">
       <c r="A3" s="2" t="str">
-        <f>CONCATENATE("['",$C3,"', ","'",$D3,"' ,",$E3,",",$F3,",",$G3,",",$H3,",",$I3,",",$J3,",",$K3,",",$L3,",",$M3,"],")</f>
-        <v>['Greg', '49ers' ,1,1,1,1,1,1,1,1,1],</v>
+        <f>CONCATENATE("['",$C3,"', ","'",$D3,"' ,",$E3,",",$F3,",",$G3,",",$H3,",",$I3,",",$J3,",",$K3,",",$L3,",",$M3,",",$N3,"],")</f>
+        <v>['Greg', '49ers' ,1,1,1,1,1,1,1,1,1,],</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" t="s">
@@ -1378,8 +1478,8 @@
     </row>
     <row r="4" spans="1:25">
       <c r="A4" s="2" t="str">
-        <f t="shared" ref="A4:A34" si="1">CONCATENATE("['",$C4,"', ","'",$D4,"' ,",$E4,",",$F4,",",$G4,",",$H4,",",$I4,",",$J4,",",$K4,",",$L4,",",$M4,"],")</f>
-        <v>['Jeff', 'Bears' ,0,0,0,1,1,1,1,2,2],</v>
+        <f t="shared" ref="A4:A34" si="1">CONCATENATE("['",$C4,"', ","'",$D4,"' ,",$E4,",",$F4,",",$G4,",",$H4,",",$I4,",",$J4,",",$K4,",",$L4,",",$M4,",",$N4,"],")</f>
+        <v>['Jeff', 'Bears' ,0,0,0,1,1,1,1,2,2,2],</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" t="s">
@@ -1415,11 +1515,14 @@
       <c r="M4">
         <v>2</v>
       </c>
+      <c r="N4">
+        <v>2</v>
+      </c>
     </row>
     <row r="5" spans="1:25">
       <c r="A5" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Tim', 'Bengals' ,1,1,1,2,2,2,3,3,3],</v>
+        <v>['Tim', 'Bengals' ,1,1,1,2,2,2,3,3,3,],</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" t="s">
@@ -1459,7 +1562,7 @@
     <row r="6" spans="1:25">
       <c r="A6" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Greg', 'Bills' ,0,0,1,2,3,4,4,4,4],</v>
+        <v>['Greg', 'Bills' ,0,0,1,2,3,4,4,4,4,4],</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" t="s">
@@ -1495,11 +1598,14 @@
       <c r="M6">
         <v>4</v>
       </c>
+      <c r="N6">
+        <v>4</v>
+      </c>
     </row>
     <row r="7" spans="1:25">
       <c r="A7" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Zach', 'Broncos' ,1,2,3,4,4,4,5,6,6],</v>
+        <v>['Zach', 'Broncos' ,1,2,3,4,4,4,5,6,6,7],</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" t="s">
@@ -1535,11 +1641,14 @@
       <c r="M7">
         <v>6</v>
       </c>
+      <c r="N7">
+        <v>7</v>
+      </c>
     </row>
     <row r="8" spans="1:25">
       <c r="A8" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Jeff', 'Browns' ,0,0,0,0,0,0,0,0,0],</v>
+        <v>['Jeff', 'Browns' ,0,0,0,0,0,0,0,0,0,0],</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" t="s">
@@ -1575,11 +1684,14 @@
       <c r="M8">
         <v>0</v>
       </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:25">
       <c r="A9" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Zach', 'Buccaneers' ,1,1,1,1,2,2,3,3,3],</v>
+        <v>['Zach', 'Buccaneers' ,1,1,1,1,2,2,3,3,3,4],</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" t="s">
@@ -1615,11 +1727,14 @@
       <c r="M9">
         <v>3</v>
       </c>
+      <c r="N9">
+        <v>4</v>
+      </c>
     </row>
     <row r="10" spans="1:25">
       <c r="A10" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Jeff', 'Cardinals' ,0,1,1,1,2,3,3,3,3],</v>
+        <v>['Jeff', 'Cardinals' ,0,1,1,1,2,3,3,3,3,],</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" t="s">
@@ -1659,7 +1774,7 @@
     <row r="11" spans="1:25">
       <c r="A11" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Jeff', 'Chargers' ,0,1,1,1,1,2,3,3,4],</v>
+        <v>['Jeff', 'Chargers' ,0,1,1,1,1,2,3,3,4,],</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" t="s">
@@ -1699,7 +1814,7 @@
     <row r="12" spans="1:25">
       <c r="A12" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Zach', 'Chiefs' ,1,1,2,2,2,3,4,5,6],</v>
+        <v>['Zach', 'Chiefs' ,1,1,2,2,2,3,4,5,6,7],</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" t="s">
@@ -1735,11 +1850,14 @@
       <c r="M12">
         <v>6</v>
       </c>
+      <c r="N12">
+        <v>7</v>
+      </c>
     </row>
     <row r="13" spans="1:25">
       <c r="A13" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Greg', 'Colts' ,0,0,1,1,2,2,3,3,4],</v>
+        <v>['Greg', 'Colts' ,0,0,1,1,2,2,3,3,4,4],</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" t="s">
@@ -1775,11 +1893,14 @@
       <c r="M13">
         <v>4</v>
       </c>
+      <c r="N13">
+        <v>4</v>
+      </c>
     </row>
     <row r="14" spans="1:25">
       <c r="A14" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Greg', 'Cowboys' ,0,1,2,3,4,5,5,6,7],</v>
+        <v>['Greg', 'Cowboys' ,0,1,2,3,4,5,5,6,7,],</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" t="s">
@@ -1819,7 +1940,7 @@
     <row r="15" spans="1:25">
       <c r="A15" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Tim', 'Dolphins' ,0,0,1,1,1,2,3,3,4],</v>
+        <v>['Tim', 'Dolphins' ,0,0,1,1,1,2,3,3,4,],</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" t="s">
@@ -1859,7 +1980,7 @@
     <row r="16" spans="1:25">
       <c r="A16" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Zach', 'Eagles' ,1,2,3,3,3,3,4,4,4],</v>
+        <v>['Zach', 'Eagles' ,1,2,3,3,3,3,4,4,4,5],</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" t="s">
@@ -1895,11 +2016,14 @@
       <c r="M16">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="1:13">
+      <c r="N16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
       <c r="A17" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Greg', 'Falcons' ,0,1,2,3,4,4,4,5,6],</v>
+        <v>['Greg', 'Falcons' ,0,1,2,3,4,4,4,5,6,6],</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" t="s">
@@ -1935,11 +2059,14 @@
       <c r="M17">
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="1:13">
+      <c r="N17">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
       <c r="A18" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Jeff', 'Giants' ,1,2,2,2,2,3,4,4,5],</v>
+        <v>['Jeff', 'Giants' ,1,2,2,2,2,3,4,4,5,],</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" t="s">
@@ -1976,10 +2103,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:14">
       <c r="A19" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Tim', 'Jaguars' ,0,0,0,1,1,2,2,2,2],</v>
+        <v>['Tim', 'Jaguars' ,0,0,0,1,1,2,2,2,2,2],</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" t="s">
@@ -2015,11 +2142,14 @@
       <c r="M19">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:13">
+      <c r="N19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
       <c r="A20" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Tim', 'Jets' ,0,1,1,1,1,1,2,3,3],</v>
+        <v>['Tim', 'Jets' ,0,1,1,1,1,1,2,3,3,3],</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" t="s">
@@ -2055,11 +2185,14 @@
       <c r="M20">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="1:13">
+      <c r="N20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
       <c r="A21" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Jeff', 'Lions' ,1,1,1,1,2,3,4,4,5],</v>
+        <v>['Jeff', 'Lions' ,1,1,1,1,2,3,4,4,5,5],</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" t="s">
@@ -2095,11 +2228,14 @@
       <c r="M21">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="1:13">
+      <c r="N21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
       <c r="A22" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Tim', 'Packers' ,1,1,2,2,3,3,4,4,4],</v>
+        <v>['Tim', 'Packers' ,1,1,2,2,3,3,4,4,4,4],</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" t="s">
@@ -2135,11 +2271,14 @@
       <c r="M22">
         <v>4</v>
       </c>
-    </row>
-    <row r="23" spans="1:13">
+      <c r="N22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
       <c r="A23" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Greg', 'Panthers' ,0,1,1,1,1,1,1,2,3],</v>
+        <v>['Greg', 'Panthers' ,0,1,1,1,1,1,1,2,3,3],</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" t="s">
@@ -2175,11 +2314,14 @@
       <c r="M23">
         <v>3</v>
       </c>
-    </row>
-    <row r="24" spans="1:13">
+      <c r="N23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
       <c r="A24" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Greg', 'Patriots' ,1,2,3,3,4,5,6,7,7],</v>
+        <v>['Greg', 'Patriots' ,1,2,3,3,4,5,6,7,7,],</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" t="s">
@@ -2216,10 +2358,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:14">
       <c r="A25" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Tim', 'Raiders' ,1,1,2,3,4,4,5,6,7],</v>
+        <v>['Tim', 'Raiders' ,1,1,2,3,4,4,5,6,7,7],</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" t="s">
@@ -2255,11 +2397,14 @@
       <c r="M25">
         <v>7</v>
       </c>
-    </row>
-    <row r="26" spans="1:13">
+      <c r="N25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
       <c r="A26" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Zach', 'Rams' ,0,1,2,3,3,3,3,3,3],</v>
+        <v>['Zach', 'Rams' ,0,1,2,3,3,3,3,3,3,4],</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" t="s">
@@ -2295,11 +2440,14 @@
       <c r="M26">
         <v>3</v>
       </c>
-    </row>
-    <row r="27" spans="1:13">
+      <c r="N26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14">
       <c r="A27" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Jeff', 'Ravens' ,1,2,3,3,3,3,3,3,4],</v>
+        <v>['Jeff', 'Ravens' ,1,2,3,3,3,3,3,3,4,5],</v>
       </c>
       <c r="B27" s="3"/>
       <c r="C27" t="s">
@@ -2335,11 +2483,14 @@
       <c r="M27">
         <v>4</v>
       </c>
-    </row>
-    <row r="28" spans="1:13">
+      <c r="N27">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14">
       <c r="A28" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Greg', 'Redskins' ,0,0,1,2,3,4,4,4,4],</v>
+        <v>['Greg', 'Redskins' ,0,0,1,2,3,4,4,4,4,5],</v>
       </c>
       <c r="B28" s="3"/>
       <c r="C28" t="s">
@@ -2375,11 +2526,14 @@
       <c r="M28">
         <v>4</v>
       </c>
-    </row>
-    <row r="29" spans="1:13">
+      <c r="N28">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14">
       <c r="A29" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Zach', 'Saints' ,0,0,0,1,1,2,2,3,4],</v>
+        <v>['Zach', 'Saints' ,0,0,0,1,1,2,2,3,4,4],</v>
       </c>
       <c r="B29" s="3"/>
       <c r="C29" t="s">
@@ -2415,11 +2569,14 @@
       <c r="M29">
         <v>4</v>
       </c>
-    </row>
-    <row r="30" spans="1:13">
+      <c r="N29">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14">
       <c r="A30" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Zach', 'Seahawks' ,1,1,2,3,3,4,4,4,5],</v>
+        <v>['Zach', 'Seahawks' ,1,1,2,3,3,4,4,4,5,],</v>
       </c>
       <c r="B30" s="3"/>
       <c r="C30" t="s">
@@ -2456,10 +2613,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:13">
+    <row r="31" spans="1:14">
       <c r="A31" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Tim', 'Steelers' ,1,2,2,3,4,4,4,4,4],</v>
+        <v>['Tim', 'Steelers' ,1,2,2,3,4,4,4,4,4,],</v>
       </c>
       <c r="B31" s="3"/>
       <c r="C31" t="s">
@@ -2496,10 +2653,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:13">
+    <row r="32" spans="1:14">
       <c r="A32" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Jeff', 'Texans' ,1,2,2,3,3,4,4,5,5],</v>
+        <v>['Jeff', 'Texans' ,1,2,2,3,3,4,4,5,5,6],</v>
       </c>
       <c r="B32" s="3"/>
       <c r="C32" t="s">
@@ -2535,11 +2692,14 @@
       <c r="M32">
         <v>5</v>
       </c>
-    </row>
-    <row r="33" spans="1:13">
+      <c r="N32">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14">
       <c r="A33" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Zach', 'Titans' ,0,1,1,1,2,3,3,4,4],</v>
+        <v>['Zach', 'Titans' ,0,1,1,1,2,3,3,4,4,5],</v>
       </c>
       <c r="B33" s="3"/>
       <c r="C33" t="s">
@@ -2575,11 +2735,14 @@
       <c r="M33">
         <v>4</v>
       </c>
-    </row>
-    <row r="34" spans="1:13">
+      <c r="N33">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14">
       <c r="A34" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Tim', 'Vikings' ,1,2,3,4,5,5,5,5,5],</v>
+        <v>['Tim', 'Vikings' ,1,2,3,4,5,5,5,5,5,5],</v>
       </c>
       <c r="B34" s="3"/>
       <c r="C34" t="s">
@@ -2615,18 +2778,21 @@
       <c r="M34">
         <v>5</v>
       </c>
-    </row>
-    <row r="35" spans="1:13" s="4" customFormat="1" ht="4" customHeight="1">
+      <c r="N34">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" s="4" customFormat="1" ht="4" customHeight="1">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="F35" s="3"/>
     </row>
-    <row r="36" spans="1:13">
+    <row r="36" spans="1:14">
       <c r="D36" t="s">
         <v>32</v>
       </c>
       <c r="E36">
-        <f t="shared" ref="E36:M38" si="2">SUMIF($C$3:$C$34,$D36,E$3:E$34)</f>
+        <f t="shared" ref="E36:N38" si="2">SUMIF($C$3:$C$34,$D36,E$3:E$34)</f>
         <v>4</v>
       </c>
       <c r="F36" s="2">
@@ -2661,8 +2827,12 @@
         <f t="shared" si="2"/>
         <v>28</v>
       </c>
-    </row>
-    <row r="37" spans="1:13">
+      <c r="N36" s="2">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14">
       <c r="D37" t="s">
         <v>33</v>
       </c>
@@ -2702,8 +2872,12 @@
         <f t="shared" si="2"/>
         <v>36</v>
       </c>
-    </row>
-    <row r="38" spans="1:13">
+      <c r="N37" s="2">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14">
       <c r="D38" t="s">
         <v>34</v>
       </c>
@@ -2743,13 +2917,17 @@
         <f t="shared" si="2"/>
         <v>32</v>
       </c>
-    </row>
-    <row r="39" spans="1:13">
+      <c r="N38" s="2">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14">
       <c r="D39" t="s">
         <v>35</v>
       </c>
       <c r="E39">
-        <f t="shared" ref="E39:M39" si="3">SUMIF($C$3:$C$34,$D$39,E$3:E$34)</f>
+        <f t="shared" ref="E39:N39" si="3">SUMIF($C$3:$C$34,$D$39,E$3:E$34)</f>
         <v>5</v>
       </c>
       <c r="F39" s="2">
@@ -2783,6 +2961,10 @@
       <c r="M39" s="2">
         <f t="shared" si="3"/>
         <v>35</v>
+      </c>
+      <c r="N39" s="2">
+        <f t="shared" si="3"/>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -2797,4 +2979,967 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Y36"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0">
+      <pane xSplit="4" topLeftCell="E1" activePane="topRight" state="frozenSplit"/>
+      <selection pane="topRight" activeCell="A2" sqref="A2:A31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="8.33203125" customWidth="1"/>
+    <col min="2" max="2" width="0.6640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="25" width="9" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25" s="1" customFormat="1" ht="16" thickBot="1">
+      <c r="A1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="8">
+        <v>42671</v>
+      </c>
+      <c r="F1" s="8">
+        <f>E1+7</f>
+        <v>42678</v>
+      </c>
+      <c r="G1" s="8">
+        <f t="shared" ref="G1:Y1" si="0">F1+7</f>
+        <v>42685</v>
+      </c>
+      <c r="H1" s="8">
+        <f t="shared" si="0"/>
+        <v>42692</v>
+      </c>
+      <c r="I1" s="8">
+        <f t="shared" si="0"/>
+        <v>42699</v>
+      </c>
+      <c r="J1" s="8">
+        <f t="shared" si="0"/>
+        <v>42706</v>
+      </c>
+      <c r="K1" s="8">
+        <f t="shared" si="0"/>
+        <v>42713</v>
+      </c>
+      <c r="L1" s="8">
+        <f t="shared" si="0"/>
+        <v>42720</v>
+      </c>
+      <c r="M1" s="8">
+        <f t="shared" si="0"/>
+        <v>42727</v>
+      </c>
+      <c r="N1" s="8">
+        <f t="shared" si="0"/>
+        <v>42734</v>
+      </c>
+      <c r="O1" s="8">
+        <f t="shared" si="0"/>
+        <v>42741</v>
+      </c>
+      <c r="P1" s="8">
+        <f t="shared" si="0"/>
+        <v>42748</v>
+      </c>
+      <c r="Q1" s="8">
+        <f t="shared" si="0"/>
+        <v>42755</v>
+      </c>
+      <c r="R1" s="8">
+        <f>Q1+7</f>
+        <v>42762</v>
+      </c>
+      <c r="S1" s="8">
+        <f t="shared" si="0"/>
+        <v>42769</v>
+      </c>
+      <c r="T1" s="8">
+        <f t="shared" si="0"/>
+        <v>42776</v>
+      </c>
+      <c r="U1" s="8">
+        <f t="shared" si="0"/>
+        <v>42783</v>
+      </c>
+      <c r="V1" s="8">
+        <f t="shared" si="0"/>
+        <v>42790</v>
+      </c>
+      <c r="W1" s="8">
+        <f t="shared" si="0"/>
+        <v>42797</v>
+      </c>
+      <c r="X1" s="8">
+        <f t="shared" si="0"/>
+        <v>42804</v>
+      </c>
+      <c r="Y1" s="8">
+        <f t="shared" si="0"/>
+        <v>42811</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25">
+      <c r="A2" s="2" t="str">
+        <f>CONCATENATE("['",$C2,"', ","'",$D2,"' ,",$E2,",",$F2,",",$G2,"],")</f>
+        <v>['Zach', 'Atlanta' ,1,3,6],</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="2">
+        <v>3</v>
+      </c>
+      <c r="G2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25">
+      <c r="A3" s="2" t="str">
+        <f t="shared" ref="A3:A31" si="1">CONCATENATE("['",$C3,"', ","'",$D3,"' ,",$E3,",",$F3,",",$G3,"],")</f>
+        <v>['Jeff', 'Boston' ,1,3,4],</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="2">
+        <v>3</v>
+      </c>
+      <c r="G3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25">
+      <c r="A4" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>['Zach', 'Brooklyn' ,1,2,3],</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="2">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25">
+      <c r="A5" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>['Jeff', 'Charlotte' ,2,4,6],</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" t="s">
+        <v>93</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5" s="2">
+        <v>4</v>
+      </c>
+      <c r="G5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25">
+      <c r="A6" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>['Greg', 'Chicago' ,1,3,5],</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" t="s">
+        <v>96</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" s="2">
+        <v>3</v>
+      </c>
+      <c r="G6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25">
+      <c r="A7" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>['Tim', 'Cleveland' ,2,5,7],</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" t="s">
+        <v>94</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7" s="2">
+        <v>5</v>
+      </c>
+      <c r="G7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25">
+      <c r="A8" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>['Tim', 'Dallas' ,0,0,2],</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" t="s">
+        <v>119</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25">
+      <c r="A9" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>['Tim', 'Denver' ,1,2,3],</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" t="s">
+        <v>110</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" s="2">
+        <v>2</v>
+      </c>
+      <c r="G9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25">
+      <c r="A10" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>['Greg', 'Detroit' ,1,3,4],</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" t="s">
+        <v>99</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10" s="2">
+        <v>3</v>
+      </c>
+      <c r="G10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25">
+      <c r="A11" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>['Zach', 'Golden State' ,1,4,7],</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" t="s">
+        <v>113</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11" s="2">
+        <v>4</v>
+      </c>
+      <c r="G11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25">
+      <c r="A12" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>['Jeff', 'Houston' ,1,3,5],</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" t="s">
+        <v>114</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12" s="2">
+        <v>3</v>
+      </c>
+      <c r="G12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25">
+      <c r="A13" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>['Tim', 'Indiana' ,1,2,4],</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" t="s">
+        <v>100</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13" s="2">
+        <v>2</v>
+      </c>
+      <c r="G13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25">
+      <c r="A14" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>['Tim', 'L.A. Lakers' ,1,3,5],</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" t="s">
+        <v>115</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14" s="2">
+        <v>3</v>
+      </c>
+      <c r="G14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25">
+      <c r="A15" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>['Greg', 'LA Clippers' ,1,4,8],</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" t="s">
+        <v>111</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15" s="2">
+        <v>4</v>
+      </c>
+      <c r="G15">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25">
+      <c r="A16" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>['Tim', 'Memphis' ,1,3,4],</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" t="s">
+        <v>112</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16" s="2">
+        <v>3</v>
+      </c>
+      <c r="G16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>['Zach', 'Miami' ,1,2,2],</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" t="s">
+        <v>101</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17" s="2">
+        <v>2</v>
+      </c>
+      <c r="G17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>['Greg', 'Milwaukee' ,0,3,4],</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" t="s">
+        <v>104</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18" s="2">
+        <v>3</v>
+      </c>
+      <c r="G18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>['Jeff', 'Minnesota' ,0,1,2],</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" t="s">
+        <v>122</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19" s="2">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>['Zach', 'New Orleans' ,0,0,1],</v>
+      </c>
+      <c r="B20" s="3"/>
+      <c r="C20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" t="s">
+        <v>120</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20" s="2">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>['Zach', 'New York' ,0,2,3],</v>
+      </c>
+      <c r="B21" s="3"/>
+      <c r="C21" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" t="s">
+        <v>105</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21" s="2">
+        <v>2</v>
+      </c>
+      <c r="G21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>['Jeff', 'Oklahoma City' ,2,4,6],</v>
+      </c>
+      <c r="B22" s="3"/>
+      <c r="C22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" t="s">
+        <v>108</v>
+      </c>
+      <c r="E22">
+        <v>2</v>
+      </c>
+      <c r="F22" s="2">
+        <v>4</v>
+      </c>
+      <c r="G22">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>['Greg', 'Orlando' ,0,2,3],</v>
+      </c>
+      <c r="B23" s="3"/>
+      <c r="C23" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23" t="s">
+        <v>103</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23" s="2">
+        <v>2</v>
+      </c>
+      <c r="G23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>['', 'Philadelphia' ,0,0,1],</v>
+      </c>
+      <c r="B24" s="3"/>
+      <c r="D24" t="s">
+        <v>106</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24" s="2">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>['', 'Phoenix' ,0,2,3],</v>
+      </c>
+      <c r="B25" s="3"/>
+      <c r="D25" t="s">
+        <v>121</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25" s="2">
+        <v>2</v>
+      </c>
+      <c r="G25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>['Greg', 'Portland' ,1,3,6],</v>
+      </c>
+      <c r="B26" s="3"/>
+      <c r="C26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26" t="s">
+        <v>116</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26" s="2">
+        <v>3</v>
+      </c>
+      <c r="G26">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>['Jeff', 'Sacramento' ,1,2,4],</v>
+      </c>
+      <c r="B27" s="3"/>
+      <c r="C27" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27" t="s">
+        <v>117</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27" s="2">
+        <v>2</v>
+      </c>
+      <c r="G27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>['Jeff', 'San Antonio' ,2,5,6],</v>
+      </c>
+      <c r="B28" s="3"/>
+      <c r="C28" t="s">
+        <v>32</v>
+      </c>
+      <c r="D28" t="s">
+        <v>109</v>
+      </c>
+      <c r="E28">
+        <v>2</v>
+      </c>
+      <c r="F28" s="2">
+        <v>5</v>
+      </c>
+      <c r="G28">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>['Greg', 'Toronto' ,1,4,6],</v>
+      </c>
+      <c r="B29" s="3"/>
+      <c r="C29" t="s">
+        <v>33</v>
+      </c>
+      <c r="D29" t="s">
+        <v>102</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29" s="2">
+        <v>4</v>
+      </c>
+      <c r="G29">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>['Zach', 'Utah' ,1,3,6],</v>
+      </c>
+      <c r="B30" s="3"/>
+      <c r="C30" t="s">
+        <v>35</v>
+      </c>
+      <c r="D30" t="s">
+        <v>118</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30" s="2">
+        <v>3</v>
+      </c>
+      <c r="G30">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>['Tim', 'Washington' ,0,1,2],</v>
+      </c>
+      <c r="B31" s="3"/>
+      <c r="C31" t="s">
+        <v>34</v>
+      </c>
+      <c r="D31" t="s">
+        <v>107</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31" s="2">
+        <v>1</v>
+      </c>
+      <c r="G31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" s="4" customFormat="1" ht="4" customHeight="1">
+      <c r="A32" s="3"/>
+      <c r="B32" s="3"/>
+      <c r="F32" s="3"/>
+    </row>
+    <row r="33" spans="4:14">
+      <c r="D33" t="s">
+        <v>32</v>
+      </c>
+      <c r="E33">
+        <f>SUMIF($C$2:$C$31,$D33,E$2:E$31)</f>
+        <v>9</v>
+      </c>
+      <c r="F33" s="2">
+        <f>SUMIF($C$2:$C$31,$D33,F$2:F$31)</f>
+        <v>22</v>
+      </c>
+      <c r="G33" s="2">
+        <f>SUMIF($C$2:$C$31,$D33,G$2:G$31)</f>
+        <v>33</v>
+      </c>
+      <c r="H33" s="2">
+        <f>SUMIF($C$2:$C$31,$D33,H$2:H$31)</f>
+        <v>0</v>
+      </c>
+      <c r="I33" s="2">
+        <f>SUMIF($C$2:$C$31,$D33,I$2:I$31)</f>
+        <v>0</v>
+      </c>
+      <c r="J33" s="2">
+        <f>SUMIF($C$2:$C$31,$D33,J$2:J$31)</f>
+        <v>0</v>
+      </c>
+      <c r="K33" s="2">
+        <f>SUMIF($C$2:$C$31,$D33,K$2:K$31)</f>
+        <v>0</v>
+      </c>
+      <c r="L33" s="2">
+        <f>SUMIF($C$2:$C$31,$D33,L$2:L$31)</f>
+        <v>0</v>
+      </c>
+      <c r="M33" s="2">
+        <f>SUMIF($C$2:$C$31,$D33,M$2:M$31)</f>
+        <v>0</v>
+      </c>
+      <c r="N33" s="2">
+        <f>SUMIF($C$2:$C$31,$D33,N$2:N$31)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="4:14">
+      <c r="D34" t="s">
+        <v>33</v>
+      </c>
+      <c r="E34">
+        <f>SUMIF($C$2:$C$31,$D34,E$2:E$31)</f>
+        <v>5</v>
+      </c>
+      <c r="F34" s="2">
+        <f>SUMIF($C$2:$C$31,$D34,F$2:F$31)</f>
+        <v>22</v>
+      </c>
+      <c r="G34" s="2">
+        <f>SUMIF($C$2:$C$31,$D34,G$2:G$31)</f>
+        <v>36</v>
+      </c>
+      <c r="H34" s="2">
+        <f>SUMIF($C$2:$C$31,$D34,H$2:H$31)</f>
+        <v>0</v>
+      </c>
+      <c r="I34" s="2">
+        <f>SUMIF($C$2:$C$31,$D34,I$2:I$31)</f>
+        <v>0</v>
+      </c>
+      <c r="J34" s="2">
+        <f>SUMIF($C$2:$C$31,$D34,J$2:J$31)</f>
+        <v>0</v>
+      </c>
+      <c r="K34" s="2">
+        <f>SUMIF($C$2:$C$31,$D34,K$2:K$31)</f>
+        <v>0</v>
+      </c>
+      <c r="L34" s="2">
+        <f>SUMIF($C$2:$C$31,$D34,L$2:L$31)</f>
+        <v>0</v>
+      </c>
+      <c r="M34" s="2">
+        <f>SUMIF($C$2:$C$31,$D34,M$2:M$31)</f>
+        <v>0</v>
+      </c>
+      <c r="N34" s="2">
+        <f>SUMIF($C$2:$C$31,$D34,N$2:N$31)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="4:14">
+      <c r="D35" t="s">
+        <v>34</v>
+      </c>
+      <c r="E35">
+        <f>SUMIF($C$2:$C$31,$D35,E$2:E$31)</f>
+        <v>6</v>
+      </c>
+      <c r="F35" s="2">
+        <f>SUMIF($C$2:$C$31,$D35,F$2:F$31)</f>
+        <v>16</v>
+      </c>
+      <c r="G35" s="2">
+        <f>SUMIF($C$2:$C$31,$D35,G$2:G$31)</f>
+        <v>27</v>
+      </c>
+      <c r="H35" s="2">
+        <f>SUMIF($C$2:$C$31,$D35,H$2:H$31)</f>
+        <v>0</v>
+      </c>
+      <c r="I35" s="2">
+        <f>SUMIF($C$2:$C$31,$D35,I$2:I$31)</f>
+        <v>0</v>
+      </c>
+      <c r="J35" s="2">
+        <f>SUMIF($C$2:$C$31,$D35,J$2:J$31)</f>
+        <v>0</v>
+      </c>
+      <c r="K35" s="2">
+        <f>SUMIF($C$2:$C$31,$D35,K$2:K$31)</f>
+        <v>0</v>
+      </c>
+      <c r="L35" s="2">
+        <f>SUMIF($C$2:$C$31,$D35,L$2:L$31)</f>
+        <v>0</v>
+      </c>
+      <c r="M35" s="2">
+        <f>SUMIF($C$2:$C$31,$D35,M$2:M$31)</f>
+        <v>0</v>
+      </c>
+      <c r="N35" s="2">
+        <f>SUMIF($C$2:$C$31,$D35,N$2:N$31)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="4:14">
+      <c r="D36" t="s">
+        <v>35</v>
+      </c>
+      <c r="E36">
+        <f>SUMIF($C$2:$C$31,$D$36,E$2:E$31)</f>
+        <v>5</v>
+      </c>
+      <c r="F36" s="2">
+        <f>SUMIF($C$2:$C$31,$D$36,F$2:F$31)</f>
+        <v>16</v>
+      </c>
+      <c r="G36" s="2">
+        <f>SUMIF($C$2:$C$31,$D$36,G$2:G$31)</f>
+        <v>28</v>
+      </c>
+      <c r="H36" s="2">
+        <f>SUMIF($C$2:$C$31,$D$36,H$2:H$31)</f>
+        <v>0</v>
+      </c>
+      <c r="I36" s="2">
+        <f>SUMIF($C$2:$C$31,$D$36,I$2:I$31)</f>
+        <v>0</v>
+      </c>
+      <c r="J36" s="2">
+        <f>SUMIF($C$2:$C$31,$D$36,J$2:J$31)</f>
+        <v>0</v>
+      </c>
+      <c r="K36" s="2">
+        <f>SUMIF($C$2:$C$31,$D$36,K$2:K$31)</f>
+        <v>0</v>
+      </c>
+      <c r="L36" s="2">
+        <f>SUMIF($C$2:$C$31,$D$36,L$2:L$31)</f>
+        <v>0</v>
+      </c>
+      <c r="M36" s="2">
+        <f>SUMIF($C$2:$C$31,$D$36,M$2:M$31)</f>
+        <v>0</v>
+      </c>
+      <c r="N36" s="2">
+        <f>SUMIF($C$2:$C$31,$D$36,N$2:N$31)</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated week 10 wins.
</commit_message>
<xml_diff>
--- a/NFL Wins.xlsx
+++ b/NFL Wins.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20720" windowHeight="16100" tabRatio="500" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8980" windowHeight="16100" tabRatio="500" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
@@ -479,7 +479,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="99">
+  <cellStyleXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -578,6 +578,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
@@ -595,7 +599,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="99">
+  <cellStyles count="103">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -647,6 +651,8 @@
     <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="97" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -694,6 +700,8 @@
     <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1313,8 +1321,8 @@
   <dimension ref="A1:Y39"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" topLeftCell="A2" workbookViewId="0">
-      <pane xSplit="4" topLeftCell="L1" activePane="topRight" state="frozenSplit"/>
-      <selection pane="topRight" activeCell="N36" sqref="N36"/>
+      <pane xSplit="4" topLeftCell="K1" activePane="topRight" state="frozenSplit"/>
+      <selection pane="topRight" activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1439,7 +1447,7 @@
     <row r="3" spans="1:25">
       <c r="A3" s="2" t="str">
         <f>CONCATENATE("['",$C3,"', ","'",$D3,"' ,",$E3,",",$F3,",",$G3,",",$H3,",",$I3,",",$J3,",",$K3,",",$L3,",",$M3,",",$N3,"],")</f>
-        <v>['Greg', '49ers' ,1,1,1,1,1,1,1,1,1,],</v>
+        <v>['Greg', '49ers' ,1,1,1,1,1,1,1,1,1,1],</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" t="s">
@@ -1473,6 +1481,9 @@
         <v>1</v>
       </c>
       <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
         <v>1</v>
       </c>
     </row>
@@ -1522,7 +1533,7 @@
     <row r="5" spans="1:25">
       <c r="A5" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Tim', 'Bengals' ,1,1,1,2,2,2,3,3,3,],</v>
+        <v>['Tim', 'Bengals' ,1,1,1,2,2,2,3,3,3,3],</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" t="s">
@@ -1558,6 +1569,9 @@
       <c r="M5">
         <v>3</v>
       </c>
+      <c r="N5">
+        <v>3</v>
+      </c>
     </row>
     <row r="6" spans="1:25">
       <c r="A6" s="2" t="str">
@@ -1734,7 +1748,7 @@
     <row r="10" spans="1:25">
       <c r="A10" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Jeff', 'Cardinals' ,0,1,1,1,2,3,3,3,3,],</v>
+        <v>['Jeff', 'Cardinals' ,0,1,1,1,2,3,3,3,3,4],</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" t="s">
@@ -1770,11 +1784,14 @@
       <c r="M10">
         <v>3</v>
       </c>
+      <c r="N10">
+        <v>4</v>
+      </c>
     </row>
     <row r="11" spans="1:25">
       <c r="A11" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Jeff', 'Chargers' ,0,1,1,1,1,2,3,3,4,],</v>
+        <v>['Jeff', 'Chargers' ,0,1,1,1,1,2,3,3,4,4],</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" t="s">
@@ -1810,6 +1827,9 @@
       <c r="M11">
         <v>4</v>
       </c>
+      <c r="N11">
+        <v>4</v>
+      </c>
     </row>
     <row r="12" spans="1:25">
       <c r="A12" s="2" t="str">
@@ -1900,7 +1920,7 @@
     <row r="14" spans="1:25">
       <c r="A14" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Greg', 'Cowboys' ,0,1,2,3,4,5,5,6,7,],</v>
+        <v>['Greg', 'Cowboys' ,0,1,2,3,4,5,5,6,7,8],</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" t="s">
@@ -1936,11 +1956,14 @@
       <c r="M14">
         <v>7</v>
       </c>
+      <c r="N14">
+        <v>8</v>
+      </c>
     </row>
     <row r="15" spans="1:25">
       <c r="A15" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Tim', 'Dolphins' ,0,0,1,1,1,2,3,3,4,],</v>
+        <v>['Tim', 'Dolphins' ,0,0,1,1,1,2,3,3,4,5],</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" t="s">
@@ -1976,6 +1999,9 @@
       <c r="M15">
         <v>4</v>
       </c>
+      <c r="N15">
+        <v>5</v>
+      </c>
     </row>
     <row r="16" spans="1:25">
       <c r="A16" s="2" t="str">
@@ -2066,7 +2092,7 @@
     <row r="18" spans="1:14">
       <c r="A18" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Jeff', 'Giants' ,1,2,2,2,2,3,4,4,5,],</v>
+        <v>['Jeff', 'Giants' ,1,2,2,2,2,3,4,4,5,6],</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" t="s">
@@ -2102,6 +2128,9 @@
       <c r="M18">
         <v>5</v>
       </c>
+      <c r="N18">
+        <v>6</v>
+      </c>
     </row>
     <row r="19" spans="1:14">
       <c r="A19" s="2" t="str">
@@ -2321,7 +2350,7 @@
     <row r="24" spans="1:14">
       <c r="A24" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Greg', 'Patriots' ,1,2,3,3,4,5,6,7,7,],</v>
+        <v>['Greg', 'Patriots' ,1,2,3,3,4,5,6,7,7,7],</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" t="s">
@@ -2357,6 +2386,9 @@
       <c r="M24">
         <v>7</v>
       </c>
+      <c r="N24">
+        <v>7</v>
+      </c>
     </row>
     <row r="25" spans="1:14">
       <c r="A25" s="2" t="str">
@@ -2576,7 +2608,7 @@
     <row r="30" spans="1:14">
       <c r="A30" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Zach', 'Seahawks' ,1,1,2,3,3,4,4,4,5,],</v>
+        <v>['Zach', 'Seahawks' ,1,1,2,3,3,4,4,4,5,6],</v>
       </c>
       <c r="B30" s="3"/>
       <c r="C30" t="s">
@@ -2612,11 +2644,14 @@
       <c r="M30">
         <v>5</v>
       </c>
+      <c r="N30">
+        <v>6</v>
+      </c>
     </row>
     <row r="31" spans="1:14">
       <c r="A31" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Tim', 'Steelers' ,1,2,2,3,4,4,4,4,4,],</v>
+        <v>['Tim', 'Steelers' ,1,2,2,3,4,4,4,4,4,4],</v>
       </c>
       <c r="B31" s="3"/>
       <c r="C31" t="s">
@@ -2650,6 +2685,9 @@
         <v>4</v>
       </c>
       <c r="M31">
+        <v>4</v>
+      </c>
+      <c r="N31">
         <v>4</v>
       </c>
     </row>
@@ -2829,7 +2867,7 @@
       </c>
       <c r="N36" s="2">
         <f t="shared" si="2"/>
-        <v>18</v>
+        <v>32</v>
       </c>
     </row>
     <row r="37" spans="1:14">
@@ -2874,7 +2912,7 @@
       </c>
       <c r="N37" s="2">
         <f t="shared" si="2"/>
-        <v>22</v>
+        <v>38</v>
       </c>
     </row>
     <row r="38" spans="1:14">
@@ -2919,7 +2957,7 @@
       </c>
       <c r="N38" s="2">
         <f t="shared" si="2"/>
-        <v>21</v>
+        <v>33</v>
       </c>
     </row>
     <row r="39" spans="1:14">
@@ -2964,7 +3002,7 @@
       </c>
       <c r="N39" s="2">
         <f t="shared" si="3"/>
-        <v>36</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -2987,7 +3025,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
       <pane xSplit="4" topLeftCell="E1" activePane="topRight" state="frozenSplit"/>
-      <selection pane="topRight" activeCell="A2" sqref="A2:A31"/>
+      <selection pane="topRight" activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3758,43 +3796,43 @@
         <v>32</v>
       </c>
       <c r="E33">
-        <f>SUMIF($C$2:$C$31,$D33,E$2:E$31)</f>
+        <f t="shared" ref="E33:N35" si="2">SUMIF($C$2:$C$31,$D33,E$2:E$31)</f>
         <v>9</v>
       </c>
       <c r="F33" s="2">
-        <f>SUMIF($C$2:$C$31,$D33,F$2:F$31)</f>
+        <f t="shared" si="2"/>
         <v>22</v>
       </c>
       <c r="G33" s="2">
-        <f>SUMIF($C$2:$C$31,$D33,G$2:G$31)</f>
+        <f t="shared" si="2"/>
         <v>33</v>
       </c>
       <c r="H33" s="2">
-        <f>SUMIF($C$2:$C$31,$D33,H$2:H$31)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I33" s="2">
-        <f>SUMIF($C$2:$C$31,$D33,I$2:I$31)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J33" s="2">
-        <f>SUMIF($C$2:$C$31,$D33,J$2:J$31)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K33" s="2">
-        <f>SUMIF($C$2:$C$31,$D33,K$2:K$31)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L33" s="2">
-        <f>SUMIF($C$2:$C$31,$D33,L$2:L$31)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M33" s="2">
-        <f>SUMIF($C$2:$C$31,$D33,M$2:M$31)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N33" s="2">
-        <f>SUMIF($C$2:$C$31,$D33,N$2:N$31)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3803,43 +3841,43 @@
         <v>33</v>
       </c>
       <c r="E34">
-        <f>SUMIF($C$2:$C$31,$D34,E$2:E$31)</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="F34" s="2">
-        <f>SUMIF($C$2:$C$31,$D34,F$2:F$31)</f>
+        <f t="shared" si="2"/>
         <v>22</v>
       </c>
       <c r="G34" s="2">
-        <f>SUMIF($C$2:$C$31,$D34,G$2:G$31)</f>
+        <f t="shared" si="2"/>
         <v>36</v>
       </c>
       <c r="H34" s="2">
-        <f>SUMIF($C$2:$C$31,$D34,H$2:H$31)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I34" s="2">
-        <f>SUMIF($C$2:$C$31,$D34,I$2:I$31)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J34" s="2">
-        <f>SUMIF($C$2:$C$31,$D34,J$2:J$31)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K34" s="2">
-        <f>SUMIF($C$2:$C$31,$D34,K$2:K$31)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L34" s="2">
-        <f>SUMIF($C$2:$C$31,$D34,L$2:L$31)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M34" s="2">
-        <f>SUMIF($C$2:$C$31,$D34,M$2:M$31)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N34" s="2">
-        <f>SUMIF($C$2:$C$31,$D34,N$2:N$31)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3848,43 +3886,43 @@
         <v>34</v>
       </c>
       <c r="E35">
-        <f>SUMIF($C$2:$C$31,$D35,E$2:E$31)</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="F35" s="2">
-        <f>SUMIF($C$2:$C$31,$D35,F$2:F$31)</f>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="G35" s="2">
-        <f>SUMIF($C$2:$C$31,$D35,G$2:G$31)</f>
+        <f t="shared" si="2"/>
         <v>27</v>
       </c>
       <c r="H35" s="2">
-        <f>SUMIF($C$2:$C$31,$D35,H$2:H$31)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I35" s="2">
-        <f>SUMIF($C$2:$C$31,$D35,I$2:I$31)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J35" s="2">
-        <f>SUMIF($C$2:$C$31,$D35,J$2:J$31)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K35" s="2">
-        <f>SUMIF($C$2:$C$31,$D35,K$2:K$31)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L35" s="2">
-        <f>SUMIF($C$2:$C$31,$D35,L$2:L$31)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M35" s="2">
-        <f>SUMIF($C$2:$C$31,$D35,M$2:M$31)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N35" s="2">
-        <f>SUMIF($C$2:$C$31,$D35,N$2:N$31)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3893,43 +3931,43 @@
         <v>35</v>
       </c>
       <c r="E36">
-        <f>SUMIF($C$2:$C$31,$D$36,E$2:E$31)</f>
+        <f t="shared" ref="E36:N36" si="3">SUMIF($C$2:$C$31,$D$36,E$2:E$31)</f>
         <v>5</v>
       </c>
       <c r="F36" s="2">
-        <f>SUMIF($C$2:$C$31,$D$36,F$2:F$31)</f>
+        <f t="shared" si="3"/>
         <v>16</v>
       </c>
       <c r="G36" s="2">
-        <f>SUMIF($C$2:$C$31,$D$36,G$2:G$31)</f>
+        <f t="shared" si="3"/>
         <v>28</v>
       </c>
       <c r="H36" s="2">
-        <f>SUMIF($C$2:$C$31,$D$36,H$2:H$31)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I36" s="2">
-        <f>SUMIF($C$2:$C$31,$D$36,I$2:I$31)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J36" s="2">
-        <f>SUMIF($C$2:$C$31,$D$36,J$2:J$31)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K36" s="2">
-        <f>SUMIF($C$2:$C$31,$D$36,K$2:K$31)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L36" s="2">
-        <f>SUMIF($C$2:$C$31,$D$36,L$2:L$31)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M36" s="2">
-        <f>SUMIF($C$2:$C$31,$D$36,M$2:M$31)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N36" s="2">
-        <f>SUMIF($C$2:$C$31,$D$36,N$2:N$31)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update NBA league weekly wins.
</commit_message>
<xml_diff>
--- a/NFL Wins.xlsx
+++ b/NFL Wins.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8980" windowHeight="16100" tabRatio="500" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8980" windowHeight="16100" tabRatio="500" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
@@ -479,7 +479,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="103">
+  <cellStyleXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -578,6 +578,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -599,7 +601,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="103">
+  <cellStyles count="105">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -653,6 +655,7 @@
     <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -702,6 +705,7 @@
     <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1320,9 +1324,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y39"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A2" workbookViewId="0">
-      <pane xSplit="4" topLeftCell="K1" activePane="topRight" state="frozenSplit"/>
-      <selection pane="topRight" activeCell="N24" sqref="N24"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <pane xSplit="4" topLeftCell="L1" activePane="topRight" state="frozenSplit"/>
+      <selection pane="topRight" activeCell="A3" sqref="A3:A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1446,8 +1450,8 @@
     </row>
     <row r="3" spans="1:25">
       <c r="A3" s="2" t="str">
-        <f>CONCATENATE("['",$C3,"', ","'",$D3,"' ,",$E3,",",$F3,",",$G3,",",$H3,",",$I3,",",$J3,",",$K3,",",$L3,",",$M3,",",$N3,"],")</f>
-        <v>['Greg', '49ers' ,1,1,1,1,1,1,1,1,1,1],</v>
+        <f>CONCATENATE("['",$C3,"', ","'",$D3,"' ,",$E3,",",$F3,",",$G3,",",$H3,",",$I3,",",$J3,",",$K3,",",$L3,",",$M3,",",$N3,",",$O3,"],")</f>
+        <v>['Greg', '49ers' ,1,1,1,1,1,1,1,1,1,1,],</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" t="s">
@@ -1489,8 +1493,8 @@
     </row>
     <row r="4" spans="1:25">
       <c r="A4" s="2" t="str">
-        <f t="shared" ref="A4:A34" si="1">CONCATENATE("['",$C4,"', ","'",$D4,"' ,",$E4,",",$F4,",",$G4,",",$H4,",",$I4,",",$J4,",",$K4,",",$L4,",",$M4,",",$N4,"],")</f>
-        <v>['Jeff', 'Bears' ,0,0,0,1,1,1,1,2,2,2],</v>
+        <f t="shared" ref="A4:A34" si="1">CONCATENATE("['",$C4,"', ","'",$D4,"' ,",$E4,",",$F4,",",$G4,",",$H4,",",$I4,",",$J4,",",$K4,",",$L4,",",$M4,",",$N4,",",$O4,"],")</f>
+        <v>['Jeff', 'Bears' ,0,0,0,1,1,1,1,2,2,2,],</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" t="s">
@@ -1533,7 +1537,7 @@
     <row r="5" spans="1:25">
       <c r="A5" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Tim', 'Bengals' ,1,1,1,2,2,2,3,3,3,3],</v>
+        <v>['Tim', 'Bengals' ,1,1,1,2,2,2,3,3,3,3,],</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" t="s">
@@ -1576,7 +1580,7 @@
     <row r="6" spans="1:25">
       <c r="A6" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Greg', 'Bills' ,0,0,1,2,3,4,4,4,4,4],</v>
+        <v>['Greg', 'Bills' ,0,0,1,2,3,4,4,4,4,4,],</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" t="s">
@@ -1619,7 +1623,7 @@
     <row r="7" spans="1:25">
       <c r="A7" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Zach', 'Broncos' ,1,2,3,4,4,4,5,6,6,7],</v>
+        <v>['Zach', 'Broncos' ,1,2,3,4,4,4,5,6,6,7,],</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" t="s">
@@ -1662,7 +1666,7 @@
     <row r="8" spans="1:25">
       <c r="A8" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Jeff', 'Browns' ,0,0,0,0,0,0,0,0,0,0],</v>
+        <v>['Jeff', 'Browns' ,0,0,0,0,0,0,0,0,0,0,],</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" t="s">
@@ -1705,7 +1709,7 @@
     <row r="9" spans="1:25">
       <c r="A9" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Zach', 'Buccaneers' ,1,1,1,1,2,2,3,3,3,4],</v>
+        <v>['Zach', 'Buccaneers' ,1,1,1,1,2,2,3,3,3,4,],</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" t="s">
@@ -1748,7 +1752,7 @@
     <row r="10" spans="1:25">
       <c r="A10" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Jeff', 'Cardinals' ,0,1,1,1,2,3,3,3,3,4],</v>
+        <v>['Jeff', 'Cardinals' ,0,1,1,1,2,3,3,3,3,4,],</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" t="s">
@@ -1791,7 +1795,7 @@
     <row r="11" spans="1:25">
       <c r="A11" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Jeff', 'Chargers' ,0,1,1,1,1,2,3,3,4,4],</v>
+        <v>['Jeff', 'Chargers' ,0,1,1,1,1,2,3,3,4,4,],</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" t="s">
@@ -1834,7 +1838,7 @@
     <row r="12" spans="1:25">
       <c r="A12" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Zach', 'Chiefs' ,1,1,2,2,2,3,4,5,6,7],</v>
+        <v>['Zach', 'Chiefs' ,1,1,2,2,2,3,4,5,6,7,],</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" t="s">
@@ -1877,7 +1881,7 @@
     <row r="13" spans="1:25">
       <c r="A13" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Greg', 'Colts' ,0,0,1,1,2,2,3,3,4,4],</v>
+        <v>['Greg', 'Colts' ,0,0,1,1,2,2,3,3,4,4,],</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" t="s">
@@ -1920,7 +1924,7 @@
     <row r="14" spans="1:25">
       <c r="A14" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Greg', 'Cowboys' ,0,1,2,3,4,5,5,6,7,8],</v>
+        <v>['Greg', 'Cowboys' ,0,1,2,3,4,5,5,6,7,8,],</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" t="s">
@@ -1963,7 +1967,7 @@
     <row r="15" spans="1:25">
       <c r="A15" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Tim', 'Dolphins' ,0,0,1,1,1,2,3,3,4,5],</v>
+        <v>['Tim', 'Dolphins' ,0,0,1,1,1,2,3,3,4,5,],</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" t="s">
@@ -2006,7 +2010,7 @@
     <row r="16" spans="1:25">
       <c r="A16" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Zach', 'Eagles' ,1,2,3,3,3,3,4,4,4,5],</v>
+        <v>['Zach', 'Eagles' ,1,2,3,3,3,3,4,4,4,5,],</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" t="s">
@@ -2046,10 +2050,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:15">
       <c r="A17" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Greg', 'Falcons' ,0,1,2,3,4,4,4,5,6,6],</v>
+        <v>['Greg', 'Falcons' ,0,1,2,3,4,4,4,5,6,6,],</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" t="s">
@@ -2089,10 +2093,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:14">
+    <row r="18" spans="1:15">
       <c r="A18" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Jeff', 'Giants' ,1,2,2,2,2,3,4,4,5,6],</v>
+        <v>['Jeff', 'Giants' ,1,2,2,2,2,3,4,4,5,6,],</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" t="s">
@@ -2132,10 +2136,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:14">
+    <row r="19" spans="1:15">
       <c r="A19" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Tim', 'Jaguars' ,0,0,0,1,1,2,2,2,2,2],</v>
+        <v>['Tim', 'Jaguars' ,0,0,0,1,1,2,2,2,2,2,],</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" t="s">
@@ -2175,10 +2179,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:14">
+    <row r="20" spans="1:15">
       <c r="A20" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Tim', 'Jets' ,0,1,1,1,1,1,2,3,3,3],</v>
+        <v>['Tim', 'Jets' ,0,1,1,1,1,1,2,3,3,3,],</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" t="s">
@@ -2218,10 +2222,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:14">
+    <row r="21" spans="1:15">
       <c r="A21" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Jeff', 'Lions' ,1,1,1,1,2,3,4,4,5,5],</v>
+        <v>['Jeff', 'Lions' ,1,1,1,1,2,3,4,4,5,5,],</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" t="s">
@@ -2261,10 +2265,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:14">
+    <row r="22" spans="1:15">
       <c r="A22" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Tim', 'Packers' ,1,1,2,2,3,3,4,4,4,4],</v>
+        <v>['Tim', 'Packers' ,1,1,2,2,3,3,4,4,4,4,],</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" t="s">
@@ -2304,10 +2308,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:14">
+    <row r="23" spans="1:15">
       <c r="A23" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Greg', 'Panthers' ,0,1,1,1,1,1,1,2,3,3],</v>
+        <v>['Greg', 'Panthers' ,0,1,1,1,1,1,1,2,3,3,4],</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" t="s">
@@ -2346,11 +2350,14 @@
       <c r="N23">
         <v>3</v>
       </c>
-    </row>
-    <row r="24" spans="1:14">
+      <c r="O23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15">
       <c r="A24" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Greg', 'Patriots' ,1,2,3,3,4,5,6,7,7,7],</v>
+        <v>['Greg', 'Patriots' ,1,2,3,3,4,5,6,7,7,7,],</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" t="s">
@@ -2390,10 +2397,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:14">
+    <row r="25" spans="1:15">
       <c r="A25" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Tim', 'Raiders' ,1,1,2,3,4,4,5,6,7,7],</v>
+        <v>['Tim', 'Raiders' ,1,1,2,3,4,4,5,6,7,7,],</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" t="s">
@@ -2433,10 +2440,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:14">
+    <row r="26" spans="1:15">
       <c r="A26" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Zach', 'Rams' ,0,1,2,3,3,3,3,3,3,4],</v>
+        <v>['Zach', 'Rams' ,0,1,2,3,3,3,3,3,3,4,],</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" t="s">
@@ -2476,10 +2483,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:14">
+    <row r="27" spans="1:15">
       <c r="A27" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Jeff', 'Ravens' ,1,2,3,3,3,3,3,3,4,5],</v>
+        <v>['Jeff', 'Ravens' ,1,2,3,3,3,3,3,3,4,5,],</v>
       </c>
       <c r="B27" s="3"/>
       <c r="C27" t="s">
@@ -2519,10 +2526,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:14">
+    <row r="28" spans="1:15">
       <c r="A28" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Greg', 'Redskins' ,0,0,1,2,3,4,4,4,4,5],</v>
+        <v>['Greg', 'Redskins' ,0,0,1,2,3,4,4,4,4,5,],</v>
       </c>
       <c r="B28" s="3"/>
       <c r="C28" t="s">
@@ -2562,10 +2569,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:14">
+    <row r="29" spans="1:15">
       <c r="A29" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Zach', 'Saints' ,0,0,0,1,1,2,2,3,4,4],</v>
+        <v>['Zach', 'Saints' ,0,0,0,1,1,2,2,3,4,4,4],</v>
       </c>
       <c r="B29" s="3"/>
       <c r="C29" t="s">
@@ -2604,11 +2611,14 @@
       <c r="N29">
         <v>4</v>
       </c>
-    </row>
-    <row r="30" spans="1:14">
+      <c r="O29">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15">
       <c r="A30" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Zach', 'Seahawks' ,1,1,2,3,3,4,4,4,5,6],</v>
+        <v>['Zach', 'Seahawks' ,1,1,2,3,3,4,4,4,5,6,],</v>
       </c>
       <c r="B30" s="3"/>
       <c r="C30" t="s">
@@ -2648,10 +2658,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:14">
+    <row r="31" spans="1:15">
       <c r="A31" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Tim', 'Steelers' ,1,2,2,3,4,4,4,4,4,4],</v>
+        <v>['Tim', 'Steelers' ,1,2,2,3,4,4,4,4,4,4,],</v>
       </c>
       <c r="B31" s="3"/>
       <c r="C31" t="s">
@@ -2691,10 +2701,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:14">
+    <row r="32" spans="1:15">
       <c r="A32" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Jeff', 'Texans' ,1,2,2,3,3,4,4,5,5,6],</v>
+        <v>['Jeff', 'Texans' ,1,2,2,3,3,4,4,5,5,6,],</v>
       </c>
       <c r="B32" s="3"/>
       <c r="C32" t="s">
@@ -2734,10 +2744,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:14">
+    <row r="33" spans="1:15">
       <c r="A33" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Zach', 'Titans' ,0,1,1,1,2,3,3,4,4,5],</v>
+        <v>['Zach', 'Titans' ,0,1,1,1,2,3,3,4,4,5,],</v>
       </c>
       <c r="B33" s="3"/>
       <c r="C33" t="s">
@@ -2777,10 +2787,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:14">
+    <row r="34" spans="1:15">
       <c r="A34" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Tim', 'Vikings' ,1,2,3,4,5,5,5,5,5,5],</v>
+        <v>['Tim', 'Vikings' ,1,2,3,4,5,5,5,5,5,5,],</v>
       </c>
       <c r="B34" s="3"/>
       <c r="C34" t="s">
@@ -2820,17 +2830,17 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:14" s="4" customFormat="1" ht="4" customHeight="1">
+    <row r="35" spans="1:15" s="4" customFormat="1" ht="4" customHeight="1">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="F35" s="3"/>
     </row>
-    <row r="36" spans="1:14">
+    <row r="36" spans="1:15">
       <c r="D36" t="s">
         <v>32</v>
       </c>
       <c r="E36">
-        <f t="shared" ref="E36:N38" si="2">SUMIF($C$3:$C$34,$D36,E$3:E$34)</f>
+        <f t="shared" ref="E36:O38" si="2">SUMIF($C$3:$C$34,$D36,E$3:E$34)</f>
         <v>4</v>
       </c>
       <c r="F36" s="2">
@@ -2869,8 +2879,12 @@
         <f t="shared" si="2"/>
         <v>32</v>
       </c>
-    </row>
-    <row r="37" spans="1:14">
+      <c r="O36" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15">
       <c r="D37" t="s">
         <v>33</v>
       </c>
@@ -2914,8 +2928,12 @@
         <f t="shared" si="2"/>
         <v>38</v>
       </c>
-    </row>
-    <row r="38" spans="1:14">
+      <c r="O37" s="2">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15">
       <c r="D38" t="s">
         <v>34</v>
       </c>
@@ -2959,13 +2977,17 @@
         <f t="shared" si="2"/>
         <v>33</v>
       </c>
-    </row>
-    <row r="39" spans="1:14">
+      <c r="O38" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15">
       <c r="D39" t="s">
         <v>35</v>
       </c>
       <c r="E39">
-        <f t="shared" ref="E39:N39" si="3">SUMIF($C$3:$C$34,$D$39,E$3:E$34)</f>
+        <f t="shared" ref="E39:O39" si="3">SUMIF($C$3:$C$34,$D$39,E$3:E$34)</f>
         <v>5</v>
       </c>
       <c r="F39" s="2">
@@ -3003,6 +3025,10 @@
       <c r="N39" s="2">
         <f t="shared" si="3"/>
         <v>42</v>
+      </c>
+      <c r="O39" s="2">
+        <f t="shared" si="3"/>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -3023,9 +3049,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y36"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <pane xSplit="4" topLeftCell="E1" activePane="topRight" state="frozenSplit"/>
-      <selection pane="topRight" activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <pane xSplit="4" topLeftCell="F1" activePane="topRight" state="frozenSplit"/>
+      <selection pane="topRight" activeCell="A2" sqref="A2:A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3134,8 +3160,8 @@
     </row>
     <row r="2" spans="1:25">
       <c r="A2" s="2" t="str">
-        <f>CONCATENATE("['",$C2,"', ","'",$D2,"' ,",$E2,",",$F2,",",$G2,"],")</f>
-        <v>['Zach', 'Atlanta' ,1,3,6],</v>
+        <f>CONCATENATE("['",$C2,"', ","'",$D2,"' ,",$E2,",",$F2,",",$G2,",",$H2,"],")</f>
+        <v>['Zach', 'Atlanta' ,1,3,6,9],</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" t="s">
@@ -3153,11 +3179,14 @@
       <c r="G2">
         <v>6</v>
       </c>
+      <c r="H2">
+        <v>9</v>
+      </c>
     </row>
     <row r="3" spans="1:25">
       <c r="A3" s="2" t="str">
-        <f t="shared" ref="A3:A31" si="1">CONCATENATE("['",$C3,"', ","'",$D3,"' ,",$E3,",",$F3,",",$G3,"],")</f>
-        <v>['Jeff', 'Boston' ,1,3,4],</v>
+        <f t="shared" ref="A3:A31" si="1">CONCATENATE("['",$C3,"', ","'",$D3,"' ,",$E3,",",$F3,",",$G3,",",$H3,"],")</f>
+        <v>['Jeff', 'Boston' ,1,3,4,6],</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" t="s">
@@ -3175,11 +3204,14 @@
       <c r="G3">
         <v>4</v>
       </c>
+      <c r="H3">
+        <v>6</v>
+      </c>
     </row>
     <row r="4" spans="1:25">
       <c r="A4" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Zach', 'Brooklyn' ,1,2,3],</v>
+        <v>['Zach', 'Brooklyn' ,1,2,3,4],</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" t="s">
@@ -3197,11 +3229,14 @@
       <c r="G4">
         <v>3</v>
       </c>
+      <c r="H4">
+        <v>4</v>
+      </c>
     </row>
     <row r="5" spans="1:25">
       <c r="A5" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Jeff', 'Charlotte' ,2,4,6],</v>
+        <v>['Jeff', 'Charlotte' ,2,4,6,8],</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" t="s">
@@ -3219,11 +3254,14 @@
       <c r="G5">
         <v>6</v>
       </c>
+      <c r="H5">
+        <v>8</v>
+      </c>
     </row>
     <row r="6" spans="1:25">
       <c r="A6" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Greg', 'Chicago' ,1,3,5],</v>
+        <v>['Greg', 'Chicago' ,1,3,5,8],</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" t="s">
@@ -3241,11 +3279,14 @@
       <c r="G6">
         <v>5</v>
       </c>
+      <c r="H6">
+        <v>8</v>
+      </c>
     </row>
     <row r="7" spans="1:25">
       <c r="A7" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Tim', 'Cleveland' ,2,5,7],</v>
+        <v>['Tim', 'Cleveland' ,2,5,7,10],</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" t="s">
@@ -3263,11 +3304,14 @@
       <c r="G7">
         <v>7</v>
       </c>
+      <c r="H7">
+        <v>10</v>
+      </c>
     </row>
     <row r="8" spans="1:25">
       <c r="A8" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Tim', 'Dallas' ,0,0,2],</v>
+        <v>['Tim', 'Dallas' ,0,0,2,2],</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" t="s">
@@ -3285,11 +3329,14 @@
       <c r="G8">
         <v>2</v>
       </c>
+      <c r="H8">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" spans="1:25">
       <c r="A9" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Tim', 'Denver' ,1,2,3],</v>
+        <v>['Tim', 'Denver' ,1,2,3,4],</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" t="s">
@@ -3307,11 +3354,14 @@
       <c r="G9">
         <v>3</v>
       </c>
+      <c r="H9">
+        <v>4</v>
+      </c>
     </row>
     <row r="10" spans="1:25">
       <c r="A10" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Greg', 'Detroit' ,1,3,4],</v>
+        <v>['Greg', 'Detroit' ,1,3,4,6],</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" t="s">
@@ -3329,11 +3379,14 @@
       <c r="G10">
         <v>4</v>
       </c>
+      <c r="H10">
+        <v>6</v>
+      </c>
     </row>
     <row r="11" spans="1:25">
       <c r="A11" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Zach', 'Golden State' ,1,4,7],</v>
+        <v>['Zach', 'Golden State' ,1,4,7,9],</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" t="s">
@@ -3351,11 +3404,14 @@
       <c r="G11">
         <v>7</v>
       </c>
+      <c r="H11">
+        <v>9</v>
+      </c>
     </row>
     <row r="12" spans="1:25">
       <c r="A12" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Jeff', 'Houston' ,1,3,5],</v>
+        <v>['Jeff', 'Houston' ,1,3,5,7],</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" t="s">
@@ -3373,11 +3429,14 @@
       <c r="G12">
         <v>5</v>
       </c>
+      <c r="H12">
+        <v>7</v>
+      </c>
     </row>
     <row r="13" spans="1:25">
       <c r="A13" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Tim', 'Indiana' ,1,2,4],</v>
+        <v>['Tim', 'Indiana' ,1,2,4,6],</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" t="s">
@@ -3395,11 +3454,14 @@
       <c r="G13">
         <v>4</v>
       </c>
+      <c r="H13">
+        <v>6</v>
+      </c>
     </row>
     <row r="14" spans="1:25">
       <c r="A14" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Tim', 'L.A. Lakers' ,1,3,5],</v>
+        <v>['Tim', 'L.A. Lakers' ,1,3,5,7],</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" t="s">
@@ -3417,11 +3479,14 @@
       <c r="G14">
         <v>5</v>
       </c>
+      <c r="H14">
+        <v>7</v>
+      </c>
     </row>
     <row r="15" spans="1:25">
       <c r="A15" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Greg', 'LA Clippers' ,1,4,8],</v>
+        <v>['Greg', 'LA Clippers' ,1,4,8,11],</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" t="s">
@@ -3439,11 +3504,14 @@
       <c r="G15">
         <v>8</v>
       </c>
+      <c r="H15">
+        <v>11</v>
+      </c>
     </row>
     <row r="16" spans="1:25">
       <c r="A16" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Tim', 'Memphis' ,1,3,4],</v>
+        <v>['Tim', 'Memphis' ,1,3,4,7],</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" t="s">
@@ -3461,11 +3529,14 @@
       <c r="G16">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="1:7">
+      <c r="H16">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Zach', 'Miami' ,1,2,2],</v>
+        <v>['Zach', 'Miami' ,1,2,2,3],</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" t="s">
@@ -3483,11 +3554,14 @@
       <c r="G17">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:7">
+      <c r="H17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Greg', 'Milwaukee' ,0,3,4],</v>
+        <v>['Greg', 'Milwaukee' ,0,3,4,5],</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" t="s">
@@ -3505,11 +3579,14 @@
       <c r="G18">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="1:7">
+      <c r="H18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Jeff', 'Minnesota' ,0,1,2],</v>
+        <v>['Jeff', 'Minnesota' ,0,1,2,4],</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" t="s">
@@ -3527,11 +3604,14 @@
       <c r="G19">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:7">
+      <c r="H19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Zach', 'New Orleans' ,0,0,1],</v>
+        <v>['Zach', 'New Orleans' ,0,0,1,2],</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" t="s">
@@ -3549,11 +3629,14 @@
       <c r="G20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:7">
+      <c r="H20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Zach', 'New York' ,0,2,3],</v>
+        <v>['Zach', 'New York' ,0,2,3,5],</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" t="s">
@@ -3571,11 +3654,14 @@
       <c r="G21">
         <v>3</v>
       </c>
-    </row>
-    <row r="22" spans="1:7">
+      <c r="H21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Jeff', 'Oklahoma City' ,2,4,6],</v>
+        <v>['Jeff', 'Oklahoma City' ,2,4,6,7],</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" t="s">
@@ -3593,11 +3679,14 @@
       <c r="G22">
         <v>6</v>
       </c>
-    </row>
-    <row r="23" spans="1:7">
+      <c r="H22">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
       <c r="A23" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Greg', 'Orlando' ,0,2,3],</v>
+        <v>['Greg', 'Orlando' ,0,2,3,5],</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" t="s">
@@ -3615,11 +3704,14 @@
       <c r="G23">
         <v>3</v>
       </c>
-    </row>
-    <row r="24" spans="1:7">
+      <c r="H23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
       <c r="A24" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['', 'Philadelphia' ,0,0,1],</v>
+        <v>['', 'Philadelphia' ,0,0,1,2],</v>
       </c>
       <c r="B24" s="3"/>
       <c r="D24" t="s">
@@ -3634,11 +3726,14 @@
       <c r="G24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:7">
+      <c r="H24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
       <c r="A25" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['', 'Phoenix' ,0,2,3],</v>
+        <v>['', 'Phoenix' ,0,2,3,3],</v>
       </c>
       <c r="B25" s="3"/>
       <c r="D25" t="s">
@@ -3653,11 +3748,14 @@
       <c r="G25">
         <v>3</v>
       </c>
-    </row>
-    <row r="26" spans="1:7">
+      <c r="H25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
       <c r="A26" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Greg', 'Portland' ,1,3,6],</v>
+        <v>['Greg', 'Portland' ,1,3,6,7],</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" t="s">
@@ -3675,11 +3773,14 @@
       <c r="G26">
         <v>6</v>
       </c>
-    </row>
-    <row r="27" spans="1:7">
+      <c r="H26">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
       <c r="A27" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Jeff', 'Sacramento' ,1,2,4],</v>
+        <v>['Jeff', 'Sacramento' ,1,2,4,4],</v>
       </c>
       <c r="B27" s="3"/>
       <c r="C27" t="s">
@@ -3697,11 +3798,14 @@
       <c r="G27">
         <v>4</v>
       </c>
-    </row>
-    <row r="28" spans="1:7">
+      <c r="H27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
       <c r="A28" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Jeff', 'San Antonio' ,2,5,6],</v>
+        <v>['Jeff', 'San Antonio' ,2,5,6,10],</v>
       </c>
       <c r="B28" s="3"/>
       <c r="C28" t="s">
@@ -3719,11 +3823,14 @@
       <c r="G28">
         <v>6</v>
       </c>
-    </row>
-    <row r="29" spans="1:7">
+      <c r="H28">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
       <c r="A29" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Greg', 'Toronto' ,1,4,6],</v>
+        <v>['Greg', 'Toronto' ,1,4,6,8],</v>
       </c>
       <c r="B29" s="3"/>
       <c r="C29" t="s">
@@ -3741,11 +3848,14 @@
       <c r="G29">
         <v>6</v>
       </c>
-    </row>
-    <row r="30" spans="1:7">
+      <c r="H29">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
       <c r="A30" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Zach', 'Utah' ,1,3,6],</v>
+        <v>['Zach', 'Utah' ,1,3,6,7],</v>
       </c>
       <c r="B30" s="3"/>
       <c r="C30" t="s">
@@ -3763,11 +3873,14 @@
       <c r="G30">
         <v>6</v>
       </c>
-    </row>
-    <row r="31" spans="1:7">
+      <c r="H30">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
       <c r="A31" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Tim', 'Washington' ,0,1,2],</v>
+        <v>['Tim', 'Washington' ,0,1,2,3],</v>
       </c>
       <c r="B31" s="3"/>
       <c r="C31" t="s">
@@ -3785,8 +3898,11 @@
       <c r="G31">
         <v>2</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" s="4" customFormat="1" ht="4" customHeight="1">
+      <c r="H31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" s="4" customFormat="1" ht="4" customHeight="1">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="F32" s="3"/>
@@ -3809,7 +3925,7 @@
       </c>
       <c r="H33" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="I33" s="2">
         <f t="shared" si="2"/>
@@ -3854,7 +3970,7 @@
       </c>
       <c r="H34" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="I34" s="2">
         <f t="shared" si="2"/>
@@ -3899,7 +4015,7 @@
       </c>
       <c r="H35" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="I35" s="2">
         <f t="shared" si="2"/>
@@ -3944,7 +4060,7 @@
       </c>
       <c r="H36" s="2">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="I36" s="2">
         <f t="shared" si="3"/>

</xml_diff>

<commit_message>
Update the NBA wins for the week.
</commit_message>
<xml_diff>
--- a/NFL Wins.xlsx
+++ b/NFL Wins.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8980" windowHeight="16100" tabRatio="500" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8980" windowHeight="16100" tabRatio="500" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
@@ -479,7 +479,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="105">
+  <cellStyleXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -578,6 +578,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -601,7 +605,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="105">
+  <cellStyles count="109">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -656,6 +660,8 @@
     <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -706,6 +712,8 @@
     <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1324,9 +1332,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y39"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <pane xSplit="4" topLeftCell="L1" activePane="topRight" state="frozenSplit"/>
-      <selection pane="topRight" activeCell="A3" sqref="A3:A34"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <pane xSplit="4" ySplit="2" topLeftCell="N8" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="topRight" activeCell="L1" sqref="L1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1450,8 +1460,8 @@
     </row>
     <row r="3" spans="1:25">
       <c r="A3" s="2" t="str">
-        <f>CONCATENATE("['",$C3,"', ","'",$D3,"' ,",$E3,",",$F3,",",$G3,",",$H3,",",$I3,",",$J3,",",$K3,",",$L3,",",$M3,",",$N3,",",$O3,"],")</f>
-        <v>['Greg', '49ers' ,1,1,1,1,1,1,1,1,1,1,],</v>
+        <f>CONCATENATE("['",$C3,"', ","'",$D3,"' ,",$E3,",",$F3,",",$G3,",",$H3,",",$I3,",",$J3,",",$K3,",",$L3,",",$M3,",",$N3,",",$O3,",",$P3,"],")</f>
+        <v>['Greg', '49ers' ,1,1,1,1,1,1,1,1,1,1,1,],</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" t="s">
@@ -1490,11 +1500,14 @@
       <c r="N3">
         <v>1</v>
       </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:25">
       <c r="A4" s="2" t="str">
-        <f t="shared" ref="A4:A34" si="1">CONCATENATE("['",$C4,"', ","'",$D4,"' ,",$E4,",",$F4,",",$G4,",",$H4,",",$I4,",",$J4,",",$K4,",",$L4,",",$M4,",",$N4,",",$O4,"],")</f>
-        <v>['Jeff', 'Bears' ,0,0,0,1,1,1,1,2,2,2,],</v>
+        <f t="shared" ref="A4:A7" si="1">CONCATENATE("['",$C4,"', ","'",$D4,"' ,",$E4,",",$F4,",",$G4,",",$H4,",",$I4,",",$J4,",",$K4,",",$L4,",",$M4,",",$N4,",",$O4,",",$P4,"],")</f>
+        <v>['Jeff', 'Bears' ,0,0,0,1,1,1,1,2,2,2,2,],</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" t="s">
@@ -1533,11 +1546,14 @@
       <c r="N4">
         <v>2</v>
       </c>
+      <c r="O4">
+        <v>2</v>
+      </c>
     </row>
     <row r="5" spans="1:25">
       <c r="A5" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Tim', 'Bengals' ,1,1,1,2,2,2,3,3,3,3,],</v>
+        <v>['Tim', 'Bengals' ,1,1,1,2,2,2,3,3,3,3,3,],</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" t="s">
@@ -1576,11 +1592,14 @@
       <c r="N5">
         <v>3</v>
       </c>
+      <c r="O5">
+        <v>3</v>
+      </c>
     </row>
     <row r="6" spans="1:25">
       <c r="A6" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Greg', 'Bills' ,0,0,1,2,3,4,4,4,4,4,],</v>
+        <v>['Greg', 'Bills' ,0,0,1,2,3,4,4,4,4,4,5,],</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" t="s">
@@ -1619,11 +1638,14 @@
       <c r="N6">
         <v>4</v>
       </c>
+      <c r="O6">
+        <v>5</v>
+      </c>
     </row>
     <row r="7" spans="1:25">
       <c r="A7" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Zach', 'Broncos' ,1,2,3,4,4,4,5,6,6,7,],</v>
+        <v>['Zach', 'Broncos' ,1,2,3,4,4,4,5,6,6,7,7,],</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" t="s">
@@ -1662,11 +1684,14 @@
       <c r="N7">
         <v>7</v>
       </c>
+      <c r="O7">
+        <v>7</v>
+      </c>
     </row>
     <row r="8" spans="1:25">
       <c r="A8" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>['Jeff', 'Browns' ,0,0,0,0,0,0,0,0,0,0,],</v>
+        <f>CONCATENATE("['",$C8,"', ","'",$D8,"' ,",$E8,",",$F8,",",$G8,",",$H8,",",$I8,",",$J8,",",$K8,",",$L8,",",$M8,",",$N8,",",$O8,",",$P8,",",$Q8,"],")</f>
+        <v>['Jeff', 'Browns' ,0,0,0,0,0,0,0,0,0,0,0,,],</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" t="s">
@@ -1705,11 +1730,14 @@
       <c r="N8">
         <v>0</v>
       </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:25">
       <c r="A9" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>['Zach', 'Buccaneers' ,1,1,1,1,2,2,3,3,3,4,],</v>
+        <f t="shared" ref="A9:A34" si="2">CONCATENATE("['",$C9,"', ","'",$D9,"' ,",$E9,",",$F9,",",$G9,",",$H9,",",$I9,",",$J9,",",$K9,",",$L9,",",$M9,",",$N9,",",$O9,",",$P9,",",$Q9,"],")</f>
+        <v>['Zach', 'Buccaneers' ,1,1,1,1,2,2,3,3,3,4,5,,],</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" t="s">
@@ -1748,11 +1776,14 @@
       <c r="N9">
         <v>4</v>
       </c>
+      <c r="O9">
+        <v>5</v>
+      </c>
     </row>
     <row r="10" spans="1:25">
       <c r="A10" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>['Jeff', 'Cardinals' ,0,1,1,1,2,3,3,3,3,4,],</v>
+        <f t="shared" si="2"/>
+        <v>['Jeff', 'Cardinals' ,0,1,1,1,2,3,3,3,3,4,4,,],</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" t="s">
@@ -1791,11 +1822,14 @@
       <c r="N10">
         <v>4</v>
       </c>
+      <c r="O10">
+        <v>4</v>
+      </c>
     </row>
     <row r="11" spans="1:25">
       <c r="A11" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>['Jeff', 'Chargers' ,0,1,1,1,1,2,3,3,4,4,],</v>
+        <f t="shared" si="2"/>
+        <v>['Jeff', 'Chargers' ,0,1,1,1,1,2,3,3,4,4,4,,],</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" t="s">
@@ -1834,11 +1868,14 @@
       <c r="N11">
         <v>4</v>
       </c>
+      <c r="O11">
+        <v>4</v>
+      </c>
     </row>
     <row r="12" spans="1:25">
       <c r="A12" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>['Zach', 'Chiefs' ,1,1,2,2,2,3,4,5,6,7,],</v>
+        <f t="shared" si="2"/>
+        <v>['Zach', 'Chiefs' ,1,1,2,2,2,3,4,5,6,7,7,,],</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" t="s">
@@ -1877,11 +1914,14 @@
       <c r="N12">
         <v>7</v>
       </c>
+      <c r="O12">
+        <v>7</v>
+      </c>
     </row>
     <row r="13" spans="1:25">
       <c r="A13" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>['Greg', 'Colts' ,0,0,1,1,2,2,3,3,4,4,],</v>
+        <f t="shared" si="2"/>
+        <v>['Greg', 'Colts' ,0,0,1,1,2,2,3,3,4,4,5,5,],</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" t="s">
@@ -1920,11 +1960,17 @@
       <c r="N13">
         <v>4</v>
       </c>
+      <c r="O13">
+        <v>5</v>
+      </c>
+      <c r="P13">
+        <v>5</v>
+      </c>
     </row>
     <row r="14" spans="1:25">
       <c r="A14" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>['Greg', 'Cowboys' ,0,1,2,3,4,5,5,6,7,8,],</v>
+        <f t="shared" si="2"/>
+        <v>['Greg', 'Cowboys' ,0,1,2,3,4,5,5,6,7,8,9,10,],</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" t="s">
@@ -1963,11 +2009,17 @@
       <c r="N14">
         <v>8</v>
       </c>
+      <c r="O14">
+        <v>9</v>
+      </c>
+      <c r="P14">
+        <v>10</v>
+      </c>
     </row>
     <row r="15" spans="1:25">
       <c r="A15" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>['Tim', 'Dolphins' ,0,0,1,1,1,2,3,3,4,5,],</v>
+        <f t="shared" si="2"/>
+        <v>['Tim', 'Dolphins' ,0,0,1,1,1,2,3,3,4,5,6,,],</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" t="s">
@@ -2006,11 +2058,14 @@
       <c r="N15">
         <v>5</v>
       </c>
+      <c r="O15">
+        <v>6</v>
+      </c>
     </row>
     <row r="16" spans="1:25">
       <c r="A16" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>['Zach', 'Eagles' ,1,2,3,3,3,3,4,4,4,5,],</v>
+        <f t="shared" si="2"/>
+        <v>['Zach', 'Eagles' ,1,2,3,3,3,3,4,4,4,5,5,,],</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" t="s">
@@ -2049,11 +2104,14 @@
       <c r="N16">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:15">
+      <c r="O16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16">
       <c r="A17" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>['Greg', 'Falcons' ,0,1,2,3,4,4,4,5,6,6,],</v>
+        <f t="shared" si="2"/>
+        <v>['Greg', 'Falcons' ,0,1,2,3,4,4,4,5,6,6,6,,],</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" t="s">
@@ -2092,11 +2150,14 @@
       <c r="N17">
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="1:15">
+      <c r="O17">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16">
       <c r="A18" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>['Jeff', 'Giants' ,1,2,2,2,2,3,4,4,5,6,],</v>
+        <f t="shared" si="2"/>
+        <v>['Jeff', 'Giants' ,1,2,2,2,2,3,4,4,5,6,7,,],</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" t="s">
@@ -2135,11 +2196,14 @@
       <c r="N18">
         <v>6</v>
       </c>
-    </row>
-    <row r="19" spans="1:15">
+      <c r="O18">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16">
       <c r="A19" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>['Tim', 'Jaguars' ,0,0,0,1,1,2,2,2,2,2,],</v>
+        <f t="shared" si="2"/>
+        <v>['Tim', 'Jaguars' ,0,0,0,1,1,2,2,2,2,2,2,,],</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" t="s">
@@ -2178,11 +2242,14 @@
       <c r="N19">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:15">
+      <c r="O19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16">
       <c r="A20" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>['Tim', 'Jets' ,0,1,1,1,1,1,2,3,3,3,],</v>
+        <f t="shared" si="2"/>
+        <v>['Tim', 'Jets' ,0,1,1,1,1,1,2,3,3,3,3,,],</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" t="s">
@@ -2221,11 +2288,14 @@
       <c r="N20">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="1:15">
+      <c r="O20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16">
       <c r="A21" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>['Jeff', 'Lions' ,1,1,1,1,2,3,4,4,5,5,],</v>
+        <f t="shared" si="2"/>
+        <v>['Jeff', 'Lions' ,1,1,1,1,2,3,4,4,5,5,6,7,],</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" t="s">
@@ -2264,11 +2334,17 @@
       <c r="N21">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="1:15">
+      <c r="O21">
+        <v>6</v>
+      </c>
+      <c r="P21">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16">
       <c r="A22" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>['Tim', 'Packers' ,1,1,2,2,3,3,4,4,4,4,],</v>
+        <f t="shared" si="2"/>
+        <v>['Tim', 'Packers' ,1,1,2,2,3,3,4,4,4,4,4,,],</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" t="s">
@@ -2307,11 +2383,14 @@
       <c r="N22">
         <v>4</v>
       </c>
-    </row>
-    <row r="23" spans="1:15">
+      <c r="O22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16">
       <c r="A23" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>['Greg', 'Panthers' ,0,1,1,1,1,1,1,2,3,3,4],</v>
+        <f t="shared" si="2"/>
+        <v>['Greg', 'Panthers' ,0,1,1,1,1,1,1,2,3,3,4,,],</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" t="s">
@@ -2354,10 +2433,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:15">
+    <row r="24" spans="1:16">
       <c r="A24" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>['Greg', 'Patriots' ,1,2,3,3,4,5,6,7,7,7,],</v>
+        <f t="shared" si="2"/>
+        <v>['Greg', 'Patriots' ,1,2,3,3,4,5,6,7,7,7,8,,],</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" t="s">
@@ -2396,11 +2475,14 @@
       <c r="N24">
         <v>7</v>
       </c>
-    </row>
-    <row r="25" spans="1:15">
+      <c r="O24">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16">
       <c r="A25" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>['Tim', 'Raiders' ,1,1,2,3,4,4,5,6,7,7,],</v>
+        <f t="shared" si="2"/>
+        <v>['Tim', 'Raiders' ,1,1,2,3,4,4,5,6,7,7,8,,],</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" t="s">
@@ -2439,11 +2521,14 @@
       <c r="N25">
         <v>7</v>
       </c>
-    </row>
-    <row r="26" spans="1:15">
+      <c r="O25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16">
       <c r="A26" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>['Zach', 'Rams' ,0,1,2,3,3,3,3,3,3,4,],</v>
+        <f t="shared" si="2"/>
+        <v>['Zach', 'Rams' ,0,1,2,3,3,3,3,3,3,4,4,,],</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" t="s">
@@ -2482,11 +2567,14 @@
       <c r="N26">
         <v>4</v>
       </c>
-    </row>
-    <row r="27" spans="1:15">
+      <c r="O26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16">
       <c r="A27" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>['Jeff', 'Ravens' ,1,2,3,3,3,3,3,3,4,5,],</v>
+        <f t="shared" si="2"/>
+        <v>['Jeff', 'Ravens' ,1,2,3,3,3,3,3,3,4,5,5,,],</v>
       </c>
       <c r="B27" s="3"/>
       <c r="C27" t="s">
@@ -2525,11 +2613,14 @@
       <c r="N27">
         <v>5</v>
       </c>
-    </row>
-    <row r="28" spans="1:15">
+      <c r="O27">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16">
       <c r="A28" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>['Greg', 'Redskins' ,0,0,1,2,3,4,4,4,4,5,],</v>
+        <f t="shared" si="2"/>
+        <v>['Greg', 'Redskins' ,0,0,1,2,3,4,4,4,4,5,6,6,],</v>
       </c>
       <c r="B28" s="3"/>
       <c r="C28" t="s">
@@ -2568,11 +2659,17 @@
       <c r="N28">
         <v>5</v>
       </c>
-    </row>
-    <row r="29" spans="1:15">
+      <c r="O28">
+        <v>6</v>
+      </c>
+      <c r="P28">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16">
       <c r="A29" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>['Zach', 'Saints' ,0,0,0,1,1,2,2,3,4,4,4],</v>
+        <f t="shared" si="2"/>
+        <v>['Zach', 'Saints' ,0,0,0,1,1,2,2,3,4,4,4,,],</v>
       </c>
       <c r="B29" s="3"/>
       <c r="C29" t="s">
@@ -2615,10 +2712,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:15">
+    <row r="30" spans="1:16">
       <c r="A30" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>['Zach', 'Seahawks' ,1,1,2,3,3,4,4,4,5,6,],</v>
+        <f t="shared" si="2"/>
+        <v>['Zach', 'Seahawks' ,1,1,2,3,3,4,4,4,5,6,7,,],</v>
       </c>
       <c r="B30" s="3"/>
       <c r="C30" t="s">
@@ -2657,11 +2754,14 @@
       <c r="N30">
         <v>6</v>
       </c>
-    </row>
-    <row r="31" spans="1:15">
+      <c r="O30">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16">
       <c r="A31" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>['Tim', 'Steelers' ,1,2,2,3,4,4,4,4,4,4,],</v>
+        <f t="shared" si="2"/>
+        <v>['Tim', 'Steelers' ,1,2,2,3,4,4,4,4,4,4,5,6,],</v>
       </c>
       <c r="B31" s="3"/>
       <c r="C31" t="s">
@@ -2700,11 +2800,17 @@
       <c r="N31">
         <v>4</v>
       </c>
-    </row>
-    <row r="32" spans="1:15">
+      <c r="O31">
+        <v>5</v>
+      </c>
+      <c r="P31">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16">
       <c r="A32" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>['Jeff', 'Texans' ,1,2,2,3,3,4,4,5,5,6,],</v>
+        <f t="shared" si="2"/>
+        <v>['Jeff', 'Texans' ,1,2,2,3,3,4,4,5,5,6,6,,],</v>
       </c>
       <c r="B32" s="3"/>
       <c r="C32" t="s">
@@ -2743,11 +2849,14 @@
       <c r="N32">
         <v>6</v>
       </c>
-    </row>
-    <row r="33" spans="1:15">
+      <c r="O32">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16">
       <c r="A33" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>['Zach', 'Titans' ,0,1,1,1,2,3,3,4,4,5,],</v>
+        <f t="shared" si="2"/>
+        <v>['Zach', 'Titans' ,0,1,1,1,2,3,3,4,4,5,5,,],</v>
       </c>
       <c r="B33" s="3"/>
       <c r="C33" t="s">
@@ -2786,11 +2895,14 @@
       <c r="N33">
         <v>5</v>
       </c>
-    </row>
-    <row r="34" spans="1:15">
+      <c r="O33">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16">
       <c r="A34" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>['Tim', 'Vikings' ,1,2,3,4,5,5,5,5,5,5,],</v>
+        <f t="shared" si="2"/>
+        <v>['Tim', 'Vikings' ,1,2,3,4,5,5,5,5,5,5,6,6,],</v>
       </c>
       <c r="B34" s="3"/>
       <c r="C34" t="s">
@@ -2829,206 +2941,228 @@
       <c r="N34">
         <v>5</v>
       </c>
-    </row>
-    <row r="35" spans="1:15" s="4" customFormat="1" ht="4" customHeight="1">
+      <c r="O34">
+        <v>6</v>
+      </c>
+      <c r="P34">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" s="4" customFormat="1" ht="4" customHeight="1">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="F35" s="3"/>
     </row>
-    <row r="36" spans="1:15">
+    <row r="36" spans="1:16">
       <c r="D36" t="s">
         <v>32</v>
       </c>
       <c r="E36">
-        <f t="shared" ref="E36:O38" si="2">SUMIF($C$3:$C$34,$D36,E$3:E$34)</f>
+        <f t="shared" ref="E36:P38" si="3">SUMIF($C$3:$C$34,$D36,E$3:E$34)</f>
         <v>4</v>
       </c>
       <c r="F36" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="G36" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="H36" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="I36" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
       <c r="J36" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>19</v>
       </c>
       <c r="K36" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>22</v>
       </c>
       <c r="L36" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>24</v>
       </c>
       <c r="M36" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>28</v>
       </c>
       <c r="N36" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>32</v>
       </c>
       <c r="O36" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15">
+        <f t="shared" si="3"/>
+        <v>34</v>
+      </c>
+      <c r="P36" s="2">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16">
       <c r="D37" t="s">
         <v>33</v>
       </c>
       <c r="E37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="F37" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="G37" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="H37" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>16</v>
       </c>
       <c r="I37" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>22</v>
       </c>
       <c r="J37" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>26</v>
       </c>
       <c r="K37" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>28</v>
       </c>
       <c r="L37" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>32</v>
       </c>
       <c r="M37" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>36</v>
       </c>
       <c r="N37" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>38</v>
       </c>
       <c r="O37" s="2">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15">
+        <f t="shared" si="3"/>
+        <v>44</v>
+      </c>
+      <c r="P37" s="2">
+        <f t="shared" si="3"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16">
       <c r="D38" t="s">
         <v>34</v>
       </c>
       <c r="E38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="F38" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="G38" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="H38" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>17</v>
       </c>
       <c r="I38" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>21</v>
       </c>
       <c r="J38" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>23</v>
       </c>
       <c r="K38" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>28</v>
       </c>
       <c r="L38" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>30</v>
       </c>
       <c r="M38" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>32</v>
       </c>
       <c r="N38" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>33</v>
       </c>
       <c r="O38" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15">
+        <f t="shared" si="3"/>
+        <v>37</v>
+      </c>
+      <c r="P38" s="2">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16">
       <c r="D39" t="s">
         <v>35</v>
       </c>
       <c r="E39">
-        <f t="shared" ref="E39:O39" si="3">SUMIF($C$3:$C$34,$D$39,E$3:E$34)</f>
+        <f t="shared" ref="E39:P39" si="4">SUMIF($C$3:$C$34,$D$39,E$3:E$34)</f>
         <v>5</v>
       </c>
       <c r="F39" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9</v>
       </c>
       <c r="G39" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="H39" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="I39" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
       <c r="J39" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>24</v>
       </c>
       <c r="K39" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>28</v>
       </c>
       <c r="L39" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>32</v>
       </c>
       <c r="M39" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>35</v>
       </c>
       <c r="N39" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>42</v>
       </c>
       <c r="O39" s="2">
-        <f t="shared" si="3"/>
-        <v>4</v>
+        <f t="shared" si="4"/>
+        <v>44</v>
+      </c>
+      <c r="P39" s="2">
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3049,9 +3183,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y36"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <pane xSplit="4" topLeftCell="F1" activePane="topRight" state="frozenSplit"/>
-      <selection pane="topRight" activeCell="A2" sqref="A2:A31"/>
+      <selection pane="topRight" activeCell="A31" sqref="A2:A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3160,8 +3294,8 @@
     </row>
     <row r="2" spans="1:25">
       <c r="A2" s="2" t="str">
-        <f>CONCATENATE("['",$C2,"', ","'",$D2,"' ,",$E2,",",$F2,",",$G2,",",$H2,"],")</f>
-        <v>['Zach', 'Atlanta' ,1,3,6,9],</v>
+        <f>CONCATENATE("['",$C2,"', ","'",$D2,"' ,",$E2,",",$F2,",",$G2,",",$H2,",",$I2,"],")</f>
+        <v>['Zach', 'Atlanta' ,1,3,6,9,10],</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" t="s">
@@ -3182,11 +3316,14 @@
       <c r="H2">
         <v>9</v>
       </c>
+      <c r="I2">
+        <v>10</v>
+      </c>
     </row>
     <row r="3" spans="1:25">
       <c r="A3" s="2" t="str">
-        <f t="shared" ref="A3:A31" si="1">CONCATENATE("['",$C3,"', ","'",$D3,"' ,",$E3,",",$F3,",",$G3,",",$H3,"],")</f>
-        <v>['Jeff', 'Boston' ,1,3,4,6],</v>
+        <f t="shared" ref="A3:A32" si="1">CONCATENATE("['",$C3,"', ","'",$D3,"' ,",$E3,",",$F3,",",$G3,",",$H3,",",$I3,"],")</f>
+        <v>['Jeff', 'Boston' ,1,3,4,6,9],</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" t="s">
@@ -3207,11 +3344,14 @@
       <c r="H3">
         <v>6</v>
       </c>
+      <c r="I3">
+        <v>9</v>
+      </c>
     </row>
     <row r="4" spans="1:25">
       <c r="A4" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Zach', 'Brooklyn' ,1,2,3,4],</v>
+        <v>['Zach', 'Brooklyn' ,1,2,3,4,4],</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" t="s">
@@ -3232,11 +3372,14 @@
       <c r="H4">
         <v>4</v>
       </c>
+      <c r="I4">
+        <v>4</v>
+      </c>
     </row>
     <row r="5" spans="1:25">
       <c r="A5" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Jeff', 'Charlotte' ,2,4,6,8],</v>
+        <v>['Jeff', 'Charlotte' ,2,4,6,8,8],</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" t="s">
@@ -3257,11 +3400,14 @@
       <c r="H5">
         <v>8</v>
       </c>
+      <c r="I5">
+        <v>8</v>
+      </c>
     </row>
     <row r="6" spans="1:25">
       <c r="A6" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Greg', 'Chicago' ,1,3,5,8],</v>
+        <v>['Greg', 'Chicago' ,1,3,5,8,10],</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" t="s">
@@ -3282,11 +3428,14 @@
       <c r="H6">
         <v>8</v>
       </c>
+      <c r="I6">
+        <v>10</v>
+      </c>
     </row>
     <row r="7" spans="1:25">
       <c r="A7" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Tim', 'Cleveland' ,2,5,7,10],</v>
+        <v>['Tim', 'Cleveland' ,2,5,7,10,12],</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" t="s">
@@ -3307,11 +3456,14 @@
       <c r="H7">
         <v>10</v>
       </c>
+      <c r="I7">
+        <v>12</v>
+      </c>
     </row>
     <row r="8" spans="1:25">
       <c r="A8" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Tim', 'Dallas' ,0,0,2,2],</v>
+        <v>['Tim', 'Dallas' ,0,0,2,2,2],</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" t="s">
@@ -3332,11 +3484,14 @@
       <c r="H8">
         <v>2</v>
       </c>
+      <c r="I8">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" spans="1:25">
       <c r="A9" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Tim', 'Denver' ,1,2,3,4],</v>
+        <v>['Tim', 'Denver' ,1,2,3,4,6],</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" t="s">
@@ -3357,11 +3512,14 @@
       <c r="H9">
         <v>4</v>
       </c>
+      <c r="I9">
+        <v>6</v>
+      </c>
     </row>
     <row r="10" spans="1:25">
       <c r="A10" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Greg', 'Detroit' ,1,3,4,6],</v>
+        <v>['Greg', 'Detroit' ,1,3,4,6,8],</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" t="s">
@@ -3382,11 +3540,14 @@
       <c r="H10">
         <v>6</v>
       </c>
+      <c r="I10">
+        <v>8</v>
+      </c>
     </row>
     <row r="11" spans="1:25">
       <c r="A11" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Zach', 'Golden State' ,1,4,7,9],</v>
+        <v>['Zach', 'Golden State' ,1,4,7,9,14],</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" t="s">
@@ -3407,11 +3568,14 @@
       <c r="H11">
         <v>9</v>
       </c>
+      <c r="I11">
+        <v>14</v>
+      </c>
     </row>
     <row r="12" spans="1:25">
       <c r="A12" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Jeff', 'Houston' ,1,3,5,7],</v>
+        <v>['Jeff', 'Houston' ,1,3,5,7,10],</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" t="s">
@@ -3432,11 +3596,14 @@
       <c r="H12">
         <v>7</v>
       </c>
+      <c r="I12">
+        <v>10</v>
+      </c>
     </row>
     <row r="13" spans="1:25">
       <c r="A13" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Tim', 'Indiana' ,1,2,4,6],</v>
+        <v>['Tim', 'Indiana' ,1,2,4,6,8],</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" t="s">
@@ -3457,11 +3624,14 @@
       <c r="H13">
         <v>6</v>
       </c>
+      <c r="I13">
+        <v>8</v>
+      </c>
     </row>
     <row r="14" spans="1:25">
       <c r="A14" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Tim', 'L.A. Lakers' ,1,3,5,7],</v>
+        <v>['Tim', 'L.A. Lakers' ,1,3,5,7,8],</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" t="s">
@@ -3482,11 +3652,14 @@
       <c r="H14">
         <v>7</v>
       </c>
+      <c r="I14">
+        <v>8</v>
+      </c>
     </row>
     <row r="15" spans="1:25">
       <c r="A15" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Greg', 'LA Clippers' ,1,4,8,11],</v>
+        <v>['Greg', 'LA Clippers' ,1,4,8,11,14],</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" t="s">
@@ -3507,11 +3680,14 @@
       <c r="H15">
         <v>11</v>
       </c>
+      <c r="I15">
+        <v>14</v>
+      </c>
     </row>
     <row r="16" spans="1:25">
       <c r="A16" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Tim', 'Memphis' ,1,3,4,7],</v>
+        <v>['Tim', 'Memphis' ,1,3,4,7,10],</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" t="s">
@@ -3532,11 +3708,14 @@
       <c r="H16">
         <v>7</v>
       </c>
-    </row>
-    <row r="17" spans="1:8">
+      <c r="I16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Zach', 'Miami' ,1,2,2,3],</v>
+        <v>['Zach', 'Miami' ,1,2,2,3,5],</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" t="s">
@@ -3557,11 +3736,14 @@
       <c r="H17">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="1:8">
+      <c r="I17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Greg', 'Milwaukee' ,0,3,4,5],</v>
+        <v>['Greg', 'Milwaukee' ,0,3,4,5,6],</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" t="s">
@@ -3582,11 +3764,14 @@
       <c r="H18">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="1:8">
+      <c r="I18">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Jeff', 'Minnesota' ,0,1,2,4],</v>
+        <v>['Jeff', 'Minnesota' ,0,1,2,4,5],</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" t="s">
@@ -3607,11 +3792,14 @@
       <c r="H19">
         <v>4</v>
       </c>
-    </row>
-    <row r="20" spans="1:8">
+      <c r="I19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Zach', 'New Orleans' ,0,0,1,2],</v>
+        <v>['Zach', 'New Orleans' ,0,0,1,2,6],</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" t="s">
@@ -3632,11 +3820,14 @@
       <c r="H20">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:8">
+      <c r="I20">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Zach', 'New York' ,0,2,3,5],</v>
+        <v>['Zach', 'New York' ,0,2,3,5,8],</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" t="s">
@@ -3657,11 +3848,14 @@
       <c r="H21">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="1:8">
+      <c r="I21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
       <c r="A22" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Jeff', 'Oklahoma City' ,2,4,6,7],</v>
+        <v>['Jeff', 'Oklahoma City' ,2,4,6,7,9],</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" t="s">
@@ -3682,11 +3876,14 @@
       <c r="H22">
         <v>7</v>
       </c>
-    </row>
-    <row r="23" spans="1:8">
+      <c r="I22">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Greg', 'Orlando' ,0,2,3,5],</v>
+        <v>['Greg', 'Orlando' ,0,2,3,5,6],</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" t="s">
@@ -3707,11 +3904,14 @@
       <c r="H23">
         <v>5</v>
       </c>
-    </row>
-    <row r="24" spans="1:8">
+      <c r="I23">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['', 'Philadelphia' ,0,0,1,2],</v>
+        <v>['', 'Philadelphia' ,0,0,1,2,4],</v>
       </c>
       <c r="B24" s="3"/>
       <c r="D24" t="s">
@@ -3729,11 +3929,14 @@
       <c r="H24">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="1:8">
+      <c r="I24">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['', 'Phoenix' ,0,2,3,3],</v>
+        <v>['', 'Phoenix' ,0,2,3,3,5],</v>
       </c>
       <c r="B25" s="3"/>
       <c r="D25" t="s">
@@ -3751,11 +3954,14 @@
       <c r="H25">
         <v>3</v>
       </c>
-    </row>
-    <row r="26" spans="1:8">
+      <c r="I25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
       <c r="A26" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Greg', 'Portland' ,1,3,6,7],</v>
+        <v>['Greg', 'Portland' ,1,3,6,7,9],</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" t="s">
@@ -3776,11 +3982,14 @@
       <c r="H26">
         <v>7</v>
       </c>
-    </row>
-    <row r="27" spans="1:8">
+      <c r="I26">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
       <c r="A27" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Jeff', 'Sacramento' ,1,2,4,4],</v>
+        <v>['Jeff', 'Sacramento' ,1,2,4,4,6],</v>
       </c>
       <c r="B27" s="3"/>
       <c r="C27" t="s">
@@ -3801,11 +4010,14 @@
       <c r="H27">
         <v>4</v>
       </c>
-    </row>
-    <row r="28" spans="1:8">
+      <c r="I27">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
       <c r="A28" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Jeff', 'San Antonio' ,2,5,6,10],</v>
+        <v>['Jeff', 'San Antonio' ,2,5,6,10,13],</v>
       </c>
       <c r="B28" s="3"/>
       <c r="C28" t="s">
@@ -3826,11 +4038,14 @@
       <c r="H28">
         <v>10</v>
       </c>
-    </row>
-    <row r="29" spans="1:8">
+      <c r="I28">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
       <c r="A29" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Greg', 'Toronto' ,1,4,6,8],</v>
+        <v>['Greg', 'Toronto' ,1,4,6,8,10],</v>
       </c>
       <c r="B29" s="3"/>
       <c r="C29" t="s">
@@ -3851,11 +4066,14 @@
       <c r="H29">
         <v>8</v>
       </c>
-    </row>
-    <row r="30" spans="1:8">
+      <c r="I29">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
       <c r="A30" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Zach', 'Utah' ,1,3,6,7],</v>
+        <v>['Zach', 'Utah' ,1,3,6,7,9],</v>
       </c>
       <c r="B30" s="3"/>
       <c r="C30" t="s">
@@ -3876,11 +4094,14 @@
       <c r="H30">
         <v>7</v>
       </c>
-    </row>
-    <row r="31" spans="1:8">
+      <c r="I30">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
       <c r="A31" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Tim', 'Washington' ,0,1,2,3],</v>
+        <v>['Tim', 'Washington' ,0,1,2,3,5],</v>
       </c>
       <c r="B31" s="3"/>
       <c r="C31" t="s">
@@ -3901,9 +4122,12 @@
       <c r="H31">
         <v>3</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" s="4" customFormat="1" ht="4" customHeight="1">
-      <c r="A32" s="3"/>
+      <c r="I31">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" s="4" customFormat="1" ht="4" customHeight="1">
+      <c r="A32" s="2"/>
       <c r="B32" s="3"/>
       <c r="F32" s="3"/>
     </row>
@@ -3929,7 +4153,7 @@
       </c>
       <c r="I33" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="J33" s="2">
         <f t="shared" si="2"/>
@@ -3974,7 +4198,7 @@
       </c>
       <c r="I34" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>63</v>
       </c>
       <c r="J34" s="2">
         <f t="shared" si="2"/>
@@ -4019,7 +4243,7 @@
       </c>
       <c r="I35" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>51</v>
       </c>
       <c r="J35" s="2">
         <f t="shared" si="2"/>
@@ -4064,7 +4288,7 @@
       </c>
       <c r="I36" s="2">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="J36" s="2">
         <f t="shared" si="3"/>

</xml_diff>

<commit_message>
Added NFL week 11 and 12 wins.
</commit_message>
<xml_diff>
--- a/NFL Wins.xlsx
+++ b/NFL Wins.xlsx
@@ -479,7 +479,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="109">
+  <cellStyleXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -578,6 +578,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -605,7 +611,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="109">
+  <cellStyles count="115">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -662,6 +668,9 @@
     <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -714,6 +723,9 @@
     <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1333,10 +1345,10 @@
   <dimension ref="A1:Y39"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="N8" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="O6" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="L1" sqref="L1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="P8" sqref="P8"/>
+      <selection pane="bottomRight" activeCell="A34" sqref="A3:A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1461,7 +1473,7 @@
     <row r="3" spans="1:25">
       <c r="A3" s="2" t="str">
         <f>CONCATENATE("['",$C3,"', ","'",$D3,"' ,",$E3,",",$F3,",",$G3,",",$H3,",",$I3,",",$J3,",",$K3,",",$L3,",",$M3,",",$N3,",",$O3,",",$P3,"],")</f>
-        <v>['Greg', '49ers' ,1,1,1,1,1,1,1,1,1,1,1,],</v>
+        <v>['Greg', '49ers' ,1,1,1,1,1,1,1,1,1,1,1,1],</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" t="s">
@@ -1503,11 +1515,14 @@
       <c r="O3">
         <v>1</v>
       </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:25">
       <c r="A4" s="2" t="str">
         <f t="shared" ref="A4:A7" si="1">CONCATENATE("['",$C4,"', ","'",$D4,"' ,",$E4,",",$F4,",",$G4,",",$H4,",",$I4,",",$J4,",",$K4,",",$L4,",",$M4,",",$N4,",",$O4,",",$P4,"],")</f>
-        <v>['Jeff', 'Bears' ,0,0,0,1,1,1,1,2,2,2,2,],</v>
+        <v>['Jeff', 'Bears' ,0,0,0,1,1,1,1,2,2,2,2,2],</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" t="s">
@@ -1549,11 +1564,14 @@
       <c r="O4">
         <v>2</v>
       </c>
+      <c r="P4">
+        <v>2</v>
+      </c>
     </row>
     <row r="5" spans="1:25">
       <c r="A5" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Tim', 'Bengals' ,1,1,1,2,2,2,3,3,3,3,3,],</v>
+        <v>['Tim', 'Bengals' ,1,1,1,2,2,2,3,3,3,3,3,3],</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" t="s">
@@ -1595,11 +1613,14 @@
       <c r="O5">
         <v>3</v>
       </c>
+      <c r="P5">
+        <v>3</v>
+      </c>
     </row>
     <row r="6" spans="1:25">
       <c r="A6" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Greg', 'Bills' ,0,0,1,2,3,4,4,4,4,4,5,],</v>
+        <v>['Greg', 'Bills' ,0,0,1,2,3,4,4,4,4,4,5,6],</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" t="s">
@@ -1641,11 +1662,14 @@
       <c r="O6">
         <v>5</v>
       </c>
+      <c r="P6">
+        <v>6</v>
+      </c>
     </row>
     <row r="7" spans="1:25">
       <c r="A7" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Zach', 'Broncos' ,1,2,3,4,4,4,5,6,6,7,7,],</v>
+        <v>['Zach', 'Broncos' ,1,2,3,4,4,4,5,6,6,7,7,7],</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" t="s">
@@ -1687,11 +1711,14 @@
       <c r="O7">
         <v>7</v>
       </c>
+      <c r="P7">
+        <v>7</v>
+      </c>
     </row>
     <row r="8" spans="1:25">
       <c r="A8" s="2" t="str">
         <f>CONCATENATE("['",$C8,"', ","'",$D8,"' ,",$E8,",",$F8,",",$G8,",",$H8,",",$I8,",",$J8,",",$K8,",",$L8,",",$M8,",",$N8,",",$O8,",",$P8,",",$Q8,"],")</f>
-        <v>['Jeff', 'Browns' ,0,0,0,0,0,0,0,0,0,0,0,,],</v>
+        <v>['Jeff', 'Browns' ,0,0,0,0,0,0,0,0,0,0,0,0,],</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" t="s">
@@ -1733,11 +1760,14 @@
       <c r="O8">
         <v>0</v>
       </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:25">
       <c r="A9" s="2" t="str">
         <f t="shared" ref="A9:A34" si="2">CONCATENATE("['",$C9,"', ","'",$D9,"' ,",$E9,",",$F9,",",$G9,",",$H9,",",$I9,",",$J9,",",$K9,",",$L9,",",$M9,",",$N9,",",$O9,",",$P9,",",$Q9,"],")</f>
-        <v>['Zach', 'Buccaneers' ,1,1,1,1,2,2,3,3,3,4,5,,],</v>
+        <v>['Zach', 'Buccaneers' ,1,1,1,1,2,2,3,3,3,4,5,6,],</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" t="s">
@@ -1779,11 +1809,14 @@
       <c r="O9">
         <v>5</v>
       </c>
+      <c r="P9">
+        <v>6</v>
+      </c>
     </row>
     <row r="10" spans="1:25">
       <c r="A10" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>['Jeff', 'Cardinals' ,0,1,1,1,2,3,3,3,3,4,4,,],</v>
+        <v>['Jeff', 'Cardinals' ,0,1,1,1,2,3,3,3,3,4,4,4,],</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" t="s">
@@ -1825,11 +1858,14 @@
       <c r="O10">
         <v>4</v>
       </c>
+      <c r="P10">
+        <v>4</v>
+      </c>
     </row>
     <row r="11" spans="1:25">
       <c r="A11" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>['Jeff', 'Chargers' ,0,1,1,1,1,2,3,3,4,4,4,,],</v>
+        <v>['Jeff', 'Chargers' ,0,1,1,1,1,2,3,3,4,4,4,5,],</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" t="s">
@@ -1871,11 +1907,14 @@
       <c r="O11">
         <v>4</v>
       </c>
+      <c r="P11">
+        <v>5</v>
+      </c>
     </row>
     <row r="12" spans="1:25">
       <c r="A12" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>['Zach', 'Chiefs' ,1,1,2,2,2,3,4,5,6,7,7,,],</v>
+        <v>['Zach', 'Chiefs' ,1,1,2,2,2,3,4,5,6,7,7,8,],</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" t="s">
@@ -1917,6 +1956,9 @@
       <c r="O12">
         <v>7</v>
       </c>
+      <c r="P12">
+        <v>8</v>
+      </c>
     </row>
     <row r="13" spans="1:25">
       <c r="A13" s="2" t="str">
@@ -2019,7 +2061,7 @@
     <row r="15" spans="1:25">
       <c r="A15" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>['Tim', 'Dolphins' ,0,0,1,1,1,2,3,3,4,5,6,,],</v>
+        <v>['Tim', 'Dolphins' ,0,0,1,1,1,2,3,3,4,5,6,7,],</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" t="s">
@@ -2061,11 +2103,14 @@
       <c r="O15">
         <v>6</v>
       </c>
+      <c r="P15">
+        <v>7</v>
+      </c>
     </row>
     <row r="16" spans="1:25">
       <c r="A16" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>['Zach', 'Eagles' ,1,2,3,3,3,3,4,4,4,5,5,,],</v>
+        <v>['Zach', 'Eagles' ,1,2,3,3,3,3,4,4,4,5,5,5,],</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" t="s">
@@ -2107,11 +2152,14 @@
       <c r="O16">
         <v>5</v>
       </c>
+      <c r="P16">
+        <v>5</v>
+      </c>
     </row>
     <row r="17" spans="1:16">
       <c r="A17" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>['Greg', 'Falcons' ,0,1,2,3,4,4,4,5,6,6,6,,],</v>
+        <v>['Greg', 'Falcons' ,0,1,2,3,4,4,4,5,6,6,6,7,],</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" t="s">
@@ -2153,11 +2201,14 @@
       <c r="O17">
         <v>6</v>
       </c>
+      <c r="P17">
+        <v>7</v>
+      </c>
     </row>
     <row r="18" spans="1:16">
       <c r="A18" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>['Jeff', 'Giants' ,1,2,2,2,2,3,4,4,5,6,7,,],</v>
+        <v>['Jeff', 'Giants' ,1,2,2,2,2,3,4,4,5,6,7,8,],</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" t="s">
@@ -2199,11 +2250,14 @@
       <c r="O18">
         <v>7</v>
       </c>
+      <c r="P18">
+        <v>8</v>
+      </c>
     </row>
     <row r="19" spans="1:16">
       <c r="A19" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>['Tim', 'Jaguars' ,0,0,0,1,1,2,2,2,2,2,2,,],</v>
+        <v>['Tim', 'Jaguars' ,0,0,0,1,1,2,2,2,2,2,2,2,],</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" t="s">
@@ -2245,11 +2299,14 @@
       <c r="O19">
         <v>2</v>
       </c>
+      <c r="P19">
+        <v>2</v>
+      </c>
     </row>
     <row r="20" spans="1:16">
       <c r="A20" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>['Tim', 'Jets' ,0,1,1,1,1,1,2,3,3,3,3,,],</v>
+        <v>['Tim', 'Jets' ,0,1,1,1,1,1,2,3,3,3,3,3,],</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" t="s">
@@ -2291,6 +2348,9 @@
       <c r="O20">
         <v>3</v>
       </c>
+      <c r="P20">
+        <v>3</v>
+      </c>
     </row>
     <row r="21" spans="1:16">
       <c r="A21" s="2" t="str">
@@ -2344,7 +2404,7 @@
     <row r="22" spans="1:16">
       <c r="A22" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>['Tim', 'Packers' ,1,1,2,2,3,3,4,4,4,4,4,,],</v>
+        <v>['Tim', 'Packers' ,1,1,2,2,3,3,4,4,4,4,4,5,],</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" t="s">
@@ -2386,11 +2446,14 @@
       <c r="O22">
         <v>4</v>
       </c>
+      <c r="P22">
+        <v>5</v>
+      </c>
     </row>
     <row r="23" spans="1:16">
       <c r="A23" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>['Greg', 'Panthers' ,0,1,1,1,1,1,1,2,3,3,4,,],</v>
+        <v>['Greg', 'Panthers' ,0,1,1,1,1,1,1,2,3,3,4,4,],</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" t="s">
@@ -2432,11 +2495,14 @@
       <c r="O23">
         <v>4</v>
       </c>
+      <c r="P23">
+        <v>4</v>
+      </c>
     </row>
     <row r="24" spans="1:16">
       <c r="A24" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>['Greg', 'Patriots' ,1,2,3,3,4,5,6,7,7,7,8,,],</v>
+        <v>['Greg', 'Patriots' ,1,2,3,3,4,5,6,7,7,7,8,9,],</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" t="s">
@@ -2478,11 +2544,14 @@
       <c r="O24">
         <v>8</v>
       </c>
+      <c r="P24">
+        <v>9</v>
+      </c>
     </row>
     <row r="25" spans="1:16">
       <c r="A25" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>['Tim', 'Raiders' ,1,1,2,3,4,4,5,6,7,7,8,,],</v>
+        <v>['Tim', 'Raiders' ,1,1,2,3,4,4,5,6,7,7,8,9,],</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" t="s">
@@ -2524,11 +2593,14 @@
       <c r="O25">
         <v>8</v>
       </c>
+      <c r="P25">
+        <v>9</v>
+      </c>
     </row>
     <row r="26" spans="1:16">
       <c r="A26" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>['Zach', 'Rams' ,0,1,2,3,3,3,3,3,3,4,4,,],</v>
+        <v>['Zach', 'Rams' ,0,1,2,3,3,3,3,3,3,4,4,4,],</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" t="s">
@@ -2570,11 +2642,14 @@
       <c r="O26">
         <v>4</v>
       </c>
+      <c r="P26">
+        <v>4</v>
+      </c>
     </row>
     <row r="27" spans="1:16">
       <c r="A27" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>['Jeff', 'Ravens' ,1,2,3,3,3,3,3,3,4,5,5,,],</v>
+        <v>['Jeff', 'Ravens' ,1,2,3,3,3,3,3,3,4,5,5,6,],</v>
       </c>
       <c r="B27" s="3"/>
       <c r="C27" t="s">
@@ -2616,6 +2691,9 @@
       <c r="O27">
         <v>5</v>
       </c>
+      <c r="P27">
+        <v>6</v>
+      </c>
     </row>
     <row r="28" spans="1:16">
       <c r="A28" s="2" t="str">
@@ -2669,7 +2747,7 @@
     <row r="29" spans="1:16">
       <c r="A29" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>['Zach', 'Saints' ,0,0,0,1,1,2,2,3,4,4,4,,],</v>
+        <v>['Zach', 'Saints' ,0,0,0,1,1,2,2,3,4,4,4,5,],</v>
       </c>
       <c r="B29" s="3"/>
       <c r="C29" t="s">
@@ -2711,11 +2789,14 @@
       <c r="O29">
         <v>4</v>
       </c>
+      <c r="P29">
+        <v>5</v>
+      </c>
     </row>
     <row r="30" spans="1:16">
       <c r="A30" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>['Zach', 'Seahawks' ,1,1,2,3,3,4,4,4,5,6,7,,],</v>
+        <v>['Zach', 'Seahawks' ,1,1,2,3,3,4,4,4,5,6,7,7,],</v>
       </c>
       <c r="B30" s="3"/>
       <c r="C30" t="s">
@@ -2757,6 +2838,9 @@
       <c r="O30">
         <v>7</v>
       </c>
+      <c r="P30">
+        <v>7</v>
+      </c>
     </row>
     <row r="31" spans="1:16">
       <c r="A31" s="2" t="str">
@@ -2810,7 +2894,7 @@
     <row r="32" spans="1:16">
       <c r="A32" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>['Jeff', 'Texans' ,1,2,2,3,3,4,4,5,5,6,6,,],</v>
+        <v>['Jeff', 'Texans' ,1,2,2,3,3,4,4,5,5,6,6,6,],</v>
       </c>
       <c r="B32" s="3"/>
       <c r="C32" t="s">
@@ -2852,11 +2936,14 @@
       <c r="O32">
         <v>6</v>
       </c>
+      <c r="P32">
+        <v>6</v>
+      </c>
     </row>
     <row r="33" spans="1:16">
       <c r="A33" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>['Zach', 'Titans' ,0,1,1,1,2,3,3,4,4,5,5,,],</v>
+        <v>['Zach', 'Titans' ,0,1,1,1,2,3,3,4,4,5,5,6,],</v>
       </c>
       <c r="B33" s="3"/>
       <c r="C33" t="s">
@@ -2897,6 +2984,9 @@
       </c>
       <c r="O33">
         <v>5</v>
+      </c>
+      <c r="P33">
+        <v>6</v>
       </c>
     </row>
     <row r="34" spans="1:16">
@@ -3003,7 +3093,7 @@
       </c>
       <c r="P36" s="2">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>38</v>
       </c>
     </row>
     <row r="37" spans="1:16">
@@ -3056,7 +3146,7 @@
       </c>
       <c r="P37" s="2">
         <f t="shared" si="3"/>
-        <v>21</v>
+        <v>48</v>
       </c>
     </row>
     <row r="38" spans="1:16">
@@ -3109,7 +3199,7 @@
       </c>
       <c r="P38" s="2">
         <f t="shared" si="3"/>
-        <v>12</v>
+        <v>41</v>
       </c>
     </row>
     <row r="39" spans="1:16">
@@ -3162,7 +3252,7 @@
       </c>
       <c r="P39" s="2">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -3322,7 +3412,7 @@
     </row>
     <row r="3" spans="1:25">
       <c r="A3" s="2" t="str">
-        <f t="shared" ref="A3:A32" si="1">CONCATENATE("['",$C3,"', ","'",$D3,"' ,",$E3,",",$F3,",",$G3,",",$H3,",",$I3,"],")</f>
+        <f t="shared" ref="A3:A31" si="1">CONCATENATE("['",$C3,"', ","'",$D3,"' ,",$E3,",",$F3,",",$G3,",",$H3,",",$I3,"],")</f>
         <v>['Jeff', 'Boston' ,1,3,4,6,9],</v>
       </c>
       <c r="B3" s="3"/>

</xml_diff>

<commit_message>
Updated win totals for the week.
</commit_message>
<xml_diff>
--- a/NFL Wins.xlsx
+++ b/NFL Wins.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8980" windowHeight="16100" tabRatio="500" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8980" windowHeight="16100" tabRatio="500" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
@@ -479,7 +479,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="115">
+  <cellStyleXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -578,6 +578,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -611,7 +613,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="115">
+  <cellStyles count="117">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -671,6 +673,7 @@
     <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -726,6 +729,7 @@
     <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1344,7 +1348,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y39"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <pane xSplit="4" ySplit="2" topLeftCell="O6" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="L1" sqref="L1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -3273,9 +3277,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y36"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <pane xSplit="4" topLeftCell="F1" activePane="topRight" state="frozenSplit"/>
-      <selection pane="topRight" activeCell="A31" sqref="A2:A31"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <pane xSplit="4" topLeftCell="H1" activePane="topRight" state="frozenSplit"/>
+      <selection pane="topRight" activeCell="A2" sqref="A2:A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3384,8 +3388,8 @@
     </row>
     <row r="2" spans="1:25">
       <c r="A2" s="2" t="str">
-        <f>CONCATENATE("['",$C2,"', ","'",$D2,"' ,",$E2,",",$F2,",",$G2,",",$H2,",",$I2,"],")</f>
-        <v>['Zach', 'Atlanta' ,1,3,6,9,10],</v>
+        <f>CONCATENATE("['",$C2,"', ","'",$D2,"' ,",$E2,",",$F2,",",$G2,",",$H2,",",$I2,",",$J2,"],")</f>
+        <v>['Zach', 'Atlanta' ,1,3,6,9,10,10],</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" t="s">
@@ -3409,11 +3413,14 @@
       <c r="I2">
         <v>10</v>
       </c>
+      <c r="J2">
+        <v>10</v>
+      </c>
     </row>
     <row r="3" spans="1:25">
       <c r="A3" s="2" t="str">
-        <f t="shared" ref="A3:A31" si="1">CONCATENATE("['",$C3,"', ","'",$D3,"' ,",$E3,",",$F3,",",$G3,",",$H3,",",$I3,"],")</f>
-        <v>['Jeff', 'Boston' ,1,3,4,6,9],</v>
+        <f t="shared" ref="A3:A31" si="1">CONCATENATE("['",$C3,"', ","'",$D3,"' ,",$E3,",",$F3,",",$G3,",",$H3,",",$I3,",",$J3,"],")</f>
+        <v>['Jeff', 'Boston' ,1,3,4,6,9,11],</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" t="s">
@@ -3437,11 +3444,14 @@
       <c r="I3">
         <v>9</v>
       </c>
+      <c r="J3">
+        <v>11</v>
+      </c>
     </row>
     <row r="4" spans="1:25">
       <c r="A4" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Zach', 'Brooklyn' ,1,2,3,4,4],</v>
+        <v>['Zach', 'Brooklyn' ,1,2,3,4,4,5],</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" t="s">
@@ -3465,11 +3475,14 @@
       <c r="I4">
         <v>4</v>
       </c>
+      <c r="J4">
+        <v>5</v>
+      </c>
     </row>
     <row r="5" spans="1:25">
       <c r="A5" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Jeff', 'Charlotte' ,2,4,6,8,8],</v>
+        <v>['Jeff', 'Charlotte' ,2,4,6,8,8,11],</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" t="s">
@@ -3493,11 +3506,14 @@
       <c r="I5">
         <v>8</v>
       </c>
+      <c r="J5">
+        <v>11</v>
+      </c>
     </row>
     <row r="6" spans="1:25">
       <c r="A6" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Greg', 'Chicago' ,1,3,5,8,10],</v>
+        <v>['Greg', 'Chicago' ,1,3,5,8,10,11],</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" t="s">
@@ -3521,11 +3537,14 @@
       <c r="I6">
         <v>10</v>
       </c>
+      <c r="J6">
+        <v>11</v>
+      </c>
     </row>
     <row r="7" spans="1:25">
       <c r="A7" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Tim', 'Cleveland' ,2,5,7,10,12],</v>
+        <v>['Tim', 'Cleveland' ,2,5,7,10,12,13],</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" t="s">
@@ -3549,11 +3568,14 @@
       <c r="I7">
         <v>12</v>
       </c>
+      <c r="J7">
+        <v>13</v>
+      </c>
     </row>
     <row r="8" spans="1:25">
       <c r="A8" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Tim', 'Dallas' ,0,0,2,2,2],</v>
+        <v>['Tim', 'Dallas' ,0,0,2,2,2,3],</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" t="s">
@@ -3577,11 +3599,14 @@
       <c r="I8">
         <v>2</v>
       </c>
+      <c r="J8">
+        <v>3</v>
+      </c>
     </row>
     <row r="9" spans="1:25">
       <c r="A9" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Tim', 'Denver' ,1,2,3,4,6],</v>
+        <v>['Tim', 'Denver' ,1,2,3,4,6,7],</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" t="s">
@@ -3605,11 +3630,14 @@
       <c r="I9">
         <v>6</v>
       </c>
+      <c r="J9">
+        <v>7</v>
+      </c>
     </row>
     <row r="10" spans="1:25">
       <c r="A10" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Greg', 'Detroit' ,1,3,4,6,8],</v>
+        <v>['Greg', 'Detroit' ,1,3,4,6,8,11],</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" t="s">
@@ -3633,11 +3661,14 @@
       <c r="I10">
         <v>8</v>
       </c>
+      <c r="J10">
+        <v>11</v>
+      </c>
     </row>
     <row r="11" spans="1:25">
       <c r="A11" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Zach', 'Golden State' ,1,4,7,9,14],</v>
+        <v>['Zach', 'Golden State' ,1,4,7,9,14,16],</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" t="s">
@@ -3661,11 +3692,14 @@
       <c r="I11">
         <v>14</v>
       </c>
+      <c r="J11">
+        <v>16</v>
+      </c>
     </row>
     <row r="12" spans="1:25">
       <c r="A12" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Jeff', 'Houston' ,1,3,5,7,10],</v>
+        <v>['Jeff', 'Houston' ,1,3,5,7,10,13],</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" t="s">
@@ -3689,11 +3723,14 @@
       <c r="I12">
         <v>10</v>
       </c>
+      <c r="J12">
+        <v>13</v>
+      </c>
     </row>
     <row r="13" spans="1:25">
       <c r="A13" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Tim', 'Indiana' ,1,2,4,6,8],</v>
+        <v>['Tim', 'Indiana' ,1,2,4,6,8,9],</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" t="s">
@@ -3717,11 +3754,14 @@
       <c r="I13">
         <v>8</v>
       </c>
+      <c r="J13">
+        <v>9</v>
+      </c>
     </row>
     <row r="14" spans="1:25">
       <c r="A14" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Tim', 'L.A. Lakers' ,1,3,5,7,8],</v>
+        <v>['Tim', 'L.A. Lakers' ,1,3,5,7,8,10],</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" t="s">
@@ -3745,11 +3785,14 @@
       <c r="I14">
         <v>8</v>
       </c>
+      <c r="J14">
+        <v>10</v>
+      </c>
     </row>
     <row r="15" spans="1:25">
       <c r="A15" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Greg', 'LA Clippers' ,1,4,8,11,14],</v>
+        <v>['Greg', 'LA Clippers' ,1,4,8,11,14,16],</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" t="s">
@@ -3773,11 +3816,14 @@
       <c r="I15">
         <v>14</v>
       </c>
+      <c r="J15">
+        <v>16</v>
+      </c>
     </row>
     <row r="16" spans="1:25">
       <c r="A16" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Tim', 'Memphis' ,1,3,4,7,10],</v>
+        <v>['Tim', 'Memphis' ,1,3,4,7,10,12],</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" t="s">
@@ -3801,11 +3847,14 @@
       <c r="I16">
         <v>10</v>
       </c>
-    </row>
-    <row r="17" spans="1:9">
+      <c r="J16">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Zach', 'Miami' ,1,2,2,3,5],</v>
+        <v>['Zach', 'Miami' ,1,2,2,3,5,7],</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" t="s">
@@ -3829,11 +3878,14 @@
       <c r="I17">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:9">
+      <c r="J17">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Greg', 'Milwaukee' ,0,3,4,5,6],</v>
+        <v>['Greg', 'Milwaukee' ,0,3,4,5,6,9],</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" t="s">
@@ -3857,11 +3909,14 @@
       <c r="I18">
         <v>6</v>
       </c>
-    </row>
-    <row r="19" spans="1:9">
+      <c r="J18">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Jeff', 'Minnesota' ,0,1,2,4,5],</v>
+        <v>['Jeff', 'Minnesota' ,0,1,2,4,5,5],</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" t="s">
@@ -3885,11 +3940,14 @@
       <c r="I19">
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="1:9">
+      <c r="J19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Zach', 'New Orleans' ,0,0,1,2,6],</v>
+        <v>['Zach', 'New Orleans' ,0,0,1,2,6,7],</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" t="s">
@@ -3913,11 +3971,14 @@
       <c r="I20">
         <v>6</v>
       </c>
-    </row>
-    <row r="21" spans="1:9">
+      <c r="J20">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Zach', 'New York' ,0,2,3,5,8],</v>
+        <v>['Zach', 'New York' ,0,2,3,5,8,10],</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" t="s">
@@ -3941,11 +4002,14 @@
       <c r="I21">
         <v>8</v>
       </c>
-    </row>
-    <row r="22" spans="1:9">
+      <c r="J21">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Jeff', 'Oklahoma City' ,2,4,6,7,9],</v>
+        <v>['Jeff', 'Oklahoma City' ,2,4,6,7,9,12],</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" t="s">
@@ -3969,11 +4033,14 @@
       <c r="I22">
         <v>9</v>
       </c>
-    </row>
-    <row r="23" spans="1:9">
+      <c r="J22">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Greg', 'Orlando' ,0,2,3,5,6],</v>
+        <v>['Greg', 'Orlando' ,0,2,3,5,6,8],</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" t="s">
@@ -3997,11 +4064,14 @@
       <c r="I23">
         <v>6</v>
       </c>
-    </row>
-    <row r="24" spans="1:9">
+      <c r="J23">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['', 'Philadelphia' ,0,0,1,2,4],</v>
+        <v>['', 'Philadelphia' ,0,0,1,2,4,4],</v>
       </c>
       <c r="B24" s="3"/>
       <c r="D24" t="s">
@@ -4022,11 +4092,14 @@
       <c r="I24">
         <v>4</v>
       </c>
-    </row>
-    <row r="25" spans="1:9">
+      <c r="J24">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['', 'Phoenix' ,0,2,3,3,5],</v>
+        <v>['', 'Phoenix' ,0,2,3,3,5,6],</v>
       </c>
       <c r="B25" s="3"/>
       <c r="D25" t="s">
@@ -4047,11 +4120,14 @@
       <c r="I25">
         <v>5</v>
       </c>
-    </row>
-    <row r="26" spans="1:9">
+      <c r="J25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Greg', 'Portland' ,1,3,6,7,9],</v>
+        <v>['Greg', 'Portland' ,1,3,6,7,9,10],</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" t="s">
@@ -4075,11 +4151,14 @@
       <c r="I26">
         <v>9</v>
       </c>
-    </row>
-    <row r="27" spans="1:9">
+      <c r="J26">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
       <c r="A27" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Jeff', 'Sacramento' ,1,2,4,4,6],</v>
+        <v>['Jeff', 'Sacramento' ,1,2,4,4,6,7],</v>
       </c>
       <c r="B27" s="3"/>
       <c r="C27" t="s">
@@ -4103,11 +4182,14 @@
       <c r="I27">
         <v>6</v>
       </c>
-    </row>
-    <row r="28" spans="1:9">
+      <c r="J27">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
       <c r="A28" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Jeff', 'San Antonio' ,2,5,6,10,13],</v>
+        <v>['Jeff', 'San Antonio' ,2,5,6,10,13,16],</v>
       </c>
       <c r="B28" s="3"/>
       <c r="C28" t="s">
@@ -4131,11 +4213,14 @@
       <c r="I28">
         <v>13</v>
       </c>
-    </row>
-    <row r="29" spans="1:9">
+      <c r="J28">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
       <c r="A29" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Greg', 'Toronto' ,1,4,6,8,10],</v>
+        <v>['Greg', 'Toronto' ,1,4,6,8,10,13],</v>
       </c>
       <c r="B29" s="3"/>
       <c r="C29" t="s">
@@ -4159,11 +4244,14 @@
       <c r="I29">
         <v>10</v>
       </c>
-    </row>
-    <row r="30" spans="1:9">
+      <c r="J29">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
       <c r="A30" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Zach', 'Utah' ,1,3,6,7,9],</v>
+        <v>['Zach', 'Utah' ,1,3,6,7,9,11],</v>
       </c>
       <c r="B30" s="3"/>
       <c r="C30" t="s">
@@ -4187,11 +4275,14 @@
       <c r="I30">
         <v>9</v>
       </c>
-    </row>
-    <row r="31" spans="1:9">
+      <c r="J30">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
       <c r="A31" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Tim', 'Washington' ,0,1,2,3,5],</v>
+        <v>['Tim', 'Washington' ,0,1,2,3,5,6],</v>
       </c>
       <c r="B31" s="3"/>
       <c r="C31" t="s">
@@ -4215,8 +4306,11 @@
       <c r="I31">
         <v>5</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" s="4" customFormat="1" ht="4" customHeight="1">
+      <c r="J31">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" s="4" customFormat="1" ht="4" customHeight="1">
       <c r="A32" s="2"/>
       <c r="B32" s="3"/>
       <c r="F32" s="3"/>
@@ -4247,7 +4341,7 @@
       </c>
       <c r="J33" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="K33" s="2">
         <f t="shared" si="2"/>
@@ -4292,7 +4386,7 @@
       </c>
       <c r="J34" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="K34" s="2">
         <f t="shared" si="2"/>
@@ -4337,7 +4431,7 @@
       </c>
       <c r="J35" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="K35" s="2">
         <f t="shared" si="2"/>
@@ -4382,7 +4476,7 @@
       </c>
       <c r="J36" s="2">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="K36" s="2">
         <f t="shared" si="3"/>

</xml_diff>

<commit_message>
Updated for week 13 NFL.
</commit_message>
<xml_diff>
--- a/NFL Wins.xlsx
+++ b/NFL Wins.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8980" windowHeight="16100" tabRatio="500" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8980" windowHeight="16100" tabRatio="500" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
@@ -479,7 +479,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="117">
+  <cellStyleXfs count="141">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -597,8 +597,32 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -612,8 +636,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="117">
+  <cellStyles count="141">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -674,6 +701,18 @@
     <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -730,6 +769,18 @@
     <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1348,11 +1399,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y39"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="O6" activePane="bottomRight" state="frozenSplit"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <pane xSplit="4" ySplit="2" topLeftCell="N8" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="L1" sqref="L1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A34" sqref="A3:A34"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3:A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1476,8 +1527,8 @@
     </row>
     <row r="3" spans="1:25">
       <c r="A3" s="2" t="str">
-        <f>CONCATENATE("['",$C3,"', ","'",$D3,"' ,",$E3,",",$F3,",",$G3,",",$H3,",",$I3,",",$J3,",",$K3,",",$L3,",",$M3,",",$N3,",",$O3,",",$P3,"],")</f>
-        <v>['Greg', '49ers' ,1,1,1,1,1,1,1,1,1,1,1,1],</v>
+        <f>CONCATENATE("['",$C3,"', ","'",$D3,"', ",$E3,",",$F3,",",$G3,",",$H3,",",$I3,",",$J3,",",$K3,",",$L3,",",$M3,",",$N3,",",$O3,",",$P3,",",$Q3,"],")</f>
+        <v>['Greg', '49ers', 1,1,1,1,1,1,1,1,1,1,1,1,1],</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" t="s">
@@ -1522,11 +1573,14 @@
       <c r="P3">
         <v>1</v>
       </c>
+      <c r="Q3">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:25">
       <c r="A4" s="2" t="str">
-        <f t="shared" ref="A4:A7" si="1">CONCATENATE("['",$C4,"', ","'",$D4,"' ,",$E4,",",$F4,",",$G4,",",$H4,",",$I4,",",$J4,",",$K4,",",$L4,",",$M4,",",$N4,",",$O4,",",$P4,"],")</f>
-        <v>['Jeff', 'Bears' ,0,0,0,1,1,1,1,2,2,2,2,2],</v>
+        <f t="shared" ref="A4:A34" si="1">CONCATENATE("['",$C4,"', ","'",$D4,"', ",$E4,",",$F4,",",$G4,",",$H4,",",$I4,",",$J4,",",$K4,",",$L4,",",$M4,",",$N4,",",$O4,",",$P4,",",$Q4,"],")</f>
+        <v>['Jeff', 'Bears', 0,0,0,1,1,1,1,2,2,2,2,2,3],</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" t="s">
@@ -1571,11 +1625,14 @@
       <c r="P4">
         <v>2</v>
       </c>
+      <c r="Q4">
+        <v>3</v>
+      </c>
     </row>
     <row r="5" spans="1:25">
       <c r="A5" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Tim', 'Bengals' ,1,1,1,2,2,2,3,3,3,3,3,3],</v>
+        <v>['Tim', 'Bengals', 1,1,1,2,2,2,3,3,3,3,3,3,4],</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" t="s">
@@ -1620,11 +1677,14 @@
       <c r="P5">
         <v>3</v>
       </c>
+      <c r="Q5">
+        <v>4</v>
+      </c>
     </row>
     <row r="6" spans="1:25">
       <c r="A6" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Greg', 'Bills' ,0,0,1,2,3,4,4,4,4,4,5,6],</v>
+        <v>['Greg', 'Bills', 0,0,1,2,3,4,4,4,4,4,5,6,6],</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" t="s">
@@ -1669,11 +1729,14 @@
       <c r="P6">
         <v>6</v>
       </c>
+      <c r="Q6">
+        <v>6</v>
+      </c>
     </row>
     <row r="7" spans="1:25">
       <c r="A7" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Zach', 'Broncos' ,1,2,3,4,4,4,5,6,6,7,7,7],</v>
+        <v>['Zach', 'Broncos', 1,2,3,4,4,4,5,6,6,7,7,7,8],</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" t="s">
@@ -1718,11 +1781,14 @@
       <c r="P7">
         <v>7</v>
       </c>
+      <c r="Q7">
+        <v>8</v>
+      </c>
     </row>
     <row r="8" spans="1:25">
       <c r="A8" s="2" t="str">
-        <f>CONCATENATE("['",$C8,"', ","'",$D8,"' ,",$E8,",",$F8,",",$G8,",",$H8,",",$I8,",",$J8,",",$K8,",",$L8,",",$M8,",",$N8,",",$O8,",",$P8,",",$Q8,"],")</f>
-        <v>['Jeff', 'Browns' ,0,0,0,0,0,0,0,0,0,0,0,0,],</v>
+        <f t="shared" si="1"/>
+        <v>['Jeff', 'Browns', 0,0,0,0,0,0,0,0,0,0,0,0,0],</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" t="s">
@@ -1767,11 +1833,14 @@
       <c r="P8">
         <v>0</v>
       </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:25">
       <c r="A9" s="2" t="str">
-        <f t="shared" ref="A9:A34" si="2">CONCATENATE("['",$C9,"', ","'",$D9,"' ,",$E9,",",$F9,",",$G9,",",$H9,",",$I9,",",$J9,",",$K9,",",$L9,",",$M9,",",$N9,",",$O9,",",$P9,",",$Q9,"],")</f>
-        <v>['Zach', 'Buccaneers' ,1,1,1,1,2,2,3,3,3,4,5,6,],</v>
+        <f t="shared" si="1"/>
+        <v>['Zach', 'Buccaneers', 1,1,1,1,2,2,3,3,3,4,5,6,7],</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" t="s">
@@ -1816,11 +1885,14 @@
       <c r="P9">
         <v>6</v>
       </c>
+      <c r="Q9">
+        <v>7</v>
+      </c>
     </row>
     <row r="10" spans="1:25">
       <c r="A10" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>['Jeff', 'Cardinals' ,0,1,1,1,2,3,3,3,3,4,4,4,],</v>
+        <f t="shared" si="1"/>
+        <v>['Jeff', 'Cardinals', 0,1,1,1,2,3,3,3,3,4,4,4,5],</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" t="s">
@@ -1865,11 +1937,14 @@
       <c r="P10">
         <v>4</v>
       </c>
+      <c r="Q10">
+        <v>5</v>
+      </c>
     </row>
     <row r="11" spans="1:25">
       <c r="A11" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>['Jeff', 'Chargers' ,0,1,1,1,1,2,3,3,4,4,4,5,],</v>
+        <f t="shared" si="1"/>
+        <v>['Jeff', 'Chargers', 0,1,1,1,1,2,3,3,4,4,4,5,5],</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" t="s">
@@ -1914,11 +1989,14 @@
       <c r="P11">
         <v>5</v>
       </c>
+      <c r="Q11">
+        <v>5</v>
+      </c>
     </row>
     <row r="12" spans="1:25">
       <c r="A12" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>['Zach', 'Chiefs' ,1,1,2,2,2,3,4,5,6,7,7,8,],</v>
+        <f t="shared" si="1"/>
+        <v>['Zach', 'Chiefs', 1,1,2,2,2,3,4,5,6,7,7,8,9],</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" t="s">
@@ -1963,11 +2041,14 @@
       <c r="P12">
         <v>8</v>
       </c>
+      <c r="Q12">
+        <v>9</v>
+      </c>
     </row>
     <row r="13" spans="1:25">
       <c r="A13" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>['Greg', 'Colts' ,0,0,1,1,2,2,3,3,4,4,5,5,],</v>
+        <f t="shared" si="1"/>
+        <v>['Greg', 'Colts', 0,0,1,1,2,2,3,3,4,4,5,5,6],</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" t="s">
@@ -2012,11 +2093,14 @@
       <c r="P13">
         <v>5</v>
       </c>
+      <c r="Q13">
+        <v>6</v>
+      </c>
     </row>
     <row r="14" spans="1:25">
       <c r="A14" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>['Greg', 'Cowboys' ,0,1,2,3,4,5,5,6,7,8,9,10,],</v>
+        <f t="shared" si="1"/>
+        <v>['Greg', 'Cowboys', 0,1,2,3,4,5,5,6,7,8,9,10,11],</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" t="s">
@@ -2061,11 +2145,14 @@
       <c r="P14">
         <v>10</v>
       </c>
+      <c r="Q14">
+        <v>11</v>
+      </c>
     </row>
     <row r="15" spans="1:25">
       <c r="A15" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>['Tim', 'Dolphins' ,0,0,1,1,1,2,3,3,4,5,6,7,],</v>
+        <f t="shared" si="1"/>
+        <v>['Tim', 'Dolphins', 0,0,1,1,1,2,3,3,4,5,6,7,7],</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" t="s">
@@ -2110,11 +2197,14 @@
       <c r="P15">
         <v>7</v>
       </c>
+      <c r="Q15">
+        <v>7</v>
+      </c>
     </row>
     <row r="16" spans="1:25">
       <c r="A16" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>['Zach', 'Eagles' ,1,2,3,3,3,3,4,4,4,5,5,5,],</v>
+        <f t="shared" si="1"/>
+        <v>['Zach', 'Eagles', 1,2,3,3,3,3,4,4,4,5,5,5,5],</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" t="s">
@@ -2159,11 +2249,14 @@
       <c r="P16">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:16">
+      <c r="Q16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17">
       <c r="A17" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>['Greg', 'Falcons' ,0,1,2,3,4,4,4,5,6,6,6,7,],</v>
+        <f t="shared" si="1"/>
+        <v>['Greg', 'Falcons', 0,1,2,3,4,4,4,5,6,6,6,7,7],</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" t="s">
@@ -2208,11 +2301,14 @@
       <c r="P17">
         <v>7</v>
       </c>
-    </row>
-    <row r="18" spans="1:16">
+      <c r="Q17">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17">
       <c r="A18" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>['Jeff', 'Giants' ,1,2,2,2,2,3,4,4,5,6,7,8,],</v>
+        <f t="shared" si="1"/>
+        <v>['Jeff', 'Giants', 1,2,2,2,2,3,4,4,5,6,7,8,8],</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" t="s">
@@ -2257,11 +2353,14 @@
       <c r="P18">
         <v>8</v>
       </c>
-    </row>
-    <row r="19" spans="1:16">
+      <c r="Q18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17">
       <c r="A19" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>['Tim', 'Jaguars' ,0,0,0,1,1,2,2,2,2,2,2,2,],</v>
+        <f t="shared" si="1"/>
+        <v>['Tim', 'Jaguars', 0,0,0,1,1,2,2,2,2,2,2,2,2],</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" t="s">
@@ -2306,11 +2405,14 @@
       <c r="P19">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:16">
+      <c r="Q19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17">
       <c r="A20" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>['Tim', 'Jets' ,0,1,1,1,1,1,2,3,3,3,3,3,],</v>
+        <f t="shared" si="1"/>
+        <v>['Tim', 'Jets', 0,1,1,1,1,1,2,3,3,3,3,3,3],</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" t="s">
@@ -2355,11 +2457,14 @@
       <c r="P20">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="1:16">
+      <c r="Q20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17">
       <c r="A21" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>['Jeff', 'Lions' ,1,1,1,1,2,3,4,4,5,5,6,7,],</v>
+        <f t="shared" si="1"/>
+        <v>['Jeff', 'Lions', 1,1,1,1,2,3,4,4,5,5,6,7,8],</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" t="s">
@@ -2404,11 +2509,14 @@
       <c r="P21">
         <v>7</v>
       </c>
-    </row>
-    <row r="22" spans="1:16">
+      <c r="Q21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17">
       <c r="A22" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>['Tim', 'Packers' ,1,1,2,2,3,3,4,4,4,4,4,5,],</v>
+        <f t="shared" si="1"/>
+        <v>['Tim', 'Packers', 1,1,2,2,3,3,4,4,4,4,4,5,6],</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" t="s">
@@ -2453,11 +2561,14 @@
       <c r="P22">
         <v>5</v>
       </c>
-    </row>
-    <row r="23" spans="1:16">
+      <c r="Q22">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17">
       <c r="A23" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>['Greg', 'Panthers' ,0,1,1,1,1,1,1,2,3,3,4,4,],</v>
+        <f t="shared" si="1"/>
+        <v>['Greg', 'Panthers', 0,1,1,1,1,1,1,2,3,3,4,4,4],</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" t="s">
@@ -2502,11 +2613,14 @@
       <c r="P23">
         <v>4</v>
       </c>
-    </row>
-    <row r="24" spans="1:16">
+      <c r="Q23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17">
       <c r="A24" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>['Greg', 'Patriots' ,1,2,3,3,4,5,6,7,7,7,8,9,],</v>
+        <f t="shared" si="1"/>
+        <v>['Greg', 'Patriots', 1,2,3,3,4,5,6,7,7,7,8,9,10],</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" t="s">
@@ -2551,11 +2665,14 @@
       <c r="P24">
         <v>9</v>
       </c>
-    </row>
-    <row r="25" spans="1:16">
+      <c r="Q24">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17">
       <c r="A25" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>['Tim', 'Raiders' ,1,1,2,3,4,4,5,6,7,7,8,9,],</v>
+        <f t="shared" si="1"/>
+        <v>['Tim', 'Raiders', 1,1,2,3,4,4,5,6,7,7,8,9,10],</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" t="s">
@@ -2600,11 +2717,14 @@
       <c r="P25">
         <v>9</v>
       </c>
-    </row>
-    <row r="26" spans="1:16">
+      <c r="Q25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17">
       <c r="A26" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>['Zach', 'Rams' ,0,1,2,3,3,3,3,3,3,4,4,4,],</v>
+        <f t="shared" si="1"/>
+        <v>['Zach', 'Rams', 0,1,2,3,3,3,3,3,3,4,4,4,4],</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" t="s">
@@ -2649,11 +2769,14 @@
       <c r="P26">
         <v>4</v>
       </c>
-    </row>
-    <row r="27" spans="1:16">
+      <c r="Q26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17">
       <c r="A27" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>['Jeff', 'Ravens' ,1,2,3,3,3,3,3,3,4,5,5,6,],</v>
+        <f t="shared" si="1"/>
+        <v>['Jeff', 'Ravens', 1,2,3,3,3,3,3,3,4,5,5,6,7],</v>
       </c>
       <c r="B27" s="3"/>
       <c r="C27" t="s">
@@ -2698,11 +2821,14 @@
       <c r="P27">
         <v>6</v>
       </c>
-    </row>
-    <row r="28" spans="1:16">
+      <c r="Q27">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17">
       <c r="A28" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>['Greg', 'Redskins' ,0,0,1,2,3,4,4,4,4,5,6,6,],</v>
+        <f t="shared" si="1"/>
+        <v>['Greg', 'Redskins', 0,0,1,2,3,4,4,4,4,5,6,6,6],</v>
       </c>
       <c r="B28" s="3"/>
       <c r="C28" t="s">
@@ -2747,11 +2873,14 @@
       <c r="P28">
         <v>6</v>
       </c>
-    </row>
-    <row r="29" spans="1:16">
+      <c r="Q28">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17">
       <c r="A29" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>['Zach', 'Saints' ,0,0,0,1,1,2,2,3,4,4,4,5,],</v>
+        <f t="shared" si="1"/>
+        <v>['Zach', 'Saints', 0,0,0,1,1,2,2,3,4,4,4,5,5],</v>
       </c>
       <c r="B29" s="3"/>
       <c r="C29" t="s">
@@ -2796,11 +2925,14 @@
       <c r="P29">
         <v>5</v>
       </c>
-    </row>
-    <row r="30" spans="1:16">
+      <c r="Q29">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17">
       <c r="A30" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>['Zach', 'Seahawks' ,1,1,2,3,3,4,4,4,5,6,7,7,],</v>
+        <f t="shared" si="1"/>
+        <v>['Zach', 'Seahawks', 1,1,2,3,3,4,4,4,5,6,7,7,8],</v>
       </c>
       <c r="B30" s="3"/>
       <c r="C30" t="s">
@@ -2845,11 +2977,14 @@
       <c r="P30">
         <v>7</v>
       </c>
-    </row>
-    <row r="31" spans="1:16">
+      <c r="Q30">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17">
       <c r="A31" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>['Tim', 'Steelers' ,1,2,2,3,4,4,4,4,4,4,5,6,],</v>
+        <f t="shared" si="1"/>
+        <v>['Tim', 'Steelers', 1,2,2,3,4,4,4,4,4,4,5,6,7],</v>
       </c>
       <c r="B31" s="3"/>
       <c r="C31" t="s">
@@ -2894,11 +3029,14 @@
       <c r="P31">
         <v>6</v>
       </c>
-    </row>
-    <row r="32" spans="1:16">
+      <c r="Q31">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17">
       <c r="A32" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>['Jeff', 'Texans' ,1,2,2,3,3,4,4,5,5,6,6,6,],</v>
+        <f t="shared" si="1"/>
+        <v>['Jeff', 'Texans', 1,2,2,3,3,4,4,5,5,6,6,6,6],</v>
       </c>
       <c r="B32" s="3"/>
       <c r="C32" t="s">
@@ -2943,14 +3081,17 @@
       <c r="P32">
         <v>6</v>
       </c>
-    </row>
-    <row r="33" spans="1:16">
+      <c r="Q32">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17">
       <c r="A33" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>['Zach', 'Titans' ,0,1,1,1,2,3,3,4,4,5,5,6,],</v>
+        <f t="shared" si="1"/>
+        <v>['Zach', 'Titans', 0,1,1,1,2,3,3,4,4,5,5,6,6],</v>
       </c>
       <c r="B33" s="3"/>
-      <c r="C33" t="s">
+      <c r="C33" s="9" t="s">
         <v>35</v>
       </c>
       <c r="D33" t="s">
@@ -2992,11 +3133,14 @@
       <c r="P33">
         <v>6</v>
       </c>
-    </row>
-    <row r="34" spans="1:16">
+      <c r="Q33">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17">
       <c r="A34" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>['Tim', 'Vikings' ,1,2,3,4,5,5,5,5,5,5,6,6,],</v>
+        <f t="shared" si="1"/>
+        <v>['Tim', 'Vikings', 1,2,3,4,5,5,5,5,5,5,6,6,6],</v>
       </c>
       <c r="B34" s="3"/>
       <c r="C34" t="s">
@@ -3041,222 +3185,241 @@
       <c r="P34">
         <v>6</v>
       </c>
-    </row>
-    <row r="35" spans="1:16" s="4" customFormat="1" ht="4" customHeight="1">
+      <c r="Q34">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" s="4" customFormat="1" ht="4" customHeight="1">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="F35" s="3"/>
     </row>
-    <row r="36" spans="1:16">
+    <row r="36" spans="1:17">
       <c r="D36" t="s">
         <v>32</v>
       </c>
       <c r="E36">
-        <f t="shared" ref="E36:P38" si="3">SUMIF($C$3:$C$34,$D36,E$3:E$34)</f>
+        <f t="shared" ref="E36:Q38" si="2">SUMIF($C$3:$C$34,$D36,E$3:E$34)</f>
         <v>4</v>
       </c>
       <c r="F36" s="2">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="G36" s="2">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="H36" s="2">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="I36" s="2">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="J36" s="2">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="K36" s="2">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="L36" s="2">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="M36" s="2">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="N36" s="2">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="O36" s="2">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="P36" s="2">
+        <f t="shared" si="2"/>
+        <v>38</v>
+      </c>
+      <c r="Q36" s="2">
+        <f t="shared" si="2"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17">
+      <c r="D37" t="s">
+        <v>33</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="F37" s="2">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="G37" s="2">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="H37" s="2">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="I37" s="2">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="J37" s="2">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+      <c r="K37" s="2">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="L37" s="2">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="M37" s="2">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="N37" s="2">
+        <f t="shared" si="2"/>
+        <v>38</v>
+      </c>
+      <c r="O37" s="2">
+        <f t="shared" si="2"/>
+        <v>44</v>
+      </c>
+      <c r="P37" s="2">
+        <f t="shared" si="2"/>
+        <v>48</v>
+      </c>
+      <c r="Q37" s="2">
+        <f t="shared" si="2"/>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17">
+      <c r="D38" t="s">
+        <v>34</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="F38" s="2">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="G38" s="2">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="H38" s="2">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="I38" s="2">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="J38" s="2">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="K38" s="2">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="L38" s="2">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="M38" s="2">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="N38" s="2">
+        <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
+      <c r="O38" s="2">
+        <f t="shared" si="2"/>
+        <v>37</v>
+      </c>
+      <c r="P38" s="2">
+        <f t="shared" si="2"/>
+        <v>41</v>
+      </c>
+      <c r="Q38" s="2">
+        <f t="shared" si="2"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17">
+      <c r="D39" t="s">
+        <v>35</v>
+      </c>
+      <c r="E39">
+        <f t="shared" ref="E39:Q39" si="3">SUMIF($C$3:$C$34,$D$39,E$3:E$34)</f>
+        <v>5</v>
+      </c>
+      <c r="F39" s="2">
         <f t="shared" si="3"/>
         <v>9</v>
       </c>
-      <c r="G36" s="2">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-      <c r="H36" s="2">
-        <f t="shared" si="3"/>
-        <v>12</v>
-      </c>
-      <c r="I36" s="2">
+      <c r="G39" s="2">
         <f t="shared" si="3"/>
         <v>14</v>
       </c>
-      <c r="J36" s="2">
+      <c r="H39" s="2">
         <f t="shared" si="3"/>
-        <v>19</v>
-      </c>
-      <c r="K36" s="2">
+        <v>18</v>
+      </c>
+      <c r="I39" s="2">
         <f t="shared" si="3"/>
-        <v>22</v>
-      </c>
-      <c r="L36" s="2">
+        <v>20</v>
+      </c>
+      <c r="J39" s="2">
         <f t="shared" si="3"/>
         <v>24</v>
       </c>
-      <c r="M36" s="2">
+      <c r="K39" s="2">
         <f t="shared" si="3"/>
         <v>28</v>
       </c>
-      <c r="N36" s="2">
+      <c r="L39" s="2">
         <f t="shared" si="3"/>
         <v>32</v>
       </c>
-      <c r="O36" s="2">
+      <c r="M39" s="2">
         <f t="shared" si="3"/>
-        <v>34</v>
-      </c>
-      <c r="P36" s="2">
+        <v>35</v>
+      </c>
+      <c r="N39" s="2">
         <f t="shared" si="3"/>
-        <v>38</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16">
-      <c r="D37" t="s">
-        <v>33</v>
-      </c>
-      <c r="E37">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="F37" s="2">
-        <f t="shared" si="3"/>
-        <v>6</v>
-      </c>
-      <c r="G37" s="2">
-        <f t="shared" si="3"/>
-        <v>12</v>
-      </c>
-      <c r="H37" s="2">
-        <f t="shared" si="3"/>
-        <v>16</v>
-      </c>
-      <c r="I37" s="2">
-        <f t="shared" si="3"/>
-        <v>22</v>
-      </c>
-      <c r="J37" s="2">
-        <f t="shared" si="3"/>
-        <v>26</v>
-      </c>
-      <c r="K37" s="2">
-        <f t="shared" si="3"/>
-        <v>28</v>
-      </c>
-      <c r="L37" s="2">
-        <f t="shared" si="3"/>
-        <v>32</v>
-      </c>
-      <c r="M37" s="2">
-        <f t="shared" si="3"/>
-        <v>36</v>
-      </c>
-      <c r="N37" s="2">
-        <f t="shared" si="3"/>
-        <v>38</v>
-      </c>
-      <c r="O37" s="2">
+        <v>42</v>
+      </c>
+      <c r="O39" s="2">
         <f t="shared" si="3"/>
         <v>44</v>
       </c>
-      <c r="P37" s="2">
+      <c r="P39" s="2">
         <f t="shared" si="3"/>
         <v>48</v>
       </c>
-    </row>
-    <row r="38" spans="1:16">
-      <c r="D38" t="s">
-        <v>34</v>
-      </c>
-      <c r="E38">
+      <c r="Q39" s="2">
         <f t="shared" si="3"/>
-        <v>5</v>
-      </c>
-      <c r="F38" s="2">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="G38" s="2">
-        <f t="shared" si="3"/>
-        <v>12</v>
-      </c>
-      <c r="H38" s="2">
-        <f t="shared" si="3"/>
-        <v>17</v>
-      </c>
-      <c r="I38" s="2">
-        <f t="shared" si="3"/>
-        <v>21</v>
-      </c>
-      <c r="J38" s="2">
-        <f t="shared" si="3"/>
-        <v>23</v>
-      </c>
-      <c r="K38" s="2">
-        <f t="shared" si="3"/>
-        <v>28</v>
-      </c>
-      <c r="L38" s="2">
-        <f t="shared" si="3"/>
-        <v>30</v>
-      </c>
-      <c r="M38" s="2">
-        <f t="shared" si="3"/>
-        <v>32</v>
-      </c>
-      <c r="N38" s="2">
-        <f t="shared" si="3"/>
-        <v>33</v>
-      </c>
-      <c r="O38" s="2">
-        <f t="shared" si="3"/>
-        <v>37</v>
-      </c>
-      <c r="P38" s="2">
-        <f t="shared" si="3"/>
-        <v>41</v>
-      </c>
-    </row>
-    <row r="39" spans="1:16">
-      <c r="D39" t="s">
-        <v>35</v>
-      </c>
-      <c r="E39">
-        <f t="shared" ref="E39:P39" si="4">SUMIF($C$3:$C$34,$D$39,E$3:E$34)</f>
-        <v>5</v>
-      </c>
-      <c r="F39" s="2">
-        <f t="shared" si="4"/>
-        <v>9</v>
-      </c>
-      <c r="G39" s="2">
-        <f t="shared" si="4"/>
-        <v>14</v>
-      </c>
-      <c r="H39" s="2">
-        <f t="shared" si="4"/>
-        <v>18</v>
-      </c>
-      <c r="I39" s="2">
-        <f t="shared" si="4"/>
-        <v>20</v>
-      </c>
-      <c r="J39" s="2">
-        <f t="shared" si="4"/>
-        <v>24</v>
-      </c>
-      <c r="K39" s="2">
-        <f t="shared" si="4"/>
-        <v>28</v>
-      </c>
-      <c r="L39" s="2">
-        <f t="shared" si="4"/>
-        <v>32</v>
-      </c>
-      <c r="M39" s="2">
-        <f t="shared" si="4"/>
-        <v>35</v>
-      </c>
-      <c r="N39" s="2">
-        <f t="shared" si="4"/>
-        <v>42</v>
-      </c>
-      <c r="O39" s="2">
-        <f t="shared" si="4"/>
-        <v>44</v>
-      </c>
-      <c r="P39" s="2">
-        <f t="shared" si="4"/>
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -3277,7 +3440,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y36"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <pane xSplit="4" topLeftCell="H1" activePane="topRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="A2" sqref="A2:A31"/>
     </sheetView>

</xml_diff>

<commit_message>
Updated formatting for smaller screens.
</commit_message>
<xml_diff>
--- a/NFL Wins.xlsx
+++ b/NFL Wins.xlsx
@@ -479,7 +479,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="163">
+  <cellStyleXfs count="169">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -578,6 +578,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -662,7 +668,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="163">
+  <cellStyles count="169">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -746,6 +752,9 @@
     <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -825,6 +834,9 @@
     <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1444,10 +1456,10 @@
   <dimension ref="A1:Y39"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="T3" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="L1" sqref="L1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A34" sqref="A3:A34"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1571,8 +1583,8 @@
     </row>
     <row r="3" spans="1:25">
       <c r="A3" s="2" t="str">
-        <f>CONCATENATE("['",$C3,"', ","'",$D3,"', ",$E3,",",$F3,",",$G3,",",$H3,",",$I3,",",$J3,",",$K3,",",$L3,",",$M3,",",$N3,",",$O3,",",$P3,",",$Q3,",",$R3,",",$S3,",",$T3,"],")</f>
-        <v>['Greg', '49ers', 1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,2],</v>
+        <f>CONCATENATE("['",$C3,"', ","'",$D3,"', ",$E3,",",$F3,",",$G3,",",$H3,",",$I3,",",$J3,",",$K3,",",$L3,",",$M3,",",$N3,",",$O3,",",$P3,",",$Q3,",",$R3,",",$S3,",",$T3,",",$U3,"],")</f>
+        <v>['Greg', '49ers', 1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,2,2],</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" t="s">
@@ -1632,11 +1644,23 @@
       <c r="U3">
         <v>2</v>
       </c>
+      <c r="V3">
+        <v>2</v>
+      </c>
+      <c r="W3">
+        <v>2</v>
+      </c>
+      <c r="X3">
+        <v>2</v>
+      </c>
+      <c r="Y3">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" spans="1:25">
       <c r="A4" s="2" t="str">
-        <f t="shared" ref="A4:A34" si="1">CONCATENATE("['",$C4,"', ","'",$D4,"', ",$E4,",",$F4,",",$G4,",",$H4,",",$I4,",",$J4,",",$K4,",",$L4,",",$M4,",",$N4,",",$O4,",",$P4,",",$Q4,",",$R4,",",$S4,",",$T4,"],")</f>
-        <v>['Jeff', 'Bears', 0,0,0,1,1,1,1,2,2,2,2,2,3,3,3,3],</v>
+        <f t="shared" ref="A4:A34" si="1">CONCATENATE("['",$C4,"', ","'",$D4,"', ",$E4,",",$F4,",",$G4,",",$H4,",",$I4,",",$J4,",",$K4,",",$L4,",",$M4,",",$N4,",",$O4,",",$P4,",",$Q4,",",$R4,",",$S4,",",$T4,",",$U4,"],")</f>
+        <v>['Jeff', 'Bears', 0,0,0,1,1,1,1,2,2,2,2,2,3,3,3,3,3],</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" t="s">
@@ -1696,11 +1720,23 @@
       <c r="U4">
         <v>3</v>
       </c>
+      <c r="V4">
+        <v>3</v>
+      </c>
+      <c r="W4">
+        <v>3</v>
+      </c>
+      <c r="X4">
+        <v>3</v>
+      </c>
+      <c r="Y4">
+        <v>3</v>
+      </c>
     </row>
     <row r="5" spans="1:25">
       <c r="A5" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Tim', 'Bengals', 1,1,1,2,2,2,3,3,3,3,3,3,4,5,5,5],</v>
+        <v>['Tim', 'Bengals', 1,1,1,2,2,2,3,3,3,3,3,3,4,5,5,5,6],</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" t="s">
@@ -1760,11 +1796,23 @@
       <c r="U5">
         <v>6</v>
       </c>
+      <c r="V5">
+        <v>6</v>
+      </c>
+      <c r="W5">
+        <v>6</v>
+      </c>
+      <c r="X5">
+        <v>6</v>
+      </c>
+      <c r="Y5">
+        <v>6</v>
+      </c>
     </row>
     <row r="6" spans="1:25">
       <c r="A6" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Greg', 'Bills', 0,0,1,2,3,4,4,4,4,4,5,6,6,6,7,7],</v>
+        <v>['Greg', 'Bills', 0,0,1,2,3,4,4,4,4,4,5,6,6,6,7,7,7],</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" t="s">
@@ -1824,10 +1872,22 @@
       <c r="U6">
         <v>7</v>
       </c>
+      <c r="V6">
+        <v>7</v>
+      </c>
+      <c r="W6">
+        <v>7</v>
+      </c>
+      <c r="X6">
+        <v>7</v>
+      </c>
+      <c r="Y6">
+        <v>7</v>
+      </c>
     </row>
     <row r="7" spans="1:25">
       <c r="A7" s="2" t="str">
-        <f>CONCATENATE("['",$C7,"', ","'",$D7,"', ",$E7,",",$F7,",",$G7,",",$H7,",",$I7,",",$J7,",",$K7,",",$L7,",",$M7,",",$N7,",",$O7,",",$P7,",",$Q7,",",$R7,",",$S7,",",$T7,",",$U7,"],")</f>
+        <f t="shared" si="1"/>
         <v>['Zach', 'Broncos', 1,2,3,4,4,4,5,6,6,7,7,7,8,8,8,8,9],</v>
       </c>
       <c r="B7" s="3"/>
@@ -1888,10 +1948,22 @@
       <c r="U7">
         <v>9</v>
       </c>
+      <c r="V7">
+        <v>9</v>
+      </c>
+      <c r="W7">
+        <v>9</v>
+      </c>
+      <c r="X7">
+        <v>9</v>
+      </c>
+      <c r="Y7">
+        <v>9</v>
+      </c>
     </row>
     <row r="8" spans="1:25">
       <c r="A8" s="2" t="str">
-        <f t="shared" ref="A8:A34" si="2">CONCATENATE("['",$C8,"', ","'",$D8,"', ",$E8,",",$F8,",",$G8,",",$H8,",",$I8,",",$J8,",",$K8,",",$L8,",",$M8,",",$N8,",",$O8,",",$P8,",",$Q8,",",$R8,",",$S8,",",$T8,",",$U8,"],")</f>
+        <f t="shared" si="1"/>
         <v>['Jeff', 'Browns', 0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,1,1],</v>
       </c>
       <c r="B8" s="3"/>
@@ -1952,10 +2024,22 @@
       <c r="U8">
         <v>1</v>
       </c>
+      <c r="V8">
+        <v>1</v>
+      </c>
+      <c r="W8">
+        <v>1</v>
+      </c>
+      <c r="X8">
+        <v>1</v>
+      </c>
+      <c r="Y8">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:25">
       <c r="A9" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>['Zach', 'Buccaneers', 1,1,1,1,2,2,3,3,3,4,5,6,7,8,8,8,9],</v>
       </c>
       <c r="B9" s="3"/>
@@ -2016,10 +2100,22 @@
       <c r="U9">
         <v>9</v>
       </c>
+      <c r="V9">
+        <v>9</v>
+      </c>
+      <c r="W9">
+        <v>9</v>
+      </c>
+      <c r="X9">
+        <v>9</v>
+      </c>
+      <c r="Y9">
+        <v>9</v>
+      </c>
     </row>
     <row r="10" spans="1:25">
       <c r="A10" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>['Jeff', 'Cardinals', 0,1,1,1,2,3,3,3,3,4,4,4,5,5,5,6,7],</v>
       </c>
       <c r="B10" s="3"/>
@@ -2080,10 +2176,22 @@
       <c r="U10">
         <v>7</v>
       </c>
+      <c r="V10">
+        <v>7</v>
+      </c>
+      <c r="W10">
+        <v>7</v>
+      </c>
+      <c r="X10">
+        <v>7</v>
+      </c>
+      <c r="Y10">
+        <v>7</v>
+      </c>
     </row>
     <row r="11" spans="1:25">
       <c r="A11" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>['Jeff', 'Chargers', 0,1,1,1,1,2,3,3,4,4,4,5,5,5,5,5,5],</v>
       </c>
       <c r="B11" s="3"/>
@@ -2144,10 +2252,22 @@
       <c r="U11">
         <v>5</v>
       </c>
+      <c r="V11">
+        <v>5</v>
+      </c>
+      <c r="W11">
+        <v>5</v>
+      </c>
+      <c r="X11">
+        <v>5</v>
+      </c>
+      <c r="Y11">
+        <v>5</v>
+      </c>
     </row>
     <row r="12" spans="1:25">
       <c r="A12" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>['Zach', 'Chiefs', 1,1,2,2,2,3,4,5,6,7,7,8,9,10,10,11,12],</v>
       </c>
       <c r="B12" s="3"/>
@@ -2211,7 +2331,7 @@
     </row>
     <row r="13" spans="1:25">
       <c r="A13" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>['Greg', 'Colts', 0,0,1,1,2,2,3,3,4,4,5,5,6,6,7,7,8],</v>
       </c>
       <c r="B13" s="3"/>
@@ -2272,10 +2392,22 @@
       <c r="U13">
         <v>8</v>
       </c>
+      <c r="V13">
+        <v>8</v>
+      </c>
+      <c r="W13">
+        <v>8</v>
+      </c>
+      <c r="X13">
+        <v>8</v>
+      </c>
+      <c r="Y13">
+        <v>8</v>
+      </c>
     </row>
     <row r="14" spans="1:25">
       <c r="A14" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>['Greg', 'Cowboys', 0,1,2,3,4,5,5,6,7,8,9,10,11,11,12,13,13],</v>
       </c>
       <c r="B14" s="3"/>
@@ -2339,7 +2471,7 @@
     </row>
     <row r="15" spans="1:25">
       <c r="A15" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>['Tim', 'Dolphins', 0,0,1,1,1,2,3,3,4,5,6,7,7,8,9,10,10],</v>
       </c>
       <c r="B15" s="3"/>
@@ -2403,7 +2535,7 @@
     </row>
     <row r="16" spans="1:25">
       <c r="A16" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>['Zach', 'Eagles', 1,2,3,3,3,3,4,4,4,5,5,5,5,5,5,6,7],</v>
       </c>
       <c r="B16" s="3"/>
@@ -2464,10 +2596,22 @@
       <c r="U16">
         <v>7</v>
       </c>
-    </row>
-    <row r="17" spans="1:21">
+      <c r="V16">
+        <v>7</v>
+      </c>
+      <c r="W16">
+        <v>7</v>
+      </c>
+      <c r="X16">
+        <v>7</v>
+      </c>
+      <c r="Y16">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25">
       <c r="A17" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>['Greg', 'Falcons', 0,1,2,3,4,4,4,5,6,6,6,7,7,8,9,10,11],</v>
       </c>
       <c r="B17" s="3"/>
@@ -2529,9 +2673,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:21">
+    <row r="18" spans="1:25">
       <c r="A18" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>['Jeff', 'Giants', 1,2,2,2,2,3,4,4,5,6,7,8,8,9,10,10,11],</v>
       </c>
       <c r="B18" s="3"/>
@@ -2593,9 +2737,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:21">
+    <row r="19" spans="1:25">
       <c r="A19" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>['Tim', 'Jaguars', 0,0,0,1,1,2,2,2,2,2,2,2,2,2,2,3,3],</v>
       </c>
       <c r="B19" s="3"/>
@@ -2656,10 +2800,22 @@
       <c r="U19">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="1:21">
+      <c r="V19">
+        <v>3</v>
+      </c>
+      <c r="W19">
+        <v>3</v>
+      </c>
+      <c r="X19">
+        <v>3</v>
+      </c>
+      <c r="Y19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25">
       <c r="A20" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>['Tim', 'Jets', 0,1,1,1,1,1,2,3,3,3,3,3,3,4,4,4,5],</v>
       </c>
       <c r="B20" s="3"/>
@@ -2720,10 +2876,22 @@
       <c r="U20">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="1:21">
+      <c r="V20">
+        <v>5</v>
+      </c>
+      <c r="W20">
+        <v>5</v>
+      </c>
+      <c r="X20">
+        <v>5</v>
+      </c>
+      <c r="Y20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25">
       <c r="A21" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>['Jeff', 'Lions', 1,1,1,1,2,3,4,4,5,5,6,7,8,9,9,9,9],</v>
       </c>
       <c r="B21" s="3"/>
@@ -2785,9 +2953,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:21">
+    <row r="22" spans="1:25">
       <c r="A22" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>['Tim', 'Packers', 1,1,2,2,3,3,4,4,4,4,4,5,6,7,8,9,10],</v>
       </c>
       <c r="B22" s="3"/>
@@ -2849,9 +3017,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:21">
+    <row r="23" spans="1:25">
       <c r="A23" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>['Greg', 'Panthers', 0,1,1,1,1,1,1,2,3,3,4,4,4,5,6,6,6],</v>
       </c>
       <c r="B23" s="3"/>
@@ -2912,10 +3080,22 @@
       <c r="U23">
         <v>6</v>
       </c>
-    </row>
-    <row r="24" spans="1:21">
+      <c r="V23">
+        <v>6</v>
+      </c>
+      <c r="W23">
+        <v>6</v>
+      </c>
+      <c r="X23">
+        <v>6</v>
+      </c>
+      <c r="Y23">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25">
       <c r="A24" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>['Greg', 'Patriots', 1,2,3,3,4,5,6,7,7,7,8,9,10,11,12,13,14],</v>
       </c>
       <c r="B24" s="3"/>
@@ -2977,9 +3157,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:21">
+    <row r="25" spans="1:25">
       <c r="A25" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>['Tim', 'Raiders', 1,1,2,3,4,4,5,6,7,7,8,9,10,10,11,12,12],</v>
       </c>
       <c r="B25" s="3"/>
@@ -3041,9 +3221,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:21">
+    <row r="26" spans="1:25">
       <c r="A26" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>['Zach', 'Rams', 0,1,2,3,3,3,3,3,3,4,4,4,4,4,4,4,4],</v>
       </c>
       <c r="B26" s="3"/>
@@ -3104,10 +3284,22 @@
       <c r="U26">
         <v>4</v>
       </c>
-    </row>
-    <row r="27" spans="1:21">
+      <c r="V26">
+        <v>4</v>
+      </c>
+      <c r="W26">
+        <v>4</v>
+      </c>
+      <c r="X26">
+        <v>4</v>
+      </c>
+      <c r="Y26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25">
       <c r="A27" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>['Jeff', 'Ravens', 1,2,3,3,3,3,3,3,4,5,5,6,7,7,8,8,8],</v>
       </c>
       <c r="B27" s="3"/>
@@ -3168,10 +3360,22 @@
       <c r="U27">
         <v>8</v>
       </c>
-    </row>
-    <row r="28" spans="1:21">
+      <c r="V27">
+        <v>8</v>
+      </c>
+      <c r="W27">
+        <v>8</v>
+      </c>
+      <c r="X27">
+        <v>8</v>
+      </c>
+      <c r="Y27">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25">
       <c r="A28" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>['Greg', 'Redskins', 0,0,1,2,3,4,4,4,4,5,6,6,6,7,7,8,8],</v>
       </c>
       <c r="B28" s="3"/>
@@ -3232,10 +3436,22 @@
       <c r="U28">
         <v>8</v>
       </c>
-    </row>
-    <row r="29" spans="1:21">
+      <c r="V28">
+        <v>8</v>
+      </c>
+      <c r="W28">
+        <v>8</v>
+      </c>
+      <c r="X28">
+        <v>8</v>
+      </c>
+      <c r="Y28">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25">
       <c r="A29" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>['Zach', 'Saints', 0,0,0,1,1,2,2,3,4,4,4,5,5,5,6,7,7],</v>
       </c>
       <c r="B29" s="3"/>
@@ -3296,10 +3512,22 @@
       <c r="U29">
         <v>7</v>
       </c>
-    </row>
-    <row r="30" spans="1:21">
+      <c r="V29">
+        <v>7</v>
+      </c>
+      <c r="W29">
+        <v>7</v>
+      </c>
+      <c r="X29">
+        <v>7</v>
+      </c>
+      <c r="Y29">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25">
       <c r="A30" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>['Zach', 'Seahawks', 1,1,2,3,3,4,4,4,5,6,7,7,8,8,9,9,10],</v>
       </c>
       <c r="B30" s="3"/>
@@ -3361,9 +3589,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:21">
+    <row r="31" spans="1:25">
       <c r="A31" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>['Tim', 'Steelers', 1,2,2,3,4,4,4,4,4,4,5,6,7,8,9,10,11],</v>
       </c>
       <c r="B31" s="3"/>
@@ -3425,9 +3653,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:21">
+    <row r="32" spans="1:25">
       <c r="A32" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>['Jeff', 'Texans', 1,2,2,3,3,4,4,5,5,6,6,6,6,7,8,9,9],</v>
       </c>
       <c r="B32" s="3"/>
@@ -3491,7 +3719,7 @@
     </row>
     <row r="33" spans="1:25">
       <c r="A33" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>['Zach', 'Titans', 0,1,1,1,2,3,3,4,4,5,5,6,6,7,8,8,9],</v>
       </c>
       <c r="B33" s="3"/>
@@ -3552,10 +3780,22 @@
       <c r="U33">
         <v>9</v>
       </c>
+      <c r="V33">
+        <v>9</v>
+      </c>
+      <c r="W33">
+        <v>9</v>
+      </c>
+      <c r="X33">
+        <v>9</v>
+      </c>
+      <c r="Y33">
+        <v>9</v>
+      </c>
     </row>
     <row r="34" spans="1:25">
       <c r="A34" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>['Tim', 'Vikings', 1,2,3,4,5,5,5,5,5,5,6,6,6,7,7,7,8],</v>
       </c>
       <c r="B34" s="3"/>
@@ -3614,6 +3854,18 @@
         <v>7</v>
       </c>
       <c r="U34">
+        <v>8</v>
+      </c>
+      <c r="V34">
+        <v>8</v>
+      </c>
+      <c r="W34">
+        <v>8</v>
+      </c>
+      <c r="X34">
+        <v>8</v>
+      </c>
+      <c r="Y34">
         <v>8</v>
       </c>
     </row>
@@ -3627,88 +3879,88 @@
         <v>32</v>
       </c>
       <c r="E36">
-        <f t="shared" ref="E36:U38" si="3">SUMIF($C$3:$C$34,$D36,E$3:E$34)</f>
+        <f t="shared" ref="E36:U38" si="2">SUMIF($C$3:$C$34,$D36,E$3:E$34)</f>
         <v>4</v>
       </c>
       <c r="F36" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="G36" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="H36" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="I36" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="J36" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>19</v>
       </c>
       <c r="K36" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>22</v>
       </c>
       <c r="L36" s="2">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="M36" s="2">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="N36" s="2">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="O36" s="2">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="P36" s="2">
+        <f t="shared" si="2"/>
+        <v>38</v>
+      </c>
+      <c r="Q36" s="2">
+        <f t="shared" si="2"/>
+        <v>42</v>
+      </c>
+      <c r="R36" s="2">
+        <f t="shared" si="2"/>
+        <v>45</v>
+      </c>
+      <c r="S36" s="2">
+        <f t="shared" si="2"/>
+        <v>48</v>
+      </c>
+      <c r="T36" s="2">
+        <f t="shared" si="2"/>
+        <v>51</v>
+      </c>
+      <c r="U36" s="2">
+        <f t="shared" si="2"/>
+        <v>53</v>
+      </c>
+      <c r="V36" s="2">
+        <f t="shared" ref="U36:Y38" si="3">SUMIF($C$3:$C$34,$D36,V$3:V$34)</f>
+        <v>24</v>
+      </c>
+      <c r="W36" s="2">
         <f t="shared" si="3"/>
         <v>24</v>
       </c>
-      <c r="M36" s="2">
+      <c r="X36" s="2">
         <f t="shared" si="3"/>
-        <v>28</v>
-      </c>
-      <c r="N36" s="2">
+        <v>24</v>
+      </c>
+      <c r="Y36" s="2">
         <f t="shared" si="3"/>
-        <v>32</v>
-      </c>
-      <c r="O36" s="2">
-        <f t="shared" si="3"/>
-        <v>34</v>
-      </c>
-      <c r="P36" s="2">
-        <f t="shared" si="3"/>
-        <v>38</v>
-      </c>
-      <c r="Q36" s="2">
-        <f t="shared" si="3"/>
-        <v>42</v>
-      </c>
-      <c r="R36" s="2">
-        <f t="shared" si="3"/>
-        <v>45</v>
-      </c>
-      <c r="S36" s="2">
-        <f t="shared" si="3"/>
-        <v>48</v>
-      </c>
-      <c r="T36" s="2">
-        <f t="shared" si="3"/>
-        <v>51</v>
-      </c>
-      <c r="U36" s="2">
-        <f t="shared" si="3"/>
-        <v>53</v>
-      </c>
-      <c r="V36" s="2">
-        <f t="shared" ref="U36:Y38" si="4">SUMIF($C$3:$C$34,$D36,V$3:V$34)</f>
-        <v>0</v>
-      </c>
-      <c r="W36" s="2">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="X36" s="2">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Y36" s="2">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <v>24</v>
       </c>
     </row>
     <row r="37" spans="1:25">
@@ -3716,88 +3968,88 @@
         <v>33</v>
       </c>
       <c r="E37">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="F37" s="2">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="G37" s="2">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="H37" s="2">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="I37" s="2">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="J37" s="2">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+      <c r="K37" s="2">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="L37" s="2">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="M37" s="2">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="N37" s="2">
+        <f t="shared" si="2"/>
+        <v>38</v>
+      </c>
+      <c r="O37" s="2">
+        <f t="shared" si="2"/>
+        <v>44</v>
+      </c>
+      <c r="P37" s="2">
+        <f t="shared" si="2"/>
+        <v>48</v>
+      </c>
+      <c r="Q37" s="2">
+        <f t="shared" si="2"/>
+        <v>51</v>
+      </c>
+      <c r="R37" s="2">
+        <f t="shared" si="2"/>
+        <v>55</v>
+      </c>
+      <c r="S37" s="2">
+        <f t="shared" si="2"/>
+        <v>61</v>
+      </c>
+      <c r="T37" s="2">
+        <f t="shared" si="2"/>
+        <v>66</v>
+      </c>
+      <c r="U37" s="2">
         <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="F37" s="2">
+        <v>69</v>
+      </c>
+      <c r="V37" s="2">
         <f t="shared" si="3"/>
-        <v>6</v>
-      </c>
-      <c r="G37" s="2">
+        <v>31</v>
+      </c>
+      <c r="W37" s="2">
         <f t="shared" si="3"/>
-        <v>12</v>
-      </c>
-      <c r="H37" s="2">
+        <v>31</v>
+      </c>
+      <c r="X37" s="2">
         <f t="shared" si="3"/>
-        <v>16</v>
-      </c>
-      <c r="I37" s="2">
+        <v>31</v>
+      </c>
+      <c r="Y37" s="2">
         <f t="shared" si="3"/>
-        <v>22</v>
-      </c>
-      <c r="J37" s="2">
-        <f t="shared" si="3"/>
-        <v>26</v>
-      </c>
-      <c r="K37" s="2">
-        <f t="shared" si="3"/>
-        <v>28</v>
-      </c>
-      <c r="L37" s="2">
-        <f t="shared" si="3"/>
-        <v>32</v>
-      </c>
-      <c r="M37" s="2">
-        <f t="shared" si="3"/>
-        <v>36</v>
-      </c>
-      <c r="N37" s="2">
-        <f t="shared" si="3"/>
-        <v>38</v>
-      </c>
-      <c r="O37" s="2">
-        <f t="shared" si="3"/>
-        <v>44</v>
-      </c>
-      <c r="P37" s="2">
-        <f t="shared" si="3"/>
-        <v>48</v>
-      </c>
-      <c r="Q37" s="2">
-        <f t="shared" si="3"/>
-        <v>51</v>
-      </c>
-      <c r="R37" s="2">
-        <f t="shared" si="3"/>
-        <v>55</v>
-      </c>
-      <c r="S37" s="2">
-        <f t="shared" si="3"/>
-        <v>61</v>
-      </c>
-      <c r="T37" s="2">
-        <f t="shared" si="3"/>
-        <v>66</v>
-      </c>
-      <c r="U37" s="2">
-        <f t="shared" si="4"/>
-        <v>69</v>
-      </c>
-      <c r="V37" s="2">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="W37" s="2">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="X37" s="2">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Y37" s="2">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <v>31</v>
       </c>
     </row>
     <row r="38" spans="1:25">
@@ -3805,88 +4057,88 @@
         <v>34</v>
       </c>
       <c r="E38">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="F38" s="2">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="G38" s="2">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="H38" s="2">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="I38" s="2">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="J38" s="2">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="K38" s="2">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="L38" s="2">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="M38" s="2">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="N38" s="2">
+        <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
+      <c r="O38" s="2">
+        <f t="shared" si="2"/>
+        <v>37</v>
+      </c>
+      <c r="P38" s="2">
+        <f t="shared" si="2"/>
+        <v>41</v>
+      </c>
+      <c r="Q38" s="2">
+        <f t="shared" si="2"/>
+        <v>45</v>
+      </c>
+      <c r="R38" s="2">
+        <f t="shared" si="2"/>
+        <v>51</v>
+      </c>
+      <c r="S38" s="2">
+        <f t="shared" si="2"/>
+        <v>55</v>
+      </c>
+      <c r="T38" s="2">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
+      <c r="U38" s="2">
         <f t="shared" si="3"/>
-        <v>5</v>
-      </c>
-      <c r="F38" s="2">
+        <v>65</v>
+      </c>
+      <c r="V38" s="2">
         <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="G38" s="2">
+        <v>22</v>
+      </c>
+      <c r="W38" s="2">
         <f t="shared" si="3"/>
-        <v>12</v>
-      </c>
-      <c r="H38" s="2">
+        <v>22</v>
+      </c>
+      <c r="X38" s="2">
         <f t="shared" si="3"/>
-        <v>17</v>
-      </c>
-      <c r="I38" s="2">
+        <v>22</v>
+      </c>
+      <c r="Y38" s="2">
         <f t="shared" si="3"/>
-        <v>21</v>
-      </c>
-      <c r="J38" s="2">
-        <f t="shared" si="3"/>
-        <v>23</v>
-      </c>
-      <c r="K38" s="2">
-        <f t="shared" si="3"/>
-        <v>28</v>
-      </c>
-      <c r="L38" s="2">
-        <f t="shared" si="3"/>
-        <v>30</v>
-      </c>
-      <c r="M38" s="2">
-        <f t="shared" si="3"/>
-        <v>32</v>
-      </c>
-      <c r="N38" s="2">
-        <f t="shared" si="3"/>
-        <v>33</v>
-      </c>
-      <c r="O38" s="2">
-        <f t="shared" si="3"/>
-        <v>37</v>
-      </c>
-      <c r="P38" s="2">
-        <f t="shared" si="3"/>
-        <v>41</v>
-      </c>
-      <c r="Q38" s="2">
-        <f t="shared" si="3"/>
-        <v>45</v>
-      </c>
-      <c r="R38" s="2">
-        <f t="shared" si="3"/>
-        <v>51</v>
-      </c>
-      <c r="S38" s="2">
-        <f t="shared" si="3"/>
-        <v>55</v>
-      </c>
-      <c r="T38" s="2">
-        <f t="shared" si="3"/>
-        <v>60</v>
-      </c>
-      <c r="U38" s="2">
-        <f t="shared" si="4"/>
-        <v>65</v>
-      </c>
-      <c r="V38" s="2">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="W38" s="2">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="X38" s="2">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Y38" s="2">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <v>22</v>
       </c>
     </row>
     <row r="39" spans="1:25">
@@ -3894,88 +4146,88 @@
         <v>35</v>
       </c>
       <c r="E39">
-        <f t="shared" ref="E39:Y39" si="5">SUMIF($C$3:$C$34,$D$39,E$3:E$34)</f>
+        <f t="shared" ref="E39:Y39" si="4">SUMIF($C$3:$C$34,$D$39,E$3:E$34)</f>
         <v>5</v>
       </c>
       <c r="F39" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>9</v>
       </c>
       <c r="G39" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="H39" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="I39" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
       <c r="J39" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>24</v>
       </c>
       <c r="K39" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>28</v>
       </c>
       <c r="L39" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>32</v>
       </c>
       <c r="M39" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>35</v>
       </c>
       <c r="N39" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>42</v>
       </c>
       <c r="O39" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>44</v>
       </c>
       <c r="P39" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>48</v>
       </c>
       <c r="Q39" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>52</v>
       </c>
       <c r="R39" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>55</v>
       </c>
       <c r="S39" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>58</v>
       </c>
       <c r="T39" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>61</v>
       </c>
       <c r="U39" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>67</v>
       </c>
       <c r="V39" s="2">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>45</v>
       </c>
       <c r="W39" s="2">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>45</v>
       </c>
       <c r="X39" s="2">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>45</v>
       </c>
       <c r="Y39" s="2">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>